<commit_message>
Cleanup of bluebook alternatives
Former-commit-id: 1ddca968d9ebaca7620890d13eb2b163377b5dcc
</commit_message>
<xml_diff>
--- a/src/analysis/python/data/bluebook_manual_data_online_WORKING.xlsx
+++ b/src/analysis/python/data/bluebook_manual_data_online_WORKING.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivergiesecke/Dropbox/MPCounterfactual/src/analysis/python/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE2747D4-C03F-DB48-A077-99FA41757E47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E61F004-E507-B64B-9B0C-C3598BEC0995}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24220" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="460" windowWidth="15600" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -1989,583 +1989,583 @@
     <t>Under alternative B, federal funds would continue to trade around 5-3/4 percent. (25) Under alternative B, market interest rates would probably remain near their current levels. (26) Alternative B embodies the staff projections for money and debt consistent with the nominal GNP and unchanged interest rates of the greenbook forecast. M3 is expected to increase at a 3 percent rate from June to September under alternative B, keeping this aggregate a Alternative Levels and Growth Rates for Key Monetary Aggregates M2 M3 M1 Alt.</t>
   </si>
   <si>
+    <t>Alternative C also would catch market participants un- aware</t>
+  </si>
+  <si>
+    <t>(28) Alternative C also would catch market participants un- awares, and short-term interest rates likely would adjust upward rather sharply.</t>
+  </si>
+  <si>
+    <t>(10) The 1/2 percentage point drop in the funds rate con- templated under alternative A is larger than the easing of policy currently anticipated in the markets; thus, short-term rates are likely to move down under this alternative--but not by as much as the cut in the funds rate--with the three-month bill rate drifting to near 5 percent. (13) The easing of monetary policy under alternative A would boost M2 to a 4-1/2 percent annual rate of expansion in September and the pace would firm further in the fourth quarter, lifting growth of this aggregate for the year to around 3 percent.</t>
+  </si>
+  <si>
+    <t>Under alternative B, federal funds would continue to trade around 5-1/2 percent, at the discount rate, in association with adjustment plus seasonal borrowing of $375 million. With reserve market pressures unchanged, as under alternative B, rates might firm a touch. The dollar likely would trade around current levels under alternative B, but could firm a notch if U.S. interest rates were to back up. (11) Under alternative B, M2 would be expected to increase over the balance of the quarter.</t>
+  </si>
+  <si>
+    <t>7 Under alternative A, federal funds would tend to trade around 4-3/4 percent, which could be fostered either by lowering the borrowing specification by $50 million to $275 million or by lowering the discount rate by a further 1/2 point to 4-1/2 percent. The latter approach to alternative A would preserve the present spread of the funds rate over the discount rate and thus the current degree of cushioning of transitory shocks to the supply and demand for reserves. (9) The size and timing of the 1/2 percentage point drop in the federal funds rate of alternative A would tend to catch financial markets unawares, inducing almost as large a drop in other short-term interest rates. (15) The 1/2 percentage point decline in the federal funds rate under alternative A would promote faster money growth than under alternative B, improving the odds that the aggregates would end up in the ranges. This reasoning yields projected M2 growth over the next three months under alternative A of 4 percent at an annual rate.</t>
+  </si>
+  <si>
+    <t>Under alternative B, the federal funds rate would be expected to remain centered on 5-1/4 percent, in as- sociation with an initial specification for adjustment plus seasonal borrowing of $325 million. Nonetheless, the unchanged federal funds rate associ- ated with alternative B is unlikely to engender a marked backup in yields in financial markets over the intermeeting period, so long as incoming nonfinancial and monetary data are mixed, as would be the case under the staff's forecast. B Growth from September to December M2 4 3 M3 2 1-1/2 M1 8-1/2 6-1/2 Implied growth from 1990:Q4 to December M2 2-3/4 2-1/2 M3 1 1 Ml 7-1/2 7 (12) Under the unchanged interest rates of alternative B, M2 growth is projected to pick up to a 3 percent rate over the last three months of the year, leaving this aggregate at the lower bound of its Alternative Levels and Growth Rates for Key Monetary Aggregates M2 M3 M1 Alt. (13) Under alternative B, growth in M3 from September to December is expected to strengthen to a 1-1/2 percent annual rate. (15) The 1/2 percentage point decline in the federal funds rate under alternative A would promote faster money growth than under alternative B, improving the odds that the aggregates would end up in the ranges.</t>
+  </si>
+  <si>
+    <t>3 Under alternative A, the federal funds rate would move down to 4-1/2 percent, achieved either through a 1/2 percentage point cut in the discount rate with the same level of bor- rowing as under alternative B or through open market operations that lowered the borrowing level to $125 million. (12) The easing contemplated in alternative A exceeds that now envisioned by the markets and thus money market interest rates would decline, perhaps by at least 1/4 percentage point. -11- (13) M2 is projected to strengthen to a 4 percent rate by December under alternative A and would be entering the new year well into its tentative range. (14) Under alternative A, M3 would expand at a 1-1/4 percent rate in November and December, on a trajectory to begin the new year within its tentative range.</t>
+  </si>
+  <si>
+    <t>Under alternative B, federal funds would continue to trade around 5 percent in combination with adjustment plus seasonal borrowing of $175 million. 3 Under alternative A, the federal funds rate would move down to 4-1/2 percent, achieved either through a 1/2 percentage point cut in the discount rate with the same level of bor- rowing as under alternative B or through open market operations that lowered the borrowing level to $125 million. B Growth from September to December M2 3-1/2 3 M3 1-1/4 1 M1 10 9 Implied growth from 1990:Q4 to December M2 2-3/4 2-1/2 M3 1 1 M1 7-3/4 7-1/2 (9) The markets appear to have built in a high probability of a further easing move in the period just ahead, and thus with the unchanged funds rate of alternative B, other market interest rates may tend to firm. A M J J A S O N D J I 11400 11200 11000 10800 10600 10400 10200 19921991 (10) M2 would be expected to continue to expand at a 3 per- cent rate in the November and December period under alternative B, the same as expected at the October FOMC meeting. (11) M3 under alternative B is seen as continuing to grow at a 1 percent annual rate over November and December, which would mean this aggregate would be entering next year around the bottom of its tentative 1992 range of 1 to 5 percent.</t>
+  </si>
+  <si>
+    <t>Although the former variant of alternative A, which involves funds trading 1/2 percentage point below the discount rate, would be technically possible, it likely would be associated with somewhat greater day-to-day volatility in the funds rate. (12) Under alternative A, the 1/2 percentage point fall in the funds rate to 4 percent would foster a smaller drop in other short-term interest rates, given the expectations of near-term policy easing al- ready incorporated in current market quotes. Unless data were clear-cut in pointing to continuing weakness in the economy, the half-point easing of alternative A--closely following the quarter-point decline in the funds rate last week--would be seen as signalling a priority on encouraging a strong recovery. Even under the lower short-term inter- est rates associated with alternative A, these aggregates probably would remain noticeably below the midpoints of their ranges. (17) The lower short-term interest rates associated with alternative A would put M2 on a path that would carry it toward the middle portion of its range later in 1992. From November to March, M2 is projected to turn in a 3-3/4 percent growth rate under alternative A. While deposit rates will be reduced further--perhaps appreciably at some institutions, if lower market rates jolt them into reassessing long-standing rates on NOW accounts and passbook savings--they are not likely to drop enough to -14- eliminate the additional stimulus to money growth of the lower interest rates in alternative A. The faster M2 growth under alternative A will show through to M3, though in muted form, since bank and thrift credit growth will accelerate by less than M2 in the short run.</t>
+  </si>
+  <si>
+    <t>Under alternative B, the federal funds rate would continue to center around 4-1/2 percent, in association with the allowance for ad- justment plus seasonal borrowing staying at $75 million. (11) Under the unchanged federal funds rate of alternative B, interest rates may exhibit an initial tendency to firm a little, as market expectations of another modest policy easing in the near term are disappointed. Under alternative B, both M2 and M3 are projected to be only somewhat above the lower edges of their tenta- tive 1992 target cones in March. (15) Under alternative B, both M2 and M3 are projected to grow a little more slowly than their average rates over October and November.</t>
+  </si>
+  <si>
+    <t>10 Under alternative A, the federal funds rate would decline to the 3-1/2 percent area in association with a reduction of the borrowing allowance to $50 million. M2 would remain in the lower half of its provisional 1992 range through March under both alternatives, but under alternative A would be on a trajectory to move up in its range over the second quarter. (24) Short-term interest rates would fall by nearly the 50 basis point decline in the federal funds rate under alternative A. 12 Under the easier conditions of alternative A, M2 would be expected to be expanding at a percentage point faster pace in March and into the next quarter; all of the added growth in M2 would occur in M1, other liquid deposits, and M2 money funds.</t>
+  </si>
+  <si>
+    <t>Under alternative B, federal funds would con- tinue to trade around 4 percent, with adjustment plus seasonal borrowing averaging around $100 million. B Growth from December to March M2 3-1/2 3 M3 1-3/4 1-1/2 Ml 15-1/2 14-1/2 Growth from 1991Q4 to March M2 3-1/2 3-1/4 M3 2 1-3/4 M1 14-1/2 13-3/4 (23) The markets appear to have built in no policy moves in the period just ahead and thus unchanged reserve market conditions under alternative B should have no effect on interest rates. 8.5% 4.5% O N D J F MA M J J A SO ND J F MA M J J A S ON D 1990 1991 1992 12400 12200 12000 11800 11600 11400 11200 11000 10800 10600 -22- (25) Even with a pickup over February and March, M2 would expand at only a 3 percent annual rate over the December-to-March period under alternative B, below the pace over the last three months of 1991. (26) M3, under alternative B, would expand at only a 2 per- cent annual rate over February and March, after even slower growth in December and January.</t>
+  </si>
+  <si>
+    <t>This alternative might cause a market reassessment of the intentions of the Federal Reserve, leading to a significant downward revision in the expected course of short-term interest rates for the next year or so</t>
+  </si>
+  <si>
+    <t>Under alternative A, the federal funds rate would decline to the 3-1/2 percent area in conjunction with a reduction in the initial borrowing allowance to $75 million. In this context, the unexpected easing of money market conditions of alternative A might cause a market reassessment of the intentions of the Federal Reserve, leading to a significant downward revision in the expected course of short-term interest rates for the next year or so. (15) Under the lower interest rates of alternative A, M2 is expected to grow at a 4-1/2 percent rate over the March-to-June period, keeping this aggregate around the midpoint of its 1992 target range.</t>
+  </si>
+  <si>
+    <t>Under alternative B, federal funds would continue to trade around 4 percent in association with an initial bor- rowing allowance of $100 million. (9) Markets appear to anticipate no change in policy over the intermeeting period, and thus interest rates should remain close to current levels under alternative B. Nevertheless, there could be a downward bias to rate movements over coming months. Under the unchanged reserve conditions of alternative B, M2 growth is projected to moderate to a 3-1/2 percent rate from March to June. (13) As a consequence of rising opportunity costs and waning effects of special factors, M2 velocity is projected to increase sig- nificantly in the second quarter--at about a 2 percent annual rate under alternative B. (14) Growth in M3 under alternative B would moderate slightly to a 1-1/2 percent pace over the March-to-June period.</t>
+  </si>
+  <si>
+    <t>5 In contrast, the funds rate would return to 4-1/2 percent and the initial borrowing allowance would increase to $125 million under alternative C. (11) The tightening of policy under alternative C would lead to about a 50 basis point rise in money market rates, which likely would be passed through fully to the prime rate. (16) M2 growth would slacken to a 2-1/2 percent rate over the March-to-June period under alternative C, bringing this aggregate ap- preciably below the midpoint of its annual range.</t>
+  </si>
+  <si>
+    <t>4 Under alternative A, the federal funds rate would drop to 3-1/4 percent. (10) The extent of the easing of reserve market conditions under alternative A would catch market participants unawares, and the 1/2 point drop in the federal funds rate would induce a nearly compar- able decline in other money market interest rates. However, following an easing move, especially of the dimensions of alternative A, investors would become more assured of sustained economic expansion, but also less confident of any longer-term decrease in inflation, which together would limit any reductions in long-term rates. If the lower funds rate of alternative A is maintained through year-end, growth of M2 for the year could be expected to come in around 4 percent.</t>
+  </si>
+  <si>
+    <t>Under alternative B, federal funds would continue trading in the 3-3/4 percent area; extending the current assumption of $100 million for adjustment plus seasonal borrowing would be expected to preserve the current 1/4 percentage point spread of the funds rate above the discount rate, at least over the first part of the intermeeting period. The same federal funds rate could be achieved by cutting the discount rate 1/2 percentage point to 3 percent and specifying borrowing at the alternative B level of $100 million. Consequently, prices in domestic credit and foreign exchange markets probably would not show much reaction should the Committee main- tain current reserve market conditions by choosing alternative B at this meeting. C Growth from March to June M2 1-1/4 1 3/4 M3 1/4 0 -1/4 M1 9-3/4 9-1/4 8-3/4 Growth from April to June M2 3 2-1/2 2 M3 2 1-3/4 1-1/2 M1 12 11-1/4 10-1/2 (13) Growth of M2 is projected to average 2-1/2 percent at an annual rate over May and June with the essentially stable money market interest rates of alternative B. 990 970 950 930 910 890 ,-' Chart 4 DEBT Billions of dollars - - Actual Level * Projected Level -- 1 12300 -I 12100 -- 11900 .5 1 11700 4.5% -4 11500 - 11300 11100 i I I I I I I I I I I I I I O N D J F M A M J J A S O N D 1991 1992 10900 -13- (14) Under alternative B, the projected turnaround in M2 over May and June should show through to M3, which is expected to register an annual growth rate of 1-3/4 percent; from March to June, M3 would be about unchanged. While growth of M3 for the year of 2 percent is expected under the constant funds rate of alternative B, this projec- tion would have to be shaded up or down by perhaps 1/4 point if alterna- tive A or C were chosen at this FOMC meeting and sustained for the rest of the year. This alternative would stress the Committee's expectation of a resump- tion of growth in broad money over May and June, in contrast to the traditional three-month specification, which would show little if any monetary growth (for example, 1 percent for M2 and zero for M3 under alternative B).</t>
+  </si>
+  <si>
+    <t>Under the policy tightening of alternative C, the federal funds rate would rise to 4-1/4 percent, in association with higher initial borrowing of $125 million. (11) The more restrictive policy of alternative C would come as a considerable surprise to market participants. -14- If alternative C is adopted and the higher rates maintained, a 3 percent annual pace for M2 would be more likely.</t>
+  </si>
+  <si>
+    <t>Under the easier alternative A, the funds rate would be reduced to 3-1/4 percent, placing it 1/4 percentage point below the discount rate, in association with a borrowing assumption of $200 million. -17- (22) Under alternative A, most of the drop of 50 basis points in the funds rate would be transmitted to other money market interest rates. Even under alternative A, M2 would be on a trajectory that would bring it closer to, though still a bit below, its lower bound in the fourth quarter, and M3 also would be expected to remain somewhat below its current range through year-end.</t>
+  </si>
+  <si>
+    <t>Under alternative B, the federal funds rate would continue to center on 3-3/4 percent. Thus, in the near-term, rates would rise somewhat under alternative B. C Growth from June to September M2 2-3/4 2 1-1/4 M3 1 1/2 0 M1 8 6-1/2 5 Growth from QIV'91 to September M2 2 1-3/4 1-1/2 M3 1/4 0 0 M1 11 10-1/2 10 (25) While M2 under all three alternatives appears likely to resume growth over the June-to-September period, under alternative B this aggregate still is projected to grow at only a 2 percent annual rate. (26) The turnaround in M2 growth under alternative B should show through to M3.</t>
+  </si>
+  <si>
+    <t>Under alternative C, the funds rate would be raised to around 4-1/4 percent by selecting a borrowing specification of $250 million. (23) The increase of 50 basis points in the funds rate under alternative C would come as a considerable surprise to market partici- pants.</t>
+  </si>
+  <si>
+    <t>(8) Under alternative A, short-term interest rates would fall by nearly the full 50 basis point drop in the federal funds rate, espe- cially were the easing to take the form of a discount rate cut, which 3. For the June-to-September period, expansion in the broad aggregates is likely to fall well short of the rates envisioned at the time of the last Committee meeting, even if alternative A is adopted. (14) The lower interest rates of alternative A would be expected to buoy money growth over the balance of the year.</t>
+  </si>
+  <si>
+    <t>Under alternative B, federal funds would continue to trade around 3-1/4 percent in combination with an initial allowance for adjustment plus seasonal borrowing of $250 million. Although money market interest rates might firm a bit over the intermeeting period under the unchanged policy of alternative B, any increase would be limited if, consistent with the Greenbook forecast, information continued to suggest modest economic expansion. The dollar, under alternative B, would be expected to trade around its recent lower levels. (12) Under alternative B, M2 is expected to resume expanding this month and to grow at a 2-1/4 percent pace on balance over the remainder of the year. This projec- tion assumes the unchanged federal funds rate of alternative B ex- tended through year-end and the Greenbook economic forecast. (13) The firming in M2 under alternative B shows through in part to M3, which bottoms out in coming months and then edges higher.</t>
+  </si>
+  <si>
+    <t>Alternative C involves a return of the federal funds rate to 3-3/4 percent and a borrowing allowance of $275 million. (9) A reversal of the July easing would take market partici- pants completely by surprise and short-term interest rates would rise by at least 1/2 percentage point under alternative C. Bond rates, too, would retrace some of their recent declines under this alternative, at least initially, and quality spreads on private debt could widen if such a tightening were seen as placing the recovery at risk. (15) Under alternative C, M2 and M3 would drop further below their annual ranges, as opportunity costs widen, banks become even more cautious lenders, and income growth is more restrained.</t>
+  </si>
+  <si>
+    <t>4 Under the easier policy stance of alternative A, the expected federal funds rate would be cut to 2-1/2 percent. With a 1/2 percentage point drop in the dis- count rate, for example, an initial borrowing assumption of $200 million would be retained under alternative A. (9) Projected growth rates of the monetary aggregates under the two policy alternatives appear on the table below. (14) The immediate 1/2 percentage point drop in the federal funds rate under alternative A would exceed the market's expected change. (15) Under alternative A, M2 and M3 likely would grow at rates of 2-3/4 and 1-1/4 percent over the September-to-December interval. In addition to the limited stimulus to M2 demands arising from the reduction in oppor- tunity costs, spending by then should have begun to respond to the -13- monetary policy easing embodied in alternative A. Real interest rates would be lower than under alternative B, though actual declines in real rates may be limited by a continued ebbing of inflation expec- tations.</t>
+  </si>
+  <si>
+    <t>Under alternative B, federal funds would continue to trade around 3 percent, in association with an initial assumption for adjustment plus seasonal borrowing of $200 million. Under these circumstances, selection of the unchanged reserve conditions of alternative B would initially induce some backup in interest rates across the maturity spectrum and some rise in the ex- change value of the dollar. (11) Under alternative B, M2 is projected to grow at a 2 percent rate from September to December, somewhat slower than in the last two months. (12) Under alternative B, the staff foresees M3 growth of 1 percent from September to December, also somewhat slower than over August and September. In addition to the limited stimulus to M2 demands arising from the reduction in oppor- tunity costs, spending by then should have begun to respond to the -13- monetary policy easing embodied in alternative A. Real interest rates would be lower than under alternative B, though actual declines in real rates may be limited by a continued ebbing of inflation expec- tations.</t>
+  </si>
+  <si>
+    <t>6 The policy ease envisaged under alternative A would trim the expected federal funds rate to 2-1/2 percent. Technically, though, the lower federal funds rate of alternative A could be achieved by reducing the borrowing assumption $25 million with an unchanged discount rate. (20) Against a backdrop of public readings that suggested some firming in economic activity, market participants would be sur- prised by the 1/2 point decline in the funds rate under alternative A. -17- Most short-term interest rates would match the decrease in the federal funds rate. (21) While the impetus to the monetary aggregates imparted by choosing alternative A would be barely discernible in 1992, the lower market interest rates embodied in that choice would push up both M2 and M3 to the lower end of their current tentative ranges for 1993 by March.</t>
+  </si>
+  <si>
+    <t>Under alternative B, the trading range for the federal funds rate would remain centered at 3 percent, in conjunction with an initial assumption for adjustment plus seasonal borrowing of $75 mil- lion. Thus, market par- ticipants would be unlikely to react to the unchanged reserve conditions of alternative B, especially if incoming data conform to the Greenbook assessment of moderately expanding real activity in the fourth quarter. (17) Under alternative B, the growth of M2 is projected to slow somewhat from its pace of the last two months.</t>
+  </si>
+  <si>
+    <t>Alternative A incor- porates a 1/2 percentage point reduction in the federal funds rate. (8) The 1/2 percentage point decline in the federal funds rate under alternative A would be passed through fully to other short-term interest rates. (13) The lower interest rates of alternative A would boost M2 growth well into 1993, putting this aggregate near the lower end of the current provisional range by March.</t>
+  </si>
+  <si>
+    <t>Under alternative B, federal funds would continue to trade around 3 percent, in association with the allowance for adjustment and seasonal borrowing remaining at $50 million. With an unchanged federal funds rate under alternative B, other private short-term rates will decline over the intermeeting period as remaining year-end pressures unwind. M1 is projected to grow at a 5-3/4 percent pace from November to March under alternative B. Much of the higher money growth over coming months relative to alternative B would reflect stronger expansion of M1. With issuance of managed liabilities weak, growth in M3 would be boosted only slightly as compared with alternative B, and that aggregate would remain below its provisional target range in March.</t>
+  </si>
+  <si>
+    <t>The 1/2 percentage point increase in the federal funds rate of alternative C could be implemented by raising the borrowing allowance by $25 million. (9) Although many market participants have come to the view that monetary policy easing has run its course for the current economic cycle, none appears to expect a tightening to be implemented in the near term, as in alternative C. Consequently, short-term Treasury rates would jump by the full 50 basis point increase in the federal funds rate. (14) M2 is projected to expand at only a 1 percent rate from November-to-March under alternative C and M3 would decline at a 1/4 percent rate.</t>
+  </si>
+  <si>
+    <t>6 Under alternative A, the federal funds rate would drop to 2-1/2 percent; this could be achieved either through a reduction in the borrowing allowance to $25 million or by a half per- centage point cut in the discount rate with unchanged borrowing. (22) Short-term interest rates--including the prime rate-- would decline by the half-point drop in the federal funds rate under alternative A. Availability constraints on business credit at banks might ease more noticeably should bankers come to see lower rates as improving the outlook for business profitability and lessening strains in this sector. (27) Under alternative A, growth in M2 would pick up to a 1 percent annual rate over February and March, returning this aggregate to its fourth-quarter 1992 level in March. A buildup of institution-only money funds, as holders responded to more attractive rate relationships, would buoy M3 over February and March -21- under alternative A, and hold down the net declines in this aggregate over these two months.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The markets appear to have built in an unchanged policy in the period just ahead </t>
+  </si>
+  <si>
+    <t>Under alternative B, the allowance for adjustment and seasonal borrowing would be retained at $50 million, in association with trading in federal funds continuing to be centered around 3 percent. (21) The markets appear to have built in an unchanged policy in the period just ahead and thus interest rates would be expected to remain near current levels under alternative B. Longer-term rates might come under a little downward pressure if, consistent with the staff greenbook forecast, news on prices continues to be good, and economic indicators point to a little less momentum in the economic expansion than in the second half of last year. The dollar would fluctuate around current levels under alternative B, moving up on any news of unexpected eco- nomic weakness or policy easing abroad, or down should the news about the U.S. economy prove to be softer than expected. C Growth from December to March M2 -1/2 -1 -1-1/2 M3 -2-1/4 -2-1/2 -2-3/4 M1 4-1/2 3-1/2 2-1/2 Growth from 1992Q4 to March M2 -1/4 -1/2 -1 M3 -2-1/4 -2-1/4 -2-1/2 M1 6-1/4 5-1/2 4-3/4 (25) Under alternative B, M2 would be about flat on average over February and March.</t>
+  </si>
+  <si>
+    <t>though market participants seem to believe that some tightening of monetary policy over the next year will be forthcoming, they do not see this happening soon and thus would be surprised by the election of alternative C.</t>
+  </si>
+  <si>
+    <t>Federal funds would trade around 3-1/2 percent under alternative C in combination with a $25 million boost to the borrowing allowance. (23) Although market participants seem to believe that some tightening of monetary policy over the next year will be forthcoming, they do not see this happening soon and thus would be surprised by the election of alternative C. Short-term rates would rise by about 1/2 percentage point. (28) Under alternative C, M2 would decline over February and March as larger opportunity costs act as an additional drag on this aggregate.</t>
+  </si>
+  <si>
+    <t>Under alternative A, the federal funds rate would decline to the 2-1/2 percent area. (9) The easing of policy under alternative A would surprise market participants and would lead to a decline in short-term rates, including the prime rate, commensurate with the 1/2 percentage point drop in the federal funds rate. (14) Under alternative A, M2 would strengthen to a 3 percent rate over the February-to-June period. M3 would grow at a 1-1/4 percent pace over February to June under alternative A, but would remain below its fourth-quarter base even by June.</t>
+  </si>
+  <si>
+    <t>Under alternative B, federal funds would continue to trade around 3 percent in association with the allowance for adjustment plus seasonal borrowing initially remaining at $50 million. This alternative could be implemented through a 1/2 percentage point drop in the discount rate, holding the initial borrowing allowance at the same level as in alternative B, or by lowering the initial borrowing allowance to $25 million and leaving the discount rate unchanged. Thus, under alternative B, short-term interest rates would stay around current levels. The dollar would be expected to fluctuate around current levels under alternative B, but could firm somewhat if rate declines in Europe prove to be faster and larger than now expected. C Growth from February to June M2 3 2-1/2 2 M3 1-1/4 1 3/4 M1 11 9-3/4 8-1/2 Implied growth from 1992:Q4 to June M2 3/4 1/2 1/4 M3 -1 -1 -1-1/4 M1 9 8-1/4 7-1/2 (12) Under alternative B, M2 is expected to resume growth over the February-to-June period.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conversely, the tightening of policy under alternative C, which also would come as a surprise to market participants, would induce a rise in short-term rates comparable to the hike in the federal funds rate. </t>
+  </si>
+  <si>
+    <t>Alternative C, involving a rise in the federal funds rate to 3-1/2 percent, could be implemented through a boost in the initial borrowing allowance to $75 million. Conversely, the tightening of policy under alternative C, which also would come as a surprise to market participants, would induce a rise in short-term rates comparable to the hike in the federal funds rate. Under alternative C, M2 would expand at a 2 percent rate over the February-to- June period, as wider opportunity costs would discourage inflows to more liquid deposits, especially M1 balances.</t>
+  </si>
+  <si>
+    <t>5 Under alternative A, the federal funds rate would be reduced to 2-1/2 percent. exchange markets probably would remain around current levels under alternative B. (10) The 1/2 percentage point reduction in the federal funds rate under alternative A would surprise market participants and should show through almost completely to other short-term interest rates. (16) The lower interest rates of alternative A would be ex- pected to provide some added lift to growth of the monetary aggregates.</t>
+  </si>
+  <si>
+    <t>Thus, market interest rates are unlikely to react to the implementation of alternative B.</t>
+  </si>
+  <si>
+    <t>Under alternative B, federal funds would continue to trade around 3 percent, in association with the allowance for adjustment and seasonal borrowing initially being maintained at its current level of $100 million. Thus, market interest rates are unlikely to react to the implementation of alternative B. exchange markets probably would remain around current levels under alternative B. (10) The 1/2 percentage point reduction in the federal funds rate under alternative A would surprise market participants and should show through almost completely to other short-term interest rates. ,oO----"" Ã‚Â¡ * Ã‚Â¡Ã‚Â¡ oÃ‚Â¡Ã‚Â¡" Ã‚Â¡_x005F_x001A_ Ã‚Â¡Ã‚Â¡Ã‚Â¡" .... %..................................................................... 0% ON D J F M A M J JASO N D J 1250 1200 1150 1100 1050 1000 950 1993 1994 Chart 7 DEBT Billions of Dollars 13000 - Actual Level * Projected Level - 12800 Monthly 4.5% 12600 12400 12200 -112000 -- 11800 --111600 -1 11400 I I I I I I I I I I I I I I I I 111200 O N D J F M A M J J A S O N D J 1993 1994 -11- (13) Under alternative B, M2 is projected to increase at about a 5-3/4 percent average rate over May and June, a considerable pickup from recent months. (14) M3 under alternative B is seen as accelerating to about a 4 percent rate over May and June. Looking further ahead, moderate average growth of M3 during the third quarter would be expected to accompany retention of the specifications of alternative B over that period. Given still-favorable conditions in longer-term markets under alternative B, issuance of corporate bonds and stocks should remain relatively heavy.</t>
+  </si>
+  <si>
+    <t>Market participants also would be surprised by the policy tightening under alternative C at this FOMC meeting.</t>
+  </si>
+  <si>
+    <t>Federal funds would trade in the neighborhood of 3-1/2 percent under alternative C, in association with an initial borrowing allowance of $125 million. (11) Market participants also would be surprised by the policy tightening under alternative C at this FOMC meeting. (17) Under alternative C, the higher money market interest rates and opportunity costs would restrain the monetary aggregates. Maintenance of the money market conditions of alternative C probably would induce M3 to contract on the year.</t>
+  </si>
+  <si>
+    <t>Under alternative A, the funds rate would be reduced to the area of 2-1/2 percent, either by choosing a $225 million borrowing allowance or by cutting the discount rate 1/2 percentage point, to 2-1/2 percent, while retaining a $250 million borrowing allowance. (27) The easing of reserve conditions embodied in alternative A would represent an unexpected direction for policy, especially in light of the market's understanding of the Committee's recent policy predilection. C Growth from June to September M2 1-1/2 1 1/2 M3 1/2 1/4 0 M1 6-3/4 5-3/4 4-3/4 Implied growth from Q4:1992 to September M2 1-1/4 1 3/4 M3 0 0 -1/4 M1 8-3/4 8-1/2 8-1/4 (29) Projected M2 growth over the third quarter diverges rela- tively little across the three alternatives, ranging from 1/2 percentage point under alternative C to 1-1/2 percentage point under alternative A. Given this damped interest rate response, even if the money market conditions of alternative A continued through year- end, M2 growth over the year would still be only 1-1/4 percent, notice- ably below the 2 percent lower bound of the Committee's current annual range. Ã¢Ë†Å¾ Ã¢Ë†Å¾ ' Chart5 M1 - Actual Level * Short-Run Alternatives Billions of Dollars 15% 10%10% -I 1100 0 0 0 5% i --11050 ON D J F MA M J J A S O N D J 1992 1993 1994 1000 1200 1150 Chart 6 DEBT Billions of Dollars - Actual Level - - Estimated Level * Projected Level ON D J 1992 I I I I I I I I I- I I 11400 F M A M J J A S N D J 1993 1994 13000 12800 12600 12400 12200 12000 11800 11600 -22- alternative C to 6-3/4 percent under alternative A.</t>
+  </si>
+  <si>
+    <t>Consequently, market interest rates would not respond initially to the implementation of alternative B</t>
+  </si>
+  <si>
+    <t>Under alternative B, federal funds would remain in a trading range around 3 percent, in association with an initial allowance for adjustment plus seasonal borrowing of $250 million, an increase of $50 million from the current allowance to accommodate the normal pattern in seasonal borrowing at this time of the year. Consequently, market interest rates would not respond initially to the implementation of alternative B. Rates would tend to remain near current levels or edge lower over subsequent weeks should data on economic activity and prices prove to be about in line with the staff projection and should the Congress continue to make progress on passage of a deficit reduction package. Total reserves and the monetary base are projected to grow from June to September at 5-3/4 and 8-1/4 percent rates, respectively, under alternative B. -23- Directive Language (32) Presented below are draft paragraphs relating to the ranges for 1993 and 1994.</t>
+  </si>
+  <si>
+    <t>The immediate tightening of reserve market conditions under alternative C is not built into financial market quotes and would induce a rise in short-term market interest rates that about matched the 1/2 percentage</t>
+  </si>
+  <si>
+    <t>Under alternative C, which could be imple- mented through a $275 million borrowing allowance, the funds rate would vary around 3-1/2 percent. (26) The immediate tightening of reserve market conditions under alternative C is not built into financial market quotes and would induce a rise in short-term market interest rates that about matched the 1/2 percentage point increase in the federal funds rate. C Growth from June to September M2 1-1/2 1 1/2 M3 1/2 1/4 0 M1 6-3/4 5-3/4 4-3/4 Implied growth from Q4:1992 to September M2 1-1/4 1 3/4 M3 0 0 -1/4 M1 8-3/4 8-1/2 8-1/4 (29) Projected M2 growth over the third quarter diverges rela- tively little across the three alternatives, ranging from 1/2 percentage point under alternative C to 1-1/2 percentage point under alternative A. Ã‚Â° Ã‚Â° ' Chart5 M1 - Actual Level * Short-Run Alternatives Billions of Dollars 15% 10%10% -I 1100 0 0 0 5% i --11050 ON D J F MA M J J A S O N D J 1992 1993 1994 1000 1200 1150 Chart 6 DEBT Billions of Dollars - Actual Level - - Estimated Level * Projected Level ON D J 1992 I I I I I I I I I- I I 11400 F M A M J J A S N D J 1993 1994 13000 12800 12600 12400 12200 12000 11800 11600 -22- alternative C to 6-3/4 percent under alternative A.</t>
+  </si>
+  <si>
+    <t>5 Under alternative A, the federal funds rate would decline to 2-1/2 percent, either through a drop in the borrowing allowance to $225 million or a cut in the discount rate of 50 basis points in combination with an unchanged level of borrowing. (11) The easing under alternative A would come as a surprise to market participants, and short-term rates would decline by the full 50 basis point drop in the funds rate. (12) In light of the likelihood of some decline in an array of real interest rates, as well as the real foreign exchange value of the dollar, alternative A might be favored if economic growth in the staff forecast were seen to be unsatisfactory and the Committee were willing to accept little or no further disinflation. Faster growth in M2 under alternative A owes both to more growth in nominal income later in the year than under alternative B and to the improvement in the attrac- tiveness of assets in M2 relative to money market instruments. M3 under alternative A would expand slowly over the final four months of the year as bank credit growth remained damped in the context of continued heavy financing in the securities markets.</t>
+  </si>
+  <si>
+    <t>Under alternative B, federal funds would continue to trade around 3 percent in association with an allowance for adjustment plus seasonal borrowing of $250 million. Thus, under alternative B, short-term interest rates should remain around current levels in the weeks ahead. (8) The interest rates under alternative B are consistent with those of the staff Greenbook forecast, which has the federal funds rate around current levels through 1994 and long-term rates edging lower. (9) Over the balance of 1993, M2 is projected to grow at about a 1-1/2 percent pace under alternative B, and, as shown in the table below, to finish the year around the lower bound of its new annual range. 7 M3 under alternative B is projected to bottom out in August and to edge higher over the remainder of the year. The lower interest rates of this alternative would tend to boost money growth relative to alternative B and, under the spending propensities incorporated in the staff forecast, would give a little more assurance that the broad aggregates would finish the year at or above the lower bounds of their ranges for 1993. Faster growth in M2 under alternative A owes both to more growth in nominal income later in the year than under alternative B and to the improvement in the attrac- tiveness of assets in M2 relative to money market instruments.</t>
+  </si>
+  <si>
+    <t>The tightening of policy under alternative C would come much sooner than is now envisioned by market participants.</t>
+  </si>
+  <si>
+    <t>Under alternative C, the federal funds rate would rise to 3-1/2 percent accompanying a boost in adjustment plus seasonal borrowing to $275 mil- lion. (13) The tightening of policy under alternative C would come much sooner than is now envisioned by market participants. (14) Alternative C might be favored if the Committee saw a need to move sooner, rather than later, to contain or reduce future inflationary pressures. With the staff's outlook for spending propensities, M2 would expand at only a 1 percent pace over the final five months of this year under alternative C, ending the year about 3/4 percent above its fourth- quarter 1992 level.</t>
+  </si>
+  <si>
+    <t>(10) Under alternative A, money market interest rates would drop by the full 50 basis point decline in the federal funds rate. Alternative A might also be chosen if the Committee saw economic activity and inflation as possibly coming in below the staff forecast; market perceptions that the Committee was signalling an expectation that the outlook for real activity had deteriorated and for disinflation had improved could result in sub- stantial declines in bond yields.</t>
+  </si>
+  <si>
+    <t>Market participants apparently believe that the federal funds rate will remain at 3 percent</t>
+  </si>
+  <si>
+    <t>Under alternative B, federal funds would continue to trade around 3 percent in combination with an initial allowance for adjustment plus seasonal borrowing of $250 million. (7) Alternative B is consistent with the staff's economic forecast. Market participants apparently believe that the federal funds rate will remain at 3 percent, at least for the next several months, and under alternative B, money market interest rates would remain around current levels. (9) As shown in the table below, M2 under alternative B is projected to grow at a 2 percent average rate over the final four months of this year. Under alternative B, M3 would grow at a 3/4 percent rate over the remainder of this year, leaving this aggregate just above both its fourth-quarter 1992 level and the bottom of its 8. These growth rates would place both aggregates near the bottom of their annual ranges for this year, and on a lower trajectory going into 1994 than under alternative B, partly reflecting damped income growth.</t>
+  </si>
+  <si>
+    <t>Under alternative C, the federal funds rate would rise to 3-1/2 percent in association with a boost in the initial borrowing allowance. (12) Under alternative C, interest rates would rise and the dollar would strengthen on foreign exchange markets. (13) Alternative C might be favored if the modest degree of price deceleration in the staff forecast were viewed to be unsatis- factory.</t>
+  </si>
+  <si>
+    <t>This alternative may surprise market participants.</t>
+  </si>
+  <si>
+    <t>(12) Alternative A contemplates an easing in reserve market pressures and a decline in the federal funds rate to 2-1/2 percent. 13 Implementation of alternative A would be especially surprising to market participants, given their view that underlying economic growth is strengthening. (13) Alternative A might be viewed as appropriate if the Com- mittee wished to make appreciable progress in reducing remaining slack in the economy, in contrast to the plateau for the unemployment rate seen in the staff forecast.</t>
+  </si>
+  <si>
+    <t>Under alternative B, the federal funds rate would continue to trade around 3 percent. C Growth from October to December M2 2-1/2 2 1-1/2 M3 1-1/4 1 1 M1 11-1/2 10-1/2 9-1/2 Growth from October to March 1994 M2 3 2-1/2 2 M3 1-3/4 1-1/2 1-1/4 M1 11-1/4 10-1/2 9-1/2 (9) As shown in the lower panel of the above table, M2 under alternative B is projected to grow at a 2-1/2 percent rate over October to March.</t>
+  </si>
+  <si>
+    <t>(10) Under Alternative C, the federal funds rate would rise 1/2 percentage point to 3-1/2 percent. (11) The Committee might favor alternative C if strength in recent economic data were seen as implying that any delay in firming ran an unacceptably high risk that economic activity could develop excessive momentum that would rapidly erode the remaining degree of slack and produce an acceleration of prices.</t>
+  </si>
+  <si>
+    <t>In the case of alternative A, the federal funds rate would decline to 2-1/2 percent and borrowing would fall, perhaps to $25 million. (13) The easing of policy under alternative A would come as a surprise to market participants, and short-term interest rates would fall by about the 50 basis point drop in the federal funds rate. Under alternative A, M2 would expand at a 2-1/4 percent pace, close to that evident since midyear, buoyed partly by less of a slowdown in M1 than under alternatives B and C, M3 would grow at a 1-1/4 percent pace from November to March. (14) Alternative A might be favored if the current strength in the economy were seen as likely to give way to a significant weak- ening in the pace of expansion next year, considering the greater fiscal restraint in train and the backup in long-term interest rates and the dollar since mid-October.</t>
+  </si>
+  <si>
+    <t>Under alternative B, federal funds would continue to trade around 3 percent in association with adjustment plus seasonal borrowing at the discount window of $50 million. (7) Alternative B is consistent with the policy assumptions underlying the staff economic forecast. Nonetheless, market interest rates are unlikely to move down much on balance under the steady funds rate of alternative B in coming months, since the market would continue to expect a tightening before long. The foreign exchange value of the dollar under alternative B should stay around current levels. M2 by March would have expanded at a 2 per- cent annual rate from its fourth-quarter 1993 base under alternative B, placing this aggregate well above the lower end of its provisional 1 to 5 percent growth range for next year. (10) Under alternative B, M3 would advance at a 1 percent annual rate over the November-to-March period; by March this aggregate would be 1-1/4 percent above its fourth-quarter 1993 base, well within its 0 to 4 percent provisional range for 1994.</t>
+  </si>
+  <si>
+    <t>The rise in the federal funds rate under alternative C, to 3-1/2 percent, would come sooner than now anticipated by market participants and built into markets interest rates.</t>
+  </si>
+  <si>
+    <t>Under alternative C, the federal funds rate would move up to 3-1/2 percent and the borrow- ing allowance to $75 million. (11) The rise in the federal funds rate under alternative C, to 3-1/2 percent, would come sooner than now anticipated by market participants and built into markets interest rates. M3 would expand under alternative C at only a 3/4 percent pace over the November-to- March period. (12) Alternative C might be preferred if there were concerns about the inflation outlook.</t>
+  </si>
+  <si>
+    <t>Alternative A embodies a downward adjustment of the federal funds rate to 2-1/2 percent and of the borrowing allowance to $25 million. (27) The easing of policy under alternative A would come as more of a surprise to market participants.</t>
+  </si>
+  <si>
+    <t>Market participants now anticipate continuation of the money market conditions implied by alternative B over the near term, and FOMC choice of this alternative would not engender any immediate reaction in security markets.</t>
+  </si>
+  <si>
+    <t>Alternative B involves a continuation of feder- al funds trading around 3 percent and of adjustment plus seasonal borrowing averaging initially about $50 million. (25) Market participants now anticipate continuation of the money market conditions implied by alternative B over the near term, and FOMC choice of this alternative would not engender any immediate reaction in security markets. C Growth from January to June M2 2-1/4 2 1-3/4 M3 1-1/2 1-1/4 1 M1 7-1/2 6-3/4 6 Growth from 1993:Q4 to June M2 2-1/4 2 1-3/4 M3 1-3/4 1-1/2 1-1/4 M1 7-1/4 6-3/4 6-1/4 (29) M2 growth likely will be held down under alternative B by a reversal of the previous bulge attributable to mortgage refinanc- ing activity, which had boosted average M2 growth by an estimated 1 percentage point during the October through December months, before becoming a minor drag in January. With demand deposits most affected by mortgage refinancing activity, M1 growth from January to June will be depressed by around 4 percentage points by this special factor under alternative B. Growth of M1 is projected at 6-3/4 percent over this period, implying growth of total reserves and the monetary base of 4-3/4 and 9-1/2 percent, respectively. (30) M3 is projected to expand at a 1-1/4 percent rate from January to June under alternative B.</t>
+  </si>
+  <si>
+    <t>The firming in the stance of policy under alternative C would come sooner than now built into market quotes</t>
+  </si>
+  <si>
+    <t>(26) The firming in the stance of policy under alternative C would come sooner than now built into market quotes and would be re- flected in increases in short-term rates nearly equal to the 50 basis 12.</t>
+  </si>
+  <si>
+    <t>With market participants expecting appreciable increases in the federal funds rate in coming months, including 25 basis points at the March FOMC meeting, interest rates could tend to drift lower under the unchanged reserve conditions of alternative B</t>
+  </si>
+  <si>
+    <t>Under alternative B, federal funds would continue to trade around 3-1/4 percent in association with ad- justment plus seasonal borrowing of $75 million. (9) With market participants expecting appreciable increases in the federal funds rate in coming months, including 25 basis points at the March FOMC meeting, interest rates could tend to drift lower under the unchanged reserve conditions of alternative B. Rate de- clines would be quite small initially if market participants still believed that the next tightening step was imminent but had merely been delayed, perhaps by the unsettled market conditions of late. (10) Alternative B might be favored if most of the increase in intermediate- and long-term real rates over recent months were thought likely to persist and be sufficient to restrain demand and 8. Even if long-term rates were expected to decline appreci- ably, alternative B might be selected were the economy nevertheless seen as remaining below its long-term potential and inflation pres- sures contained. C Growth from February to June M2 2-1/2 2-1/4 M3 1-1/2 1-1/4 Ml 6 5-1/4 Implied growth from 1993:Q4 to June M2 2 1-3/4 M3 1/2 1/4 M1 6 5-3/4 (16) Growth in M2 would average 2-1/2 percent at an annual rate over the February-to-June period under alternative B, up from only 3/4 percent over January and February, even as growth in nominal income continues to slow. Nonetheless, M2 velocity would con- tinue to rise in the second quarter under alternative B, but its 2-3/4 percent annual pace of expansion would be well below that of the two previous quarters. Under alternative B, this aggregate would expand at a 1-1/2 percent pace over the February-to-June period.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Alternative C involves a larger immediate tightening than now built into the structure of market rates.</t>
+  </si>
+  <si>
+    <t>(11) Alternative C involves a larger immediate tightening than now built into the structure of market rates. (12) In addition to possibly contributing to more settled market conditions, alternative C might be preferred if the Committee saw significant risks of greater inflation going forward. Under alternative C, M2 would grow at a 2-1/4 percent rate over the February-to-June period, restrained by weaker inflows to liquid components as opportunity costs widen more. Still, by June, M2 would have grown at a 1-3/4 percent rate from its fourth-quarter 1993 base under alternative C, above the lower end of its 1994 annual range. Under alternative C, M3 would pick up by less, expanding at a 1-1/4 percent rate over February to June, restrained by some further outflows from M3-type money market funds. By June, M3 would stand 1/4 percent at an annual rate above its fourth-quarter base under alternative C, only a little above the lower end of its annual growth cone.</t>
+  </si>
+  <si>
+    <t>Under alternative B. federal funds would continue to trade around 3-3/4 percent, in association with the al- lowance for adjustment plus seasonal borrowing remaining initially at $175 million. (14) The case for standing pat, alternative B, is a more extreme version of the rationale for alternative C: In this case, the market assessment, and even that of the staff, of the strength of aggregate demand would be judged to be seriously off the mark, perhaps because the rise in long-term rates, along with the decline in house- hold wealth, will have a more significant restraining influence on aggregate demand. Choice of alternative B would come as a consider- able surprise--and disappointment--to financial markets; very short- term interest rates would be likely to fall appreciably, but this alternative risks a significant sell-off in the bond market before weakness in aggregate demand becomes apparent.</t>
+  </si>
+  <si>
+    <t>5 Under alternative C, the federal funds rate would move up 1/4 percentage point (one-half the usual adjustment shown in previous bluebooks for "alternative C") to 4 percent, effectuated by increasing the initial borrowing allowance to $200 million. (13) The case for increasing the intended federal funds rate only 25 basis points as under alternative C would seem to hinge on the judgment that financial market participants have exaggerated the like- ly strength of future spending relative to the economy's potential and hence of prospective inflation pressures. (14) The case for standing pat, alternative B, is a more extreme version of the rationale for alternative C: In this case, the market assessment, and even that of the staff, of the strength of aggregate demand would be judged to be seriously off the mark, perhaps because the rise in long-term rates, along with the decline in house- hold wealth, will have a more significant restraining influence on aggregate demand.</t>
+  </si>
+  <si>
+    <t>Under alternative D, the federal funds rate would be raised to 4-1/4 per- cent, either by increasing the initial borrowing allowance to $225 million or by raising the discount rate to 3-1/2 percent, while keep- ing the initial allowance for discount window borrowing at $175 mil- lion. Very short-term rates might thus increase slightly under alternative D. The behavior of rates on instruments of a few months' maturity or longer would depend importantly on whether the market interpreted the larger increase of alternative D as indicating a steeper trajectory of future policy actions, and perhaps the need for greater cumulative tightening. Bond yields could still back up somewhat in the aftermath of an announce- ment of the Federal Reserve's choice of alternative D, but these other influences should limit any increase and work to reduce yields over time. The recent increases in opportunity costs on liquid retail deposits aris- ing from the previous tightenings in the stance of monetary policy, and under alternative D from an additional firming move as well, will serve to hold back growth of M1 and some of the other components of M2 and M3.</t>
+  </si>
+  <si>
+    <t>Alternative B might be chosen by the Committee if it wished to await confirmation of the strength of aggregate demand, perhaps because there were questions about whether that strength would in fact be forthcoming. Accordingly, short-term interest rates are likely to move down a little after the meeting under alternative B. Long-term rates are not likely to decline, however, under this alternative; the dollar 15. M1 is expected to increase at only a 3-1/2 percent rate from June to September under alternative B.17 (32) Expansion of M3 is projected to pick up only slightly in the next few months.</t>
+  </si>
+  <si>
+    <t>15 The federal funds rate would be boosted 1/4 percentage point to 4-1/2 percent under alternative C, and the borrow- ing allowance would be raised to $350 million. (28) The Committee could see alternative C as appropriate if it believed that sufficient evidence had accumulated to warrant a continued gradual tightening of policy to prevent the economy from overheating.</t>
+  </si>
+  <si>
+    <t>Alternative D would increase the federal funds rate 1/2 percentage point to 4-3/4 percent. (29) Concerns that the recent behavior of the dollar and commodity prices might imply rising prices more broadly and might be associated with a ratcheting up of inflation expectations could moti- vate the Committee to select alternative D.</t>
+  </si>
+  <si>
+    <t>Under alternative B, federal funds would continue to trade around 4-1/4 percent in association with re- taining the $450 million allowance for adjustment plus seasonal bor- rowing. (8) Alternative B might be preferred if it were thought that there would be less strength in the economy than in the staff fore- cast. In these circumstances, the choice of no change in the stance of policy under alternative B would result in some decline in short-term interest rates, and the dollar might tend to weaken on foreign exchange markets. The path for alternative B -10- is based on the assumption of no change in the federal funds rate for the rest of this year. D Growth from July to December M2 1-1/2 1 M3 3/4 1/2 M1 3 2-1/4 Implied growth 93Q4 to 94Q4 M2 1-1/2 1-1/4 M3 1/2 1/2 M1 4 3-1/2 (15) M2 would grow at a 1-1/2 percent rate over the July-to- December period under alternative B, down from the July pace but quicker than that over the first six months of the year. Moreover, with short-term rates unchanged under alternative B, insti- tution-only money funds should be stable after large runoffs through the spring. M1 would expand at about a 3 percent rate over the July-to- December period under alternative B. Continued rapid currency growth would account for this expansion, as higher opportunity costs reached earlier this year and slow mortgage refinancing activity hold transaction deposits about flat.</t>
+  </si>
+  <si>
+    <t>As noted above, alternative C is about what is built into the structure of market interest rates, and neither interest nor exchange rates are likely to react very strongly to such an actio</t>
+  </si>
+  <si>
+    <t>8 Under alternative C, the federal funds rate would be raised to 4-1/2 percent and the initial borrowing allowance to $475 million. (11) Alternative C embodies a move of 25 basis points. As noted above, alternative C is about what is built into the structure of market interest rates, and neither interest nor exchange rates are likely to react very strongly to such an action. In this regard, the 50 basis points of alternative D would imply more assurance of this outcome than alternative C and, therefore, would be more likely to be followed by a period of stability of short-term rates. 9 (Money growth under the reserve conditions of alternative C would lie half way between alternatives B and D.) Alt.</t>
+  </si>
+  <si>
+    <t>Under alternative D, the funds rate would be moved to 4-3/4 percent, either through an increase in the initial borrowing allowance to $500 million or a hike in the discount rate to 4 percent and un- changed adjustment plus seasonal borrowing. (12) The more forceful move of alternative D might be chosen if the Committee viewed the economic situation as highly likely to require substantial additional monetary tightening, for example, of the scope embodied in the steep tilt to the yield curve over the next few years. In this regard, the 50 basis points of alternative D would imply more assurance of this outcome than alternative C and, therefore, would be more likely to be followed by a period of stability of short-term rates. Alternative D assumes a 50 basis point increase in the funds rate at this meeting and no change thereafter. Although these money growth rates are roughly the same as those projected for alternative D, the higher year-end level of rates assumed in the Greenbook implies slower growth of money and income in the first half of 1995 than would alternative D. Alternative Levels and Growth Rates for Key Monetary Aggregates M2 Alt. (16) Under alternative D, M2 would grow at a 1 percent rate over the July-to-December period.</t>
+  </si>
+  <si>
+    <t>Nonetheless, maintenance of existing reserve conditions under alternative B might elicit little reaction in rates beyond the very shortest maturities because market participants would assume that tightening had simply been postponed.</t>
+  </si>
+  <si>
+    <t>Under alternative B, the federal funds rate would continue to trade around 4-3/4 percent, consistent with retaining an allowance of $475 million for adjustment plus sea- sonal borrowing. (8) Alternative B, which would retain current reserve condi- tions, is not inconsistent with the staff assumption of policy firm- ing, provided that firming resumes some time soon. Nonetheless, maintenance of existing reserve conditions under alternative B might elicit little reaction in rates beyond the very shortest maturities because market participants would assume that tightening had simply been postponed. For illustrative purposes, the path under alternative B was derived assuming that the funds rate would hold at its current level for the remainder of the year. D Growth from September to December M2 1-1/2 1/2 M3 1-1/4 3/4 M1 2-1/2 1-1/2 Implied growth from 93:Q4 to 94:Q4 M2 1-1/4 1 M3 3/4 3/4 M1 3-1/4 3 (14) Over the September-to-December period, M2 would expand at a 1-1/2 percent rate under alternative B. As a result, under alternative B, the monetary base should expand at about a 8-1/4 percent rate, while total reserves should grow at a 1-3/4 percent rate over the September-to-December period.</t>
+  </si>
+  <si>
+    <t>Alternative C is consistent with the current structure of market rates, and this policy action might well trigger only muted interest rate reactions.</t>
+  </si>
+  <si>
+    <t>5 Alternative C envisages raising the federal funds rate 1/4 percentage point, to 5 percent, in conjunction with an increase in the borrowing allowance to $500 million. If the Committee were uncertain about how much tightening would be required but wanted to respond to recent data, the more modest 25 basis point move of alternative C might be considered appropriate. (11) The 25 basis point tightening of alternative C is con- sistent with the current structure of market rates, and this policy action might well trigger only muted interest rate reactions. How- ever, since most market participants expect either no action or a 50 basis point tightening, alternative C could raise questions about System intentions, potentially unsettling markets. (The response of the aggregates under alternative C would lie midway between the two alternatives.)</t>
+  </si>
+  <si>
+    <t>The 50 basis point firming of alternative D is the most likely of the three policy options to keep the Federal Reserve "ahead of the curve" of inflation pressures and consequently to limit the extent to which policy might later need to tighten. A considerable portion of the 50 basis point increase in the federal funds rate under alternative D would pass through to other short-term rates. The path for the aggregates under alternative D assumes that the funds rate moves up to 5-1/4 percent at this meeting and stays there for the balance of the year. (15) Under alternative D, M2 would grow at a 1/2 percent rate over the September-to-December period. M3 would grow at a 3/4 percent rate over the remaining months of the year, pulled down by a runoff of institu- tion-only money funds as their yields lag behind the increase in money market rates that would be in train under alternative D. 6.</t>
+  </si>
+  <si>
+    <t>Alternative B would keep the intended federal funds rate unchanged at 4-3/4 percent, in association with retaining an allowance of $225 million for adjustment plus sea- sonal borrowing at the discount window. (9) Choice of the unchanged policy of alternative B might be based on the judgments that most of the effects of previous increases in interest rates are still in the pipeline, that convincing signs of higher inflation have not yet appeared, and that under these circum- stances the Committee can await evidence indicating whether the effects of previous monetary tightening will be sufficient to restrain spending adequately. 5 (More detailed data appear on the table and charts on the following pages.) Under alternative B, offering rates through the first quarter would continue to adjust upward in the face of steady money market rates. M1 is projected to decline at a 1 percent rate from October to March under alternative B, as currency flows abroad remain robust but demand and other checkable deposits continue to decline. Rapid issuance of large time deposits will continue to fill some of the gap left by still-sluggish retail deposits, and thus M3 is projected to outpace M2 from October to March, likely expanding at a 2-1/2 percent rate under alternative B. Alt. C Growth from October to March M2 1 0 M3 2-1/2 2 M1 -1 -2 Implied growth from 1994:Q4 to March M2 1-1/2 1/2 M3 2-1/2 2-1/4 M1 0 -1-1/4 (16) Under the 50 basis point increase in the funds rate of alternative C, both M2 and M3 would record slower growth over the next five months than under alternative B.</t>
+  </si>
+  <si>
+    <t>With market participants generally appearing to have built in a move of at least this size, interest rates could exhibit little initial reaction to the implementation of alternative C</t>
+  </si>
+  <si>
+    <t>4 Alternative C embodies a 50 basis point increase in the federal funds rate to 5-1/4 percent, accomplished either by an equal rise in the discount rate to 4-1/2 percent with the borrowing allowance kept at $225 million or by an increase in the borrowing allowance to $275 million at the current discount rate of 4 percent. A still larger increase in the federal funds rate than envisioned under alternative C is also discussed. (12) With market participants generally appearing to have built in a move of at least this size, interest rates could exhibit little initial reaction to the implementation of alternative C. C Growth from October to March M2 1 0 M3 2-1/2 2 M1 -1 -2 Implied growth from 1994:Q4 to March M2 1-1/2 1/2 M3 2-1/2 2-1/4 M1 0 -1-1/4 (16) Under the 50 basis point increase in the funds rate of alternative C, both M2 and M3 would record slower growth over the next five months than under alternative B.</t>
+  </si>
+  <si>
+    <t>Alternative B would keep the intended federal funds rate at 5-1/2 percent. In these circumstances, and given the seemingly greater confidence of late in financial markets that the System will act as appropriate to counter a buildup in inflationary pressures, interest rates and the foreign exchange value of the dollar are unlikely to change very much in the immediate aftermath of a deci- sion to leave policy unchanged, as under Alternative B. Movements in financial markets subsequently will depend, of course, on the nature of incoming data. C M2 1-1/4 1/2 M3 2-1/4 2 M1 -1 -2 (15) Under alternative B, M2 would strengthen to a 1-1/4 percent rate over the November-to-March period. M2 would expand at only a 1/2 percent rate over the Novem- ber-to-March period, restrained by faster runoffs of M1 and savings deposits (including MMDAs) than under alternative B.</t>
+  </si>
+  <si>
+    <t>Alternative C entails a 50 basis point rise in the federal funds rate, to 6 percent, achieved either through an equivalent increase in the discount rate with the same path for the borrowing allowance or an increase in the initial borrowing allowance to $175 million, with the same seasonal reductions thereafter. (11) The 1/2 percentage point rise in the federal funds rate under alternative C might be favored if the Committee viewed the recent string of surprisingly strong economic data as clearly indicat- ing that the risks are still tilted in the direction of sustained faster inflation. The inclination to adopt alternative C would be bolstered by a belief that financial markets have largely absorbed the Orange County shock and the risks of further disruptions are de minimus. (12) Under alternative C, money market interest rates would firm somewhat, especially those at the shortest end, as the tightening would come somewhat sooner than now expected. The staff expects the growth of the monetary aggregates to remain damped over coming months, restrained by prior (and under alternative C, current) increases in opportunity costs. (16) Under alternative C, opportunity costs would tend to increase as the rise in money market rates outpaced those on M2 com- ponents.</t>
+  </si>
+  <si>
+    <t>While market participants currently anticipate a 50 basis point increase in the federal funds rate at this meeting, their response to the Committee's selection of alternative B would depend on how the decision were interpreted.</t>
+  </si>
+  <si>
+    <t>Under alternative B, federal funds would continue to trade around 5-1/2 percent, in association with keeping the allowance for adjustment plus seasonal borrowing at $75 million. (26) Choice of alternative B might be viewed as appropriate if the Committee desired additional readings on the extent of the economy's forward momentum and of underlying inflationary pressures to provide a firmer basis for judging whether incremental restraint will be required to damp aggregate demand sufficiently. (27) While market participants currently anticipate a 50 basis point increase in the federal funds rate at this meeting, their response to the Committee's selection of alternative B would depend on how the decision were interpreted. C Growth from January to June M2 2-1/4 1-1/2 M3 2-1/2 2 M1 1 -1/4 Growth from 1994:Q4 to June M2 2-1/2 2 M3 3 2-3/4 M1 1 1/4 (31) Under the unchanged federal funds rate of alternative B, M2 growth would be supported by some narrowing of its opportunity cost, as offering rates on retail deposits rise further in partial catch-up to earlier increases in short-term interest rates. (32) Under alternative C, the 1/2 percentage point higher funds rate would induce less rapid expansion of M2 and M3 than under alternative B as opportunity costs resumed their upward movement.</t>
+  </si>
+  <si>
+    <t>Alternative C is in line with current financial market expectations.</t>
+  </si>
+  <si>
+    <t>Under the tighter alternative C, the federal funds rate would be raised 1/2 percentage point, to 6 percent, either by an equivalent rise in the discount rate to 5-1/4 percent with the same borrowing allowance or by an increase in the borrowing allowance to $125 million with the same discount rate. (28) Concern about the possibility of an adverse market reaction, combined with a view that the economic situation still pointed to significant risk of accelerating inflation, would argue for the 50 basis point firming in the federal funds rate associated with alternative C. (29) The 1/2 percentage point rise in the federal funds rate embodied in alternative C, by matching current financial market expec- tations, would have few initial repercussions on market interest rates or exchange rates against our other G-10 trading partners. (32) Under alternative C, the 1/2 percentage point higher funds rate would induce less rapid expansion of M2 and M3 than under alternative B as opportunity costs resumed their upward movement. Growth rates of 1-1/2 percent and 2 percent, respectively, from January to June are anticipated by the staff under alternative C. 11.</t>
+  </si>
+  <si>
+    <t>Alternative A, involving a reduction of the intended funds rate to 5-1/2 percent, could be effected by lowering either the borrowing allowance to $50 million or the discount rate by 50 basis points. In effect, choice of alternative A would imply a view that not only have longer-term interest and exchange rates not overshot on the downside, but that policy may still be too tight to allow markets to compensate fully for oncoming economic weakness. (13) The 50 basis point easing of the federal funds rate under alternative A also would surprise market participants. Somewhat slower growth in the monetary aggre- gates would result from the higher opportunity costs of alternative C, while somewhat faster growth would occur under alternative A. -... *. . * A - - ,- '- " .... .... ..................................... B................. 0% Dec 1200 1150 -- 1100 Feb 1050 1994 Aug I I I I I I II I I I I I '' '''''' '' '' '' 1995 Chart 5 DEBT Billions of Dollars 1 14200 Actual Level S Projected Level - 14000 -- 13800 --1 13600 13400 - 13200 -- 13000 -- 12800 - 12600 Aug Dec 1994 Dec SI I I I l-I I II L 1995 the growth of the broader aggregates be expected to breach the upper or lower bands of their annual ranges, although M3 is virtually at the upper end of its range under alternative A. (15) Consistent with the forecasted moderation in nominal spending, the debt of domestic nonfinancial sectors is expected to slow to around a 4-3/4 percent pace from February to September, bring- ing its rate of growth from the fourth quarter of last year to 5 per- cent--the mid-point of its monitoring range.</t>
+  </si>
+  <si>
+    <t>Under alternative B, federal funds trading would continue around 6 percent, in association with adjustment plus seasonal borrowing of $75 mil- lion. If the Committee believes such an outcome were both likely and acceptable, then it may be inclined to leave the current level of the federal funds rate in place, as under alternative B, unless and 6. Consequently, there would likely be little change in interest rates in response to the choice of alternative B. (14) The table below shows staff projections of money and debt aggregates through September under the unchanged reserve market conditions of alternative B. (More detailed data, including money growth rates under alternatives A and C, are shown in the table and charts on the following pages.) From a March base, average M2 growth would pick up to a 2-1/2 percent rate, while average M3 growth would slow to a 3 percent pace. The Alternative B Growth from March to September M2 2-1/2 M3 3 M1 1/4 Domestic Nonfinancial Debt1 4-3/4 Growth from 1994:Q4 to September M2 2-1/4 M3 3-3/4 M1 1/4 Domestic Nonfinancial Debt 5 1.</t>
+  </si>
+  <si>
+    <t>With financial markets having built in no near-term monetary policy tightening, choice of alternative C would come as a surprise.</t>
+  </si>
+  <si>
+    <t>6 Under alternative C, the federal funds rate would be in- creased to 6-1/2 percent by raising either the borrowing allowance to $125 million or the discount rate by 50 basis points. (10) A case for the 1/2 percentage point increase in the federal funds rate of alternative C could be made on the grounds that, with economic activity having already overshot its potential and the persistence of the slowdown in economic growth not yet firmly estab- lished, more insurance should be taken out against a serious deterior- ation in inflation trends. (11) With financial markets having built in no near-term monetary policy tightening, choice of alternative C would come as a surprise. Somewhat slower growth in the monetary aggre- gates would result from the higher opportunity costs of alternative C, while somewhat faster growth would occur under alternative A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> This alternative would represent a considerably more aggressive policy action than currently is priced into financial markets.</t>
+  </si>
+  <si>
+    <t>Alternative A would reduce the intended trading level of the funds rate to 5-1/2 percent. Alternative C could be accomplished through an increase in the borrowing allowance to $275 million, while alternative A could be implemented by leaving the allowance for borrowing unchanged at $175 million in the face of seasonally elevated demand. (12) The Committee might consider the easing of monetary policy under alternative A appropriate if it saw substantial risks that the recent sluggish growth of final demand and the associated inventory correction could develop into a prolonged period of growth below potential. (13) Short-term market rates under alternative A would like- ly drop close to one-half percentage point.</t>
+  </si>
+  <si>
+    <t>Under alternative B, federal funds would continue to trade around 6 percent. If the Committee sees the staff forecast as the likely and desired outcome and the risks around it to be reasonably well-balanced, then selection of unchanged reserve market conditions, as under alternative B, would be favored. To accommodate rising demands for seasonal credit, the allowance for adjustment and seasonal borrowings would be raised initially to $225 million under alternative B. Further increases would likely be necessary during the intermeeting period under all of the alterna- tives. Thus, market rates would not be expected to react to selection of alternative B by the Committee. (14) Growth of the monetary and credit aggregates under the unchanged reserve market conditions of alternative B is presented in the table below. Nonetheless, M3 is projected to remain above the upper end of its current 0-to-4 percent annual range through September under alternative B, and even the tighter reserve market conditions of alternative C would not likely be adequate to bring M3 within its range by September. (17) M2 growth, by contrast, is projected to edge up slight- ly from that of the previous four months, to a 2-1/2 percent pace over April through September; this aggregate would remain in the lower half of its l-to-5 percent annual range under alternative B. Although slower growth of nominal income over the second and third quarters will damp the demand for money, opportunity costs of holding M2 assets have leveled off and begun to fall; as the depressing effects of earlier increases in opportunity costs diminish, M2 should grow more closely in line with income.</t>
+  </si>
+  <si>
+    <t>With markets apparently having concluded that rates are unlikely to rise significantly further, the response in the financial markets to the 50 basis point increase of alternative C could be sub- stantial.</t>
+  </si>
+  <si>
+    <t>Under alternative C, the federal funds rate would be boosted 1/2 percentage point, to 6-1/2 percent. Alternative C could be accomplished through an increase in the borrowing allowance to $275 million, while alternative A could be implemented by leaving the allowance for borrowing unchanged at $175 million in the face of seasonally elevated demand. (10) The fifty-basis-point firming of alternative C might be favored by the Committee if it wished to provide more assurance that pressures on resources would soon diminish, so as not to perpetuate the recently elevated rate of inflation and, over time, to return the economy toward a disinflationary path. (11) With markets apparently having concluded that rates are unlikely to rise significantly further, the response in the financial markets to the 50 basis point increase of alternative C could be sub- stantial. Nonetheless, M3 is projected to remain above the upper end of its current 0-to-4 percent annual range through September under alternative B, and even the tighter reserve market conditions of alternative C would not likely be adequate to bring M3 within its range by September.</t>
+  </si>
+  <si>
+    <t>Under the easier policy stance of alternative A, the intended federal funds rate would be reduced by 1/2 percentage point to 5-1/2 percent. (28) A reduction in the federal funds rate, perhaps of the 1/2 percentage point size embodied in alternative A, could be favored as a form of insurance against the downside risks in the economic outlook. (29) Immediate implementation of the 1/2 percentage point cut in the federal funds rate of alternative A would represent a considerably more aggressive policy action than currently is priced into financial markets.</t>
+  </si>
+  <si>
+    <t>Under alternative B, the intended federal funds rate would be maintained at 6 percent. (26) The decision to leave reserve market conditions un- changed, as under alternative B, might be favored if the staff economic forecast, which assumes a constant federal funds rate through early 1996, were viewed as both a reasonable and desirable outcome. (27) Over the past few days, markets have come to view policy action at this meeting as much less likely, and interest and exchange rates probably would change little with the choice of alternative B, -20- though a further small backup in yields cannot be ruled out with the disappointment of some residual expectations of prompt easing. That is, the financial market conditions associated with the unchanged policy of alternative B, including the backup in long-term rates in -21- the staff forecast, might be seen as unnecessarily risking weak spend- ing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> This alternative would be much larger and sooner than market participants currently expect. </t>
+  </si>
+  <si>
+    <t>(10) A further easing of policy, as under alternative A, could be supported if recent price and wage news were read as suggest- ing that the underlying determinants of inflation were more favorable than in the staff forecast. (11) The drop in the federal funds rate of 1/2 percentage point contemplated under alternative A would be much larger and sooner than market participants currently expect. For the year, M2 is expected to remain below the 5 percent upper bound of its annual range, even under alternative A.4 The projected softening in M3 owes primarily to lower growth in institutional money funds as their yields become better aligned with market rates.</t>
+  </si>
+  <si>
+    <t>Thus, the choice of the unchanged federal funds rate of alternative B should have little immediate impact on market interest rates. (9) Alternative B might be favored to the extent that the staff forecast were seen to be credible and the outcome to balance acceptably Committee concerns about expansion in output with those of the containment of inflation. Growth rates based on alternative B. (15) Growth rates of the broad monetary aggregates are ex- pected to continue to slow from their recent very rapid pace, but to remain relatively strong.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Alternative C would come as a surprise to market par- ticipants, and money market interest rates would rise at least 50 basis points</t>
+  </si>
+  <si>
+    <t>(12) The choice of the higher rates of alternative C would seem to rest on concerns about the longer-term inflation outlook. (13) Alternative C would come as a surprise to market par- ticipants, and money market interest rates would rise at least 50 basis points and the dollar would strengthen further on foreign ex- change markets.</t>
+  </si>
+  <si>
+    <t>(12) If the Committee saw reasonably high odds of more restrictive effects on the economy than the staff forecast, it might -10- favor an easing of the funds rate, as under alternative A.</t>
+  </si>
+  <si>
+    <t>(10) The case for keeping the funds rate at 5-3/4 percent as under alternative B could rest on an assessment that the current funds rate may well provide the appropriate monetary impulse, at least for the time being. Thus, choice by the Commit- tee of alternative B's unchanged funds rate likely would engender just a minor increase of short-term rates. Implied Sept. to1 1994-Q4 1995 December to 1995-Q4 Ranges M2 5.7 4.9 1 - 5 M3 6.0 6.7 2 - 6 M1 -1.6 -1.0 Total debt 4.0 5.2 3 - 7 Nonfederal 4.3 5.4 Note: Growth rates based on alternative B. 1. 4 Under alternative B, M2 is projected to grow at a 5-3/4 percent rate over the final three months of the year. M1 is expected to continue to decline over the remainder of the year, at about a 1-1/2 percent rate under alternative B, as still more banks introduce sweep accounts that transfer funds automatically from NOW accounts to MMDAs to reduce reserve requirements. Actual M1 over the four quarters of this year is now projected to edge down by 1 percent under alternative B. Alternative Levels and Growth Rates for Key Monetary Aggregates M2 Alt.</t>
+  </si>
+  <si>
+    <t>The 1/2 percentage point hike in the funds rate of alternative C would catch market participants off guard.</t>
+  </si>
+  <si>
+    <t>On the basis of relationships embodied in the Greenbook alternative simulation, a policy tightening of the dimensions of alternative C would nudge economic growth to below 2 percent over the next two years, opening up enough slack in labor and product markets to make more noticeable progress toward price stability in 1997 and beyond. (15) The 1/2 percentage point hike in the funds rate of alternative C would catch market participants off guard.</t>
+  </si>
+  <si>
+    <t>The cut in the federal funds rate of 50 basis points under alternative A would come sooner and be larger than now expected in the market.</t>
+  </si>
+  <si>
+    <t>(11) The choice of easing under alternative A might be favored if it were thought that some information about spending--for example, soft industrial commodity prices and a sluggish manufacturing sector or slowing growth of broad money and credit--was suggesting a weakening in aggregate demand not yet evident in more general statis- tics. -10- (12) The cut in the federal funds rate of 50 basis points under alternative A would come sooner and be larger than now expected in the market.</t>
+  </si>
+  <si>
+    <t>Despite the lack of a downward tilt to the inflation projection, the Committee still might favor the unchanged stance of policy in alternative B if it viewed the benefits of further disinflation as insufficient to justify a more restrictive policy stance that pushed the economy below its potential. The case for alternative B would be even stronger if the Committee viewed the staff inflation forecast as too pessimistic-- either because spending would be weaker or because the price-output relationship would be more favorable than the staff assessment. (10) Earlier expectations of the possibility of easing at the November FOMC meeting have largely been erased and, thus, the choice of alternative B should have little impact on market interest rates. -11- (15) The table below presents expected growth of money and debt under the unchanged reserve conditions of alternative B. The rebound in M2 growth, combined with still-brisk issuance of large time deposits to fund bank credit, would result in about 5-1/2 percent M3 growth under alternative B.</t>
+  </si>
+  <si>
+    <t>Alternative C would surprise market participants, who continue to hold the view, supported by statements from some Committee members, that the next policy move will be to ease.</t>
+  </si>
+  <si>
+    <t>(13) The choice of alternative C might be favored to the extent that the Committee wished to have greater assurance that infla- tion would continue to edge down. (14) A move to tighten policy by 50 basis points as under alternative C would especially surprise market participants, who con- tinue to hold the view, supported by statements from some Committee members, that the next policy move will be to ease.</t>
+  </si>
+  <si>
+    <t>Although market participants expect monetary policy to be eased over the next few months, a reduction of 50 basis points in the federal funds rate implemented at this meeting, as called for under alternative A, would be larger than generally expected.</t>
+  </si>
+  <si>
+    <t>(11) Although market participants expect monetary policy to be eased over the next few months, a reduction of 50 basis points in the federal funds rate implemented at this meeting, as called for under alternative A, would be larger than generally expected. (12) Under the staff forecast, alternative A would risk fostering greater inflation pressures, and the move would eventually need to be reversed.</t>
+  </si>
+  <si>
+    <t>(9) In these circumstances, adoption of the unchanged money market conditions of alternative B could prompt a small backup in market interest rates. Accordingly, in the staff forecast, alternative B keeps policy on a path that produces results for economic growth and inflation over 1996 closely in line with the Committee's expectations for next year that were reported in July. (15) The table below presents staff forecasts for money and credit growth for the November-to-March period under the unchanged money market conditions of alternative B.7 Broad measures of money 7. Expansion of M3 picks up to a 5-3/4 percent annual rate over the November-to-March period under alternative B. M2 growth also firms from its unexpectedly weak pace so far in the fourth quarter.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">With market participants expecting an easing rather than a tightening of policy, the 50-basis-point increase in the federal funds rate under alternative C would lead to a sharp jump in other money market interest rates. </t>
+  </si>
+  <si>
+    <t>-10- (13) With market participants expecting an easing rather than a tightening of policy, the 50-basis-point increase in the federal funds rate under alternative C would lead to a sharp jump in other money market interest rates. (14) The FOMC might select alternative C if it saw the risks to inflation at current interest rates as reasonably well balanced and wished to gain more assurance of making longer-term progress toward price stability. Given the demand and inflation relationships incorporated in the staff forecast, the rise in the federal funds rate under alternative C would tilt the inflation rate down slightly in 1997.</t>
+  </si>
+  <si>
+    <t>(25) Justification for a quarter-point reduction in the federal funds rate under alternative A would seem to rest on a belief that the economy is weaker than in the staff outlook, as might be inferred from the tone of some anecdotal reports and recent data, or that the prospects for disinflation are brighter. (26) Money market interest rates would fall by less than a quarter point under alternative A, given current expectations.</t>
+  </si>
+  <si>
+    <t>-18- Short-run Policy Alternatives (23) The unchanged funds rate of alternative B is consistent with the staff Greenbook forecast. Not only might alternative B be seen as attractive if the Committee concurred with this outlook and found the results acceptable, but it also might have appeal as a "wait and see" strategy because delays in data have curtailed the new infor- mation available to the Committee since it eased policy in December. Thus, rates could edge higher under alternative B.16 However, the extent of any rise in such rates likely would be tempered in the near term by the perception that the Committee had merely postponed easing pending the availabi- lity of more information. (28) The table below shows money and credit growth under alternative B for the January-to-June period.</t>
+  </si>
+  <si>
+    <t>(27) If the Committee agreed with the staff outlook for spending and inflation and wanted to make deliberate progress toward price stability, the choice of a quarter-point increase in the federal funds rate under alternative C might be favored.</t>
+  </si>
+  <si>
+    <t>it is difficult to gauge how market participants would react to the 1/2 percentage point of policy ease envisioned under alternative A.</t>
+  </si>
+  <si>
+    <t>(10) Given the staff's assessment of the economy, the 1/2 percentage point easing in reserve market conditions offered under alternative A would boost the economy marginally further beyond its potential and tilt the inflation rate up a bit more noticeably. With the latter outcome apparently inconsistent with the Committee's strategy for achieving its long-run goals, adopting alternative A would seem to require that, relative to the staff, Committee members expect somewhat weaker spending or better inflation. (11) In light of the uncertainty about the current economic situation and the widespread expectation that System policy is on hold, it is difficult to gauge how market participants would react to the 1/2 percentage point of policy ease envisioned under alternative A.</t>
+  </si>
+  <si>
+    <t>With market participants apparently expecting no policy action over the next few months, maintenance of current reserve condi- tions, as under alternative B, would elicit little reaction in credit markets.</t>
+  </si>
+  <si>
+    <t>(8) An unchanged policy stance, as in alternative B, would probably be preferred if the Committee concurred with the staff's as- sessment of the economy, viewed potential risks as about evenly balanced, and was willing to accept the possibility of a slight inten- sification of price pressures. (9) With market participants apparently expecting no policy action over the next few months, maintenance of current reserve condi- tions, as under alternative B, would elicit little reaction in credit markets.</t>
+  </si>
+  <si>
+    <t>The 50 basis point tightening of alternative C would catch market participants unawares and show through to instruments at the shortest maturities.</t>
+  </si>
+  <si>
+    <t>(12) A 1/2 percentage point tightening in reserve conditions, as under alternative C, might be favored if the Committee agreed with the staff forecast but viewed its outcome for inflation as undesir- able, particularly if the Committee wanted to make some progress to- ward price stability. (13) The 50 basis point tightening of alternative C would catch market participants unawares and show through to instruments at the shortest maturities.</t>
+  </si>
+  <si>
+    <t>Financial market partici- pants are anticipating that the FOMC will leave its policy stance unchanged at this meeting, implying that selection of alternative B would have little market impact.</t>
+  </si>
+  <si>
+    <t>In these circumstances, the Committee may prefer to adopt alternative B, 3. Financial market partici- pants are anticipating that the FOMC will leave its policy stance unchanged at this meeting, implying that selection of alternative B would have little market impact. (12) The interest rates of alternative B and associated staff forecast for the economy are thought to be consistent with a slight moderation in the growth of money and credit over coming months relative to their pace of expansion so far in 1996.</t>
+  </si>
+  <si>
+    <t>The Federal Reserve is not expected by market participants to tighten for several months, and hence, investors would be caught off guard</t>
+  </si>
+  <si>
+    <t>Alternative C embodies a 50 basis point increase in the federal funds rate to 5-3/4 percent in order to counter the incipient increase in price pressures. The Federal Reserve is not expected by market participants to tighten for several months, and hence, investors would be caught off guard by the FOMC's choice of alternative C at this meeting.</t>
+  </si>
+  <si>
+    <t>Under alternative B, federal funds would continue to trade around 5-1/4 percent. (23) The money and credit flows associated with a flat federal funds rate under alternative B were discussed in the previous sections of this document under the baseline case.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A 25 basis point rise in the federal funds rate at this meeting as under alternative C would exceed the small amount currently built into money market yields.</t>
+  </si>
+  <si>
+    <t>-18- (21) A 1/4 percentage point increase in the federal funds rate, as under alternative C, might be favored if the Committee wished to impose greater restraint on spending to reduce the odds of a gradual increase of inflation pressures. (22) A 25 basis point rise in the federal funds rate at this meeting as under alternative C would exceed the small amount currently built into money market yields. Money growth would be expected to slow somewhat more under alternative C, putting the broad aggregates on paths more likely to leave them below the upper ends of their longer-term ranges.</t>
+  </si>
+  <si>
+    <t>(8) Nonetheless, the Committee may well feel that it can afford to wait, as in alternative B, for additional data to accumulate to allow a more confident judgment concerning whether an underlying process of rising inflation seems to be taking hold.</t>
+  </si>
+  <si>
+    <t>Market participants would be somewhat surprised by a Committee decision to raise its intended federal funds rate by 25 basis points</t>
+  </si>
+  <si>
+    <t>(11) Given the recent adjustment to their expectations for monetary policy, market participants would be somewhat surprised by a Committee decision to raise its intended federal funds rate by 25 basis points, as under alternative C.</t>
+  </si>
+  <si>
+    <t>With market participants apparently placing greater than even odds on policy tightening at this meeting, interest rates would likely decline and the dollar weaken on foreign exchange markets if the unchanged policy of alternative B were adopted. Even before the discount rate story earlier this week, markets had built in close to 50/50 odds of a slight policy tightening, and alternative B probably would trigger rate declines that not only reversed the increases associated with the story, but some of those registered earlier in the intermeeting period as well</t>
+  </si>
+  <si>
+    <t>Nonetheless, there are reasons why the Committee might choose the unchanged federal funds rate of alternative B for the upcoming intermeeting period. (9) With market participants apparently placing greater than even odds on policy tightening at this meeting, interest rates would likely decline and the dollar weaken on foreign exchange markets if the unchanged policy of alternative B were adopted. Even before the discount rate story earlier this week, markets had built in close to 50/50 odds of a slight policy tightening, and alternative B probably would trigger rate declines that not only reversed the increases associated with the story, but some of those registered earlier in the intermeeting period as well. M2 is now expected to increase at a 4-1/2 percent rate this year and M3 at a 5-3/4 percent rate under alternative B, somewhat below the upper ends of their growth ranges for the year. Over the August-to-December period, the expansion of M2 is projected to pick up to about a 4-3/4 percent pace, broadly in line with GDP growth under alternative B.</t>
+  </si>
+  <si>
+    <t>(10) A tightening of policy at this Committee meeting, whether by 50 basis points, as assumed in alternative C, or by only 25 basis points, would improve the chances that price pressures would be contained and inflation outcomes would be consistent with the Commit- tee members' expectations in July.</t>
+  </si>
+  <si>
+    <t>This alternative would most likely be read as evidence that the Committee has serious reservations about the prospects for spending.</t>
+  </si>
+  <si>
+    <t>(10) A 50 basis point reduction in the federal funds rate, as under alternative A, might be favored if the Committee viewed the recent softness of final sales as likely to persist. A 50 basis point reduction in the funds rate, as under alternative A, would most likely be read as evidence that the Committee has serious reservations about the prospects for spending.</t>
+  </si>
+  <si>
+    <t>With market participants widely expecting policy to remain on hold for some time, the Committee's selection of alternative B should elicit little response in financial markets.</t>
+  </si>
+  <si>
+    <t>(6) If the Committee views the staff forecast as both likely and acceptable, it presumably would favor standing pat--alternative B. Even if the Committee found unacceptable the forecasted upcreep in core inflation (abstracting from technical CPI adjustments), it might want to wait for more evidence that such an outcome is in train before taking action. (7) With market participants widely expecting policy to remain on hold for some time, the Committee's selection of alternative B should elicit little response in financial markets. (13) In coming months, offering rates on M2 accounts are not expected to change much under alternative B, maintaining opportunity costs at around their recent levels. As a result, M1 is anticipated to decline at a 9 percent rate over the October-to-March period under alternative B; adjusted for sweeps, M1 would increase at a 3-3/4 percent rate over that span.</t>
+  </si>
+  <si>
+    <t>The choice of alternative C would come as a surprise to market participants.</t>
+  </si>
+  <si>
+    <t>(8) A policy tightening, such as the 50 basis point firming of the federal funds rate under alternative C, might be favored should the Committee wish to move promptly to counter the updrift in underlying inflation embedded in the staff outlook. (9) The choice of alternative C would come as a surprise to market participants.</t>
+  </si>
+  <si>
+    <t>the market is not expecting a change in policy, a 50 basis point funds rate reduction would show through completely to other short-term rates.</t>
+  </si>
+  <si>
+    <t>(12) A 50 basis point reduction in the federal funds rate (alternative A) would seem to require a judgment that the upward pressure on prices is less than in the staff forecast at current interest rate levels. (13) Because the market is not expecting a change in policy, a 50 basis point funds rate reduction, as in alternative A, would show through completely to other short-term rates.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">With market participants almost universally expecting policy to be on hold for a time, the Committee's selection of alternative B would prompt little response in financial markets. </t>
+  </si>
+  <si>
+    <t>In these circumstances, the Committee may wish to keep policy unchanged (alternative B), awaiting more information to assess how markets may evolve and how the other uncertainties may be resolved. (9) With market participants almost universally expecting policy to be on hold for a time, the Committee's selection of alternative B would prompt little response in -8- financial markets. (14) Under alternative B and the staff forecast, both debt and money should expand at moderate rates in coming months, in line with projected nominal GDP.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The choice of alternative C would surprise market participants and perhaps lead them to reconsider their view on the Federal Reserve's longer-term objectives.</t>
+  </si>
+  <si>
+    <t>(10) A 50 basis point firming of the funds rate (alternative C) might be favored if the Committee wished to move promptly to stem the rise in underlying inflation in the staff forecast and increase the odds on making some headway on its longer-run objective of price stability. (11) The choice of alternative C would surprise market participants and perhaps lead them to reconsider their view on the Federal Reserve's longer-term objectives.</t>
+  </si>
+  <si>
+    <t>Under alternative B, the federal funds rate would kept at 5-1/4 percent. (22) Financial markets currently are not anticipating a change in policy at the February meeting, and thus the choice of alternative B should initially have little impact on interest rates or the foreign exchange value of the dollar. (25) Growth of the broad monetary aggregates is expected to slow under alternative B from the very rapid pace of late 1996.</t>
+  </si>
+  <si>
+    <t>The tightening of policy under alternative C would surprise market participants, and short-term interest rates, including the prime rate, would rise by the half-point hike in the federal funds rate.</t>
+  </si>
+  <si>
+    <t>Under alternative C, the federal funds rate would be raised by 1/2 percentage point to 5-3/4 percent, either through a less generous provision of nonborrowed reserves or a hike in the discount rate. While inflation does not deteriorate appreciably in the near term, given the lags in the effect of policy, the sooner the Committee begins to tighten--as under alternative C--the lower the odds that higher inflation will become embedded in price and wage setting. (24) The tightening of policy under alternative C would surprise market participants, and short-term interest rates, including the prime rate, would rise by the half-point hike in the federal funds rate.</t>
+  </si>
+  <si>
+    <t>With market participants apparently placing high odds on a 25 basis point tightening in the federal funds rate at the March meeting, interest rates probably would fall somewhat if the unchanged policy of alternative B were adopted.</t>
+  </si>
+  <si>
+    <t>(7) Nonetheless, a number of considerations regarding the outlook might induce the Committee to forgo tightening at the March meeting, as under alternative B. (8) With market participants apparently placing high odds on a 25 basis point tightening in the federal funds rate at the March meeting, interest rates probably would fall somewhat if the unchanged policy of alternative B were adopted. (12) Under alternative B and the staff forecast, debt is expected to continue to grow around its recent pace in the months ahead, while money growth tends to moderate as the expansion of nominal GDP slows. (13) M2 growth from February to June under alternative B is projected to slow to a 4-1/2 percent rate, reflecting the deceleration in nominal GDP.</t>
+  </si>
+  <si>
+    <t>(9) The Committee might choose to increase the federal funds rate, perhaps by the 50 basis points of alternative C, in order to lean against the likely buildup of inflation pressures.</t>
+  </si>
+  <si>
+    <t>(8) Despite the staffs perception that underlying inflation pressures will be building, the Committee may find reasons to leave its policy stance unchanged, at least for the time being, as incorporated in alternative B, which keeps the intended federal funds rate at 5-1/2 percent. However, in recent weeks, markets appear to have removed all but modest odds of any action, and the choice of alternative B should trigger a relatively minor decline in rates. - 11 - (14) The runoff of the tax-related deposit surge of April should be completed in May, after which the monthly growth of M2 and M3 under alternative B is expected to stabilize at annual rates of 4-1/2 and 6 percent, respectively, through September--somewhat below the pace of the first five months of the year.</t>
+  </si>
+  <si>
+    <t>Rise in the federal funds rate under alternative C would come as a major surprise to financial market participants</t>
+  </si>
+  <si>
+    <t>(11) The 1/2 percentage point rise in the federal funds rate under alternative C would come as a major surprise to financial market participants and likely would spark a considerable rise in interest rates and the exchange value of the dollar.</t>
+  </si>
+  <si>
+    <t>No change in the stance of monetary policy at this FOMC meeting is built into the structure of market interest rates, so financial market prices would react little to the Committee's choice of alternative B.</t>
+  </si>
+  <si>
+    <t>Under alternative B, the intended federal funds rate would be maintained at its current 5-1/2 percent level. (34) The Committee may favor the unchanged federal funds rate of alternative B if it thinks that chances are that the staff has not gone far enough to incorporate a more favorable tradeoff between resource use and inflation into the outlook. No change in the stance of monetary policy at this FOMC meeting is built into the structure of market interest rates, so financial market prices would react little to the Committee's choice of alternative B. (37) The staffs projections of money and debt growth this year, assuming main- tenance of the unchanged federal funds rate of alternative B, were described in the previous section.</t>
+  </si>
+  <si>
+    <t>Under alternative C, it would be raised 1/4 percentage point to 5-3/4 percent. (35) The 1/4 percentage-point increase in the federal funds rate embodied in alternative C might seem appropriate if the Committee sees the likelihood of intensifying inflation pressures, as in the Greenbook, and wishes to impart some resistance to the anticipated acceleration of prices. (36) The 25 basis point firming in alternative C would catch market participants off guard, inducing an immediate selloff in securities markets and an appreciation of the dollar in exchange markets, with short-term interest rates jumping by virtually the same amount as the intended funds rate. Maintenance of the slightly higher short-term interest rates of alternative C would lower these growth rates only slightly over this year.</t>
+  </si>
+  <si>
+    <t>Market participants uniformly do not expect a near-term policy move by the Federal Reserve, and selection of alternative B by the Committee should elicit little imme- diate market reaction.</t>
+  </si>
+  <si>
+    <t>Under alternative B, the intended federal funds rate would be kept at its current level of 5-1/2 percent. (8) Market participants uniformly do not expect a near-term policy move by the Federal Reserve, and selection of alternative B by the Committee should elicit little imme- diate market reaction. (11) Under the unchanged federal funds rate of alternative B, M2 is projected to grow at a moderate 4-1/2 percent rate on average over the remaining months of the year, around the expected rate of expansion of nominal GDP, leaving this aggregate a little below the upper limit of its 1 to 5 percent growth range for the year.</t>
+  </si>
+  <si>
+    <t>Under alternative C, it would be boosted to 5-3/4 percent, either through reduced provision of nonborrowed reserves or a hike in the discount rate. If the Committee wants more insurance against the possibility that inflation will begin to pick up, and especially if it wishes to tilt the odds a little in the direction of further progress toward price stability over coming years, it may wish to raise the intended federal funds rate at this meeting, perhaps by the 25 basis points of alternative C. (10) With no near-term tightening expected, the market response to implementation of alternative C could be sharp.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Virtually no one in the market anticipates action at this meeting, so that yields across the term structure are not likely to budge much and the dollar should continue to trade around its current level on foreign exchange markets immediately following the adoption of the unchanged policy stance of alternative B. </t>
+  </si>
+  <si>
+    <t>(6) The staff assessment of the pressures on resources implies that policy restraint is in order at some point to check an upcreep in inflation, but the Committee may, nonetheless, prefer to hold the federal funds rate at its current level of 5-1/2 percent at this meeting, as in alternative B. (8) Virtually no one in the market anticipates action at this meeting, so that yields across the term structure are not likely to budge much and the dollar should continue to trade around its current level on foreign exchange markets immediately following the adoption of the unchanged policy stance of alternative B. Treasury bill rates have been depressed of late by low issuance, and the turnaround in bill sales in the fourth quarter prompted by the seasonal bulge in the federal deficit may roll back some of the decline in rates on those securities. - 10- (10) Under the unchanged policy stance of alternative B, the growth of the monetary aggregates should slow significantly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Committee's choice of alternative C at this meeting would catch market participants completely unawares. </t>
+  </si>
+  <si>
+    <t>(7) If the Committee were confident that the staff had correctly identified the threat that inflation would pick up, or wanted some greater assurance of further progress toward price stability, it would likely favor raising the federal funds rate promptly, perhaps at this meeting by the 25 basis points of alternative C. (9) The Committee's choice of alternative C at this meeting would catch market participants completely unawares. Under alternative C, even though opportunity costs would likely rise with the imposition of monetary restraint, M2 might be bolstered to some extent in the near term should a correction in the stock and bond markets induce investors to favor money market over bond and stock mutual funds.</t>
+  </si>
+  <si>
+    <t>(10) Alternative B, which would leave the intended federal funds rate at 5-1/2 percent, could be chosen at this meeting either merely as a deferral of a tighter stance until financial markets have become more resilient, or, more positively, as a justifiable policy posture, absent some change in the tenor of incoming information about inflation prospects. (12) The staff anticipates that, under alternative B, M2 and M3 will grow at annual rates of 4-1/2 and 6-1/4 percent, respectively, over the five months from October to March of next year.</t>
+  </si>
+  <si>
+    <t>(9) If the Committee shares the staffs assessment that the U.S. economy has overshot its sustainable productive potential, it may be disposed to tighten its policy stance, as in the 25 basis point rise in the funds rate in alternative C.</t>
+  </si>
+  <si>
+    <t>(13) The 25 basis point easing of Alternative A might be favored if the Committee were concerned that turmoil abroad might have an even greater impact on the U.S. economy than the staff has built into the forecast.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The markets expect no policy action over the next few months and would react little, if at all, to the choice of alternative B</t>
+  </si>
+  <si>
+    <t>Even if the Committee is concerned about the pressures on labor resources and finds the eventual uptrend in underlying -9- inflation unacceptable, it may be willing to keep the funds rate constant at this meeting, as under Alternative B. Under alternative B, the Committee would be buying time to assess the extent to which developments abroad restrain aggregate demand, depress oil prices, and support the dollar, as well as the degree to which recent momentum in the economy might be sustained. (10) The markets expect no policy action over the next few months and would react little, if at all, to the choice of alternative B. Apart from year-end effects, interest rates-- especially Treasury yields--should fluctuate close to recent lows over the intermeeting period. M2 growth is projected at around a 4 percent annual pace over the November-to-March period under alternative B, leaving this aggregate near the upper end of its provisional 1998 range.</t>
+  </si>
+  <si>
+    <t>(11) The 25 basis point tightening of Alternative C might be favored if the Committee wanted to lean against the inflationary bias that may well be inherent in the current and prospective tautness of labor markets.</t>
+  </si>
+  <si>
+    <t>sufficient chances of a shortfall in activity from the staff forecast to suggest a small easing at this time-</t>
+  </si>
+  <si>
+    <t>The dollar would be expected to trade around its levels of late, off some from its recent peak (23) The Committee may see sufficient chances of a shortfall in activity from the staff forecast to suggest a small easing at this time--as in the 25 basis point decline in the federal funds rate under alternative A.</t>
+  </si>
+  <si>
+    <t>The staff forecast is built on an unchanged federal funds rate, and if the Committee agrees that this is both a reasonable and desirable outcome under those conditions, retaining the current stance of policy under alternative B would be appropriate.</t>
+  </si>
+  <si>
     <t>?</t>
-  </si>
-  <si>
-    <t>Alternative C also would catch market participants un- aware</t>
-  </si>
-  <si>
-    <t>(28) Alternative C also would catch market participants un- awares, and short-term interest rates likely would adjust upward rather sharply.</t>
-  </si>
-  <si>
-    <t>(10) The 1/2 percentage point drop in the funds rate con- templated under alternative A is larger than the easing of policy currently anticipated in the markets; thus, short-term rates are likely to move down under this alternative--but not by as much as the cut in the funds rate--with the three-month bill rate drifting to near 5 percent. (13) The easing of monetary policy under alternative A would boost M2 to a 4-1/2 percent annual rate of expansion in September and the pace would firm further in the fourth quarter, lifting growth of this aggregate for the year to around 3 percent.</t>
-  </si>
-  <si>
-    <t>Under alternative B, federal funds would continue to trade around 5-1/2 percent, at the discount rate, in association with adjustment plus seasonal borrowing of $375 million. With reserve market pressures unchanged, as under alternative B, rates might firm a touch. The dollar likely would trade around current levels under alternative B, but could firm a notch if U.S. interest rates were to back up. (11) Under alternative B, M2 would be expected to increase over the balance of the quarter.</t>
-  </si>
-  <si>
-    <t>7 Under alternative A, federal funds would tend to trade around 4-3/4 percent, which could be fostered either by lowering the borrowing specification by $50 million to $275 million or by lowering the discount rate by a further 1/2 point to 4-1/2 percent. The latter approach to alternative A would preserve the present spread of the funds rate over the discount rate and thus the current degree of cushioning of transitory shocks to the supply and demand for reserves. (9) The size and timing of the 1/2 percentage point drop in the federal funds rate of alternative A would tend to catch financial markets unawares, inducing almost as large a drop in other short-term interest rates. (15) The 1/2 percentage point decline in the federal funds rate under alternative A would promote faster money growth than under alternative B, improving the odds that the aggregates would end up in the ranges. This reasoning yields projected M2 growth over the next three months under alternative A of 4 percent at an annual rate.</t>
-  </si>
-  <si>
-    <t>Under alternative B, the federal funds rate would be expected to remain centered on 5-1/4 percent, in as- sociation with an initial specification for adjustment plus seasonal borrowing of $325 million. Nonetheless, the unchanged federal funds rate associ- ated with alternative B is unlikely to engender a marked backup in yields in financial markets over the intermeeting period, so long as incoming nonfinancial and monetary data are mixed, as would be the case under the staff's forecast. B Growth from September to December M2 4 3 M3 2 1-1/2 M1 8-1/2 6-1/2 Implied growth from 1990:Q4 to December M2 2-3/4 2-1/2 M3 1 1 Ml 7-1/2 7 (12) Under the unchanged interest rates of alternative B, M2 growth is projected to pick up to a 3 percent rate over the last three months of the year, leaving this aggregate at the lower bound of its Alternative Levels and Growth Rates for Key Monetary Aggregates M2 M3 M1 Alt. (13) Under alternative B, growth in M3 from September to December is expected to strengthen to a 1-1/2 percent annual rate. (15) The 1/2 percentage point decline in the federal funds rate under alternative A would promote faster money growth than under alternative B, improving the odds that the aggregates would end up in the ranges.</t>
-  </si>
-  <si>
-    <t>3 Under alternative A, the federal funds rate would move down to 4-1/2 percent, achieved either through a 1/2 percentage point cut in the discount rate with the same level of bor- rowing as under alternative B or through open market operations that lowered the borrowing level to $125 million. (12) The easing contemplated in alternative A exceeds that now envisioned by the markets and thus money market interest rates would decline, perhaps by at least 1/4 percentage point. -11- (13) M2 is projected to strengthen to a 4 percent rate by December under alternative A and would be entering the new year well into its tentative range. (14) Under alternative A, M3 would expand at a 1-1/4 percent rate in November and December, on a trajectory to begin the new year within its tentative range.</t>
-  </si>
-  <si>
-    <t>Under alternative B, federal funds would continue to trade around 5 percent in combination with adjustment plus seasonal borrowing of $175 million. 3 Under alternative A, the federal funds rate would move down to 4-1/2 percent, achieved either through a 1/2 percentage point cut in the discount rate with the same level of bor- rowing as under alternative B or through open market operations that lowered the borrowing level to $125 million. B Growth from September to December M2 3-1/2 3 M3 1-1/4 1 M1 10 9 Implied growth from 1990:Q4 to December M2 2-3/4 2-1/2 M3 1 1 M1 7-3/4 7-1/2 (9) The markets appear to have built in a high probability of a further easing move in the period just ahead, and thus with the unchanged funds rate of alternative B, other market interest rates may tend to firm. A M J J A S O N D J I 11400 11200 11000 10800 10600 10400 10200 19921991 (10) M2 would be expected to continue to expand at a 3 per- cent rate in the November and December period under alternative B, the same as expected at the October FOMC meeting. (11) M3 under alternative B is seen as continuing to grow at a 1 percent annual rate over November and December, which would mean this aggregate would be entering next year around the bottom of its tentative 1992 range of 1 to 5 percent.</t>
-  </si>
-  <si>
-    <t>Although the former variant of alternative A, which involves funds trading 1/2 percentage point below the discount rate, would be technically possible, it likely would be associated with somewhat greater day-to-day volatility in the funds rate. (12) Under alternative A, the 1/2 percentage point fall in the funds rate to 4 percent would foster a smaller drop in other short-term interest rates, given the expectations of near-term policy easing al- ready incorporated in current market quotes. Unless data were clear-cut in pointing to continuing weakness in the economy, the half-point easing of alternative A--closely following the quarter-point decline in the funds rate last week--would be seen as signalling a priority on encouraging a strong recovery. Even under the lower short-term inter- est rates associated with alternative A, these aggregates probably would remain noticeably below the midpoints of their ranges. (17) The lower short-term interest rates associated with alternative A would put M2 on a path that would carry it toward the middle portion of its range later in 1992. From November to March, M2 is projected to turn in a 3-3/4 percent growth rate under alternative A. While deposit rates will be reduced further--perhaps appreciably at some institutions, if lower market rates jolt them into reassessing long-standing rates on NOW accounts and passbook savings--they are not likely to drop enough to -14- eliminate the additional stimulus to money growth of the lower interest rates in alternative A. The faster M2 growth under alternative A will show through to M3, though in muted form, since bank and thrift credit growth will accelerate by less than M2 in the short run.</t>
-  </si>
-  <si>
-    <t>Under alternative B, the federal funds rate would continue to center around 4-1/2 percent, in association with the allowance for ad- justment plus seasonal borrowing staying at $75 million. (11) Under the unchanged federal funds rate of alternative B, interest rates may exhibit an initial tendency to firm a little, as market expectations of another modest policy easing in the near term are disappointed. Under alternative B, both M2 and M3 are projected to be only somewhat above the lower edges of their tenta- tive 1992 target cones in March. (15) Under alternative B, both M2 and M3 are projected to grow a little more slowly than their average rates over October and November.</t>
-  </si>
-  <si>
-    <t>10 Under alternative A, the federal funds rate would decline to the 3-1/2 percent area in association with a reduction of the borrowing allowance to $50 million. M2 would remain in the lower half of its provisional 1992 range through March under both alternatives, but under alternative A would be on a trajectory to move up in its range over the second quarter. (24) Short-term interest rates would fall by nearly the 50 basis point decline in the federal funds rate under alternative A. 12 Under the easier conditions of alternative A, M2 would be expected to be expanding at a percentage point faster pace in March and into the next quarter; all of the added growth in M2 would occur in M1, other liquid deposits, and M2 money funds.</t>
-  </si>
-  <si>
-    <t>Under alternative B, federal funds would con- tinue to trade around 4 percent, with adjustment plus seasonal borrowing averaging around $100 million. B Growth from December to March M2 3-1/2 3 M3 1-3/4 1-1/2 Ml 15-1/2 14-1/2 Growth from 1991Q4 to March M2 3-1/2 3-1/4 M3 2 1-3/4 M1 14-1/2 13-3/4 (23) The markets appear to have built in no policy moves in the period just ahead and thus unchanged reserve market conditions under alternative B should have no effect on interest rates. 8.5% 4.5% O N D J F MA M J J A SO ND J F MA M J J A S ON D 1990 1991 1992 12400 12200 12000 11800 11600 11400 11200 11000 10800 10600 -22- (25) Even with a pickup over February and March, M2 would expand at only a 3 percent annual rate over the December-to-March period under alternative B, below the pace over the last three months of 1991. (26) M3, under alternative B, would expand at only a 2 per- cent annual rate over February and March, after even slower growth in December and January.</t>
-  </si>
-  <si>
-    <t>This alternative might cause a market reassessment of the intentions of the Federal Reserve, leading to a significant downward revision in the expected course of short-term interest rates for the next year or so</t>
-  </si>
-  <si>
-    <t>Under alternative A, the federal funds rate would decline to the 3-1/2 percent area in conjunction with a reduction in the initial borrowing allowance to $75 million. In this context, the unexpected easing of money market conditions of alternative A might cause a market reassessment of the intentions of the Federal Reserve, leading to a significant downward revision in the expected course of short-term interest rates for the next year or so. (15) Under the lower interest rates of alternative A, M2 is expected to grow at a 4-1/2 percent rate over the March-to-June period, keeping this aggregate around the midpoint of its 1992 target range.</t>
-  </si>
-  <si>
-    <t>Under alternative B, federal funds would continue to trade around 4 percent in association with an initial bor- rowing allowance of $100 million. (9) Markets appear to anticipate no change in policy over the intermeeting period, and thus interest rates should remain close to current levels under alternative B. Nevertheless, there could be a downward bias to rate movements over coming months. Under the unchanged reserve conditions of alternative B, M2 growth is projected to moderate to a 3-1/2 percent rate from March to June. (13) As a consequence of rising opportunity costs and waning effects of special factors, M2 velocity is projected to increase sig- nificantly in the second quarter--at about a 2 percent annual rate under alternative B. (14) Growth in M3 under alternative B would moderate slightly to a 1-1/2 percent pace over the March-to-June period.</t>
-  </si>
-  <si>
-    <t>5 In contrast, the funds rate would return to 4-1/2 percent and the initial borrowing allowance would increase to $125 million under alternative C. (11) The tightening of policy under alternative C would lead to about a 50 basis point rise in money market rates, which likely would be passed through fully to the prime rate. (16) M2 growth would slacken to a 2-1/2 percent rate over the March-to-June period under alternative C, bringing this aggregate ap- preciably below the midpoint of its annual range.</t>
-  </si>
-  <si>
-    <t>4 Under alternative A, the federal funds rate would drop to 3-1/4 percent. (10) The extent of the easing of reserve market conditions under alternative A would catch market participants unawares, and the 1/2 point drop in the federal funds rate would induce a nearly compar- able decline in other money market interest rates. However, following an easing move, especially of the dimensions of alternative A, investors would become more assured of sustained economic expansion, but also less confident of any longer-term decrease in inflation, which together would limit any reductions in long-term rates. If the lower funds rate of alternative A is maintained through year-end, growth of M2 for the year could be expected to come in around 4 percent.</t>
-  </si>
-  <si>
-    <t>Under alternative B, federal funds would continue trading in the 3-3/4 percent area; extending the current assumption of $100 million for adjustment plus seasonal borrowing would be expected to preserve the current 1/4 percentage point spread of the funds rate above the discount rate, at least over the first part of the intermeeting period. The same federal funds rate could be achieved by cutting the discount rate 1/2 percentage point to 3 percent and specifying borrowing at the alternative B level of $100 million. Consequently, prices in domestic credit and foreign exchange markets probably would not show much reaction should the Committee main- tain current reserve market conditions by choosing alternative B at this meeting. C Growth from March to June M2 1-1/4 1 3/4 M3 1/4 0 -1/4 M1 9-3/4 9-1/4 8-3/4 Growth from April to June M2 3 2-1/2 2 M3 2 1-3/4 1-1/2 M1 12 11-1/4 10-1/2 (13) Growth of M2 is projected to average 2-1/2 percent at an annual rate over May and June with the essentially stable money market interest rates of alternative B. 990 970 950 930 910 890 ,-' Chart 4 DEBT Billions of dollars - - Actual Level * Projected Level -- 1 12300 -I 12100 -- 11900 .5 1 11700 4.5% -4 11500 - 11300 11100 i I I I I I I I I I I I I I O N D J F M A M J J A S O N D 1991 1992 10900 -13- (14) Under alternative B, the projected turnaround in M2 over May and June should show through to M3, which is expected to register an annual growth rate of 1-3/4 percent; from March to June, M3 would be about unchanged. While growth of M3 for the year of 2 percent is expected under the constant funds rate of alternative B, this projec- tion would have to be shaded up or down by perhaps 1/4 point if alterna- tive A or C were chosen at this FOMC meeting and sustained for the rest of the year. This alternative would stress the Committee's expectation of a resump- tion of growth in broad money over May and June, in contrast to the traditional three-month specification, which would show little if any monetary growth (for example, 1 percent for M2 and zero for M3 under alternative B).</t>
-  </si>
-  <si>
-    <t>Under the policy tightening of alternative C, the federal funds rate would rise to 4-1/4 percent, in association with higher initial borrowing of $125 million. (11) The more restrictive policy of alternative C would come as a considerable surprise to market participants. -14- If alternative C is adopted and the higher rates maintained, a 3 percent annual pace for M2 would be more likely.</t>
-  </si>
-  <si>
-    <t>Under the easier alternative A, the funds rate would be reduced to 3-1/4 percent, placing it 1/4 percentage point below the discount rate, in association with a borrowing assumption of $200 million. -17- (22) Under alternative A, most of the drop of 50 basis points in the funds rate would be transmitted to other money market interest rates. Even under alternative A, M2 would be on a trajectory that would bring it closer to, though still a bit below, its lower bound in the fourth quarter, and M3 also would be expected to remain somewhat below its current range through year-end.</t>
-  </si>
-  <si>
-    <t>Under alternative B, the federal funds rate would continue to center on 3-3/4 percent. Thus, in the near-term, rates would rise somewhat under alternative B. C Growth from June to September M2 2-3/4 2 1-1/4 M3 1 1/2 0 M1 8 6-1/2 5 Growth from QIV'91 to September M2 2 1-3/4 1-1/2 M3 1/4 0 0 M1 11 10-1/2 10 (25) While M2 under all three alternatives appears likely to resume growth over the June-to-September period, under alternative B this aggregate still is projected to grow at only a 2 percent annual rate. (26) The turnaround in M2 growth under alternative B should show through to M3.</t>
-  </si>
-  <si>
-    <t>Under alternative C, the funds rate would be raised to around 4-1/4 percent by selecting a borrowing specification of $250 million. (23) The increase of 50 basis points in the funds rate under alternative C would come as a considerable surprise to market partici- pants.</t>
-  </si>
-  <si>
-    <t>(8) Under alternative A, short-term interest rates would fall by nearly the full 50 basis point drop in the federal funds rate, espe- cially were the easing to take the form of a discount rate cut, which 3. For the June-to-September period, expansion in the broad aggregates is likely to fall well short of the rates envisioned at the time of the last Committee meeting, even if alternative A is adopted. (14) The lower interest rates of alternative A would be expected to buoy money growth over the balance of the year.</t>
-  </si>
-  <si>
-    <t>Under alternative B, federal funds would continue to trade around 3-1/4 percent in combination with an initial allowance for adjustment plus seasonal borrowing of $250 million. Although money market interest rates might firm a bit over the intermeeting period under the unchanged policy of alternative B, any increase would be limited if, consistent with the Greenbook forecast, information continued to suggest modest economic expansion. The dollar, under alternative B, would be expected to trade around its recent lower levels. (12) Under alternative B, M2 is expected to resume expanding this month and to grow at a 2-1/4 percent pace on balance over the remainder of the year. This projec- tion assumes the unchanged federal funds rate of alternative B ex- tended through year-end and the Greenbook economic forecast. (13) The firming in M2 under alternative B shows through in part to M3, which bottoms out in coming months and then edges higher.</t>
-  </si>
-  <si>
-    <t>Alternative C involves a return of the federal funds rate to 3-3/4 percent and a borrowing allowance of $275 million. (9) A reversal of the July easing would take market partici- pants completely by surprise and short-term interest rates would rise by at least 1/2 percentage point under alternative C. Bond rates, too, would retrace some of their recent declines under this alternative, at least initially, and quality spreads on private debt could widen if such a tightening were seen as placing the recovery at risk. (15) Under alternative C, M2 and M3 would drop further below their annual ranges, as opportunity costs widen, banks become even more cautious lenders, and income growth is more restrained.</t>
-  </si>
-  <si>
-    <t>4 Under the easier policy stance of alternative A, the expected federal funds rate would be cut to 2-1/2 percent. With a 1/2 percentage point drop in the dis- count rate, for example, an initial borrowing assumption of $200 million would be retained under alternative A. (9) Projected growth rates of the monetary aggregates under the two policy alternatives appear on the table below. (14) The immediate 1/2 percentage point drop in the federal funds rate under alternative A would exceed the market's expected change. (15) Under alternative A, M2 and M3 likely would grow at rates of 2-3/4 and 1-1/4 percent over the September-to-December interval. In addition to the limited stimulus to M2 demands arising from the reduction in oppor- tunity costs, spending by then should have begun to respond to the -13- monetary policy easing embodied in alternative A. Real interest rates would be lower than under alternative B, though actual declines in real rates may be limited by a continued ebbing of inflation expec- tations.</t>
-  </si>
-  <si>
-    <t>Under alternative B, federal funds would continue to trade around 3 percent, in association with an initial assumption for adjustment plus seasonal borrowing of $200 million. Under these circumstances, selection of the unchanged reserve conditions of alternative B would initially induce some backup in interest rates across the maturity spectrum and some rise in the ex- change value of the dollar. (11) Under alternative B, M2 is projected to grow at a 2 percent rate from September to December, somewhat slower than in the last two months. (12) Under alternative B, the staff foresees M3 growth of 1 percent from September to December, also somewhat slower than over August and September. In addition to the limited stimulus to M2 demands arising from the reduction in oppor- tunity costs, spending by then should have begun to respond to the -13- monetary policy easing embodied in alternative A. Real interest rates would be lower than under alternative B, though actual declines in real rates may be limited by a continued ebbing of inflation expec- tations.</t>
-  </si>
-  <si>
-    <t>6 The policy ease envisaged under alternative A would trim the expected federal funds rate to 2-1/2 percent. Technically, though, the lower federal funds rate of alternative A could be achieved by reducing the borrowing assumption $25 million with an unchanged discount rate. (20) Against a backdrop of public readings that suggested some firming in economic activity, market participants would be sur- prised by the 1/2 point decline in the funds rate under alternative A. -17- Most short-term interest rates would match the decrease in the federal funds rate. (21) While the impetus to the monetary aggregates imparted by choosing alternative A would be barely discernible in 1992, the lower market interest rates embodied in that choice would push up both M2 and M3 to the lower end of their current tentative ranges for 1993 by March.</t>
-  </si>
-  <si>
-    <t>Under alternative B, the trading range for the federal funds rate would remain centered at 3 percent, in conjunction with an initial assumption for adjustment plus seasonal borrowing of $75 mil- lion. Thus, market par- ticipants would be unlikely to react to the unchanged reserve conditions of alternative B, especially if incoming data conform to the Greenbook assessment of moderately expanding real activity in the fourth quarter. (17) Under alternative B, the growth of M2 is projected to slow somewhat from its pace of the last two months.</t>
-  </si>
-  <si>
-    <t>Alternative A incor- porates a 1/2 percentage point reduction in the federal funds rate. (8) The 1/2 percentage point decline in the federal funds rate under alternative A would be passed through fully to other short-term interest rates. (13) The lower interest rates of alternative A would boost M2 growth well into 1993, putting this aggregate near the lower end of the current provisional range by March.</t>
-  </si>
-  <si>
-    <t>Under alternative B, federal funds would continue to trade around 3 percent, in association with the allowance for adjustment and seasonal borrowing remaining at $50 million. With an unchanged federal funds rate under alternative B, other private short-term rates will decline over the intermeeting period as remaining year-end pressures unwind. M1 is projected to grow at a 5-3/4 percent pace from November to March under alternative B. Much of the higher money growth over coming months relative to alternative B would reflect stronger expansion of M1. With issuance of managed liabilities weak, growth in M3 would be boosted only slightly as compared with alternative B, and that aggregate would remain below its provisional target range in March.</t>
-  </si>
-  <si>
-    <t>The 1/2 percentage point increase in the federal funds rate of alternative C could be implemented by raising the borrowing allowance by $25 million. (9) Although many market participants have come to the view that monetary policy easing has run its course for the current economic cycle, none appears to expect a tightening to be implemented in the near term, as in alternative C. Consequently, short-term Treasury rates would jump by the full 50 basis point increase in the federal funds rate. (14) M2 is projected to expand at only a 1 percent rate from November-to-March under alternative C and M3 would decline at a 1/4 percent rate.</t>
-  </si>
-  <si>
-    <t>6 Under alternative A, the federal funds rate would drop to 2-1/2 percent; this could be achieved either through a reduction in the borrowing allowance to $25 million or by a half per- centage point cut in the discount rate with unchanged borrowing. (22) Short-term interest rates--including the prime rate-- would decline by the half-point drop in the federal funds rate under alternative A. Availability constraints on business credit at banks might ease more noticeably should bankers come to see lower rates as improving the outlook for business profitability and lessening strains in this sector. (27) Under alternative A, growth in M2 would pick up to a 1 percent annual rate over February and March, returning this aggregate to its fourth-quarter 1992 level in March. A buildup of institution-only money funds, as holders responded to more attractive rate relationships, would buoy M3 over February and March -21- under alternative A, and hold down the net declines in this aggregate over these two months.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The markets appear to have built in an unchanged policy in the period just ahead </t>
-  </si>
-  <si>
-    <t>Under alternative B, the allowance for adjustment and seasonal borrowing would be retained at $50 million, in association with trading in federal funds continuing to be centered around 3 percent. (21) The markets appear to have built in an unchanged policy in the period just ahead and thus interest rates would be expected to remain near current levels under alternative B. Longer-term rates might come under a little downward pressure if, consistent with the staff greenbook forecast, news on prices continues to be good, and economic indicators point to a little less momentum in the economic expansion than in the second half of last year. The dollar would fluctuate around current levels under alternative B, moving up on any news of unexpected eco- nomic weakness or policy easing abroad, or down should the news about the U.S. economy prove to be softer than expected. C Growth from December to March M2 -1/2 -1 -1-1/2 M3 -2-1/4 -2-1/2 -2-3/4 M1 4-1/2 3-1/2 2-1/2 Growth from 1992Q4 to March M2 -1/4 -1/2 -1 M3 -2-1/4 -2-1/4 -2-1/2 M1 6-1/4 5-1/2 4-3/4 (25) Under alternative B, M2 would be about flat on average over February and March.</t>
-  </si>
-  <si>
-    <t>though market participants seem to believe that some tightening of monetary policy over the next year will be forthcoming, they do not see this happening soon and thus would be surprised by the election of alternative C.</t>
-  </si>
-  <si>
-    <t>Federal funds would trade around 3-1/2 percent under alternative C in combination with a $25 million boost to the borrowing allowance. (23) Although market participants seem to believe that some tightening of monetary policy over the next year will be forthcoming, they do not see this happening soon and thus would be surprised by the election of alternative C. Short-term rates would rise by about 1/2 percentage point. (28) Under alternative C, M2 would decline over February and March as larger opportunity costs act as an additional drag on this aggregate.</t>
-  </si>
-  <si>
-    <t>Under alternative A, the federal funds rate would decline to the 2-1/2 percent area. (9) The easing of policy under alternative A would surprise market participants and would lead to a decline in short-term rates, including the prime rate, commensurate with the 1/2 percentage point drop in the federal funds rate. (14) Under alternative A, M2 would strengthen to a 3 percent rate over the February-to-June period. M3 would grow at a 1-1/4 percent pace over February to June under alternative A, but would remain below its fourth-quarter base even by June.</t>
-  </si>
-  <si>
-    <t>Under alternative B, federal funds would continue to trade around 3 percent in association with the allowance for adjustment plus seasonal borrowing initially remaining at $50 million. This alternative could be implemented through a 1/2 percentage point drop in the discount rate, holding the initial borrowing allowance at the same level as in alternative B, or by lowering the initial borrowing allowance to $25 million and leaving the discount rate unchanged. Thus, under alternative B, short-term interest rates would stay around current levels. The dollar would be expected to fluctuate around current levels under alternative B, but could firm somewhat if rate declines in Europe prove to be faster and larger than now expected. C Growth from February to June M2 3 2-1/2 2 M3 1-1/4 1 3/4 M1 11 9-3/4 8-1/2 Implied growth from 1992:Q4 to June M2 3/4 1/2 1/4 M3 -1 -1 -1-1/4 M1 9 8-1/4 7-1/2 (12) Under alternative B, M2 is expected to resume growth over the February-to-June period.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conversely, the tightening of policy under alternative C, which also would come as a surprise to market participants, would induce a rise in short-term rates comparable to the hike in the federal funds rate. </t>
-  </si>
-  <si>
-    <t>Alternative C, involving a rise in the federal funds rate to 3-1/2 percent, could be implemented through a boost in the initial borrowing allowance to $75 million. Conversely, the tightening of policy under alternative C, which also would come as a surprise to market participants, would induce a rise in short-term rates comparable to the hike in the federal funds rate. Under alternative C, M2 would expand at a 2 percent rate over the February-to- June period, as wider opportunity costs would discourage inflows to more liquid deposits, especially M1 balances.</t>
-  </si>
-  <si>
-    <t>5 Under alternative A, the federal funds rate would be reduced to 2-1/2 percent. exchange markets probably would remain around current levels under alternative B. (10) The 1/2 percentage point reduction in the federal funds rate under alternative A would surprise market participants and should show through almost completely to other short-term interest rates. (16) The lower interest rates of alternative A would be ex- pected to provide some added lift to growth of the monetary aggregates.</t>
-  </si>
-  <si>
-    <t>Thus, market interest rates are unlikely to react to the implementation of alternative B.</t>
-  </si>
-  <si>
-    <t>Under alternative B, federal funds would continue to trade around 3 percent, in association with the allowance for adjustment and seasonal borrowing initially being maintained at its current level of $100 million. Thus, market interest rates are unlikely to react to the implementation of alternative B. exchange markets probably would remain around current levels under alternative B. (10) The 1/2 percentage point reduction in the federal funds rate under alternative A would surprise market participants and should show through almost completely to other short-term interest rates. ,oO----"" Ã‚Â¡ * Ã‚Â¡Ã‚Â¡ oÃ‚Â¡Ã‚Â¡" Ã‚Â¡_x005F_x001A_ Ã‚Â¡Ã‚Â¡Ã‚Â¡" .... %..................................................................... 0% ON D J F M A M J JASO N D J 1250 1200 1150 1100 1050 1000 950 1993 1994 Chart 7 DEBT Billions of Dollars 13000 - Actual Level * Projected Level - 12800 Monthly 4.5% 12600 12400 12200 -112000 -- 11800 --111600 -1 11400 I I I I I I I I I I I I I I I I 111200 O N D J F M A M J J A S O N D J 1993 1994 -11- (13) Under alternative B, M2 is projected to increase at about a 5-3/4 percent average rate over May and June, a considerable pickup from recent months. (14) M3 under alternative B is seen as accelerating to about a 4 percent rate over May and June. Looking further ahead, moderate average growth of M3 during the third quarter would be expected to accompany retention of the specifications of alternative B over that period. Given still-favorable conditions in longer-term markets under alternative B, issuance of corporate bonds and stocks should remain relatively heavy.</t>
-  </si>
-  <si>
-    <t>Market participants also would be surprised by the policy tightening under alternative C at this FOMC meeting.</t>
-  </si>
-  <si>
-    <t>Federal funds would trade in the neighborhood of 3-1/2 percent under alternative C, in association with an initial borrowing allowance of $125 million. (11) Market participants also would be surprised by the policy tightening under alternative C at this FOMC meeting. (17) Under alternative C, the higher money market interest rates and opportunity costs would restrain the monetary aggregates. Maintenance of the money market conditions of alternative C probably would induce M3 to contract on the year.</t>
-  </si>
-  <si>
-    <t>Under alternative A, the funds rate would be reduced to the area of 2-1/2 percent, either by choosing a $225 million borrowing allowance or by cutting the discount rate 1/2 percentage point, to 2-1/2 percent, while retaining a $250 million borrowing allowance. (27) The easing of reserve conditions embodied in alternative A would represent an unexpected direction for policy, especially in light of the market's understanding of the Committee's recent policy predilection. C Growth from June to September M2 1-1/2 1 1/2 M3 1/2 1/4 0 M1 6-3/4 5-3/4 4-3/4 Implied growth from Q4:1992 to September M2 1-1/4 1 3/4 M3 0 0 -1/4 M1 8-3/4 8-1/2 8-1/4 (29) Projected M2 growth over the third quarter diverges rela- tively little across the three alternatives, ranging from 1/2 percentage point under alternative C to 1-1/2 percentage point under alternative A. Given this damped interest rate response, even if the money market conditions of alternative A continued through year- end, M2 growth over the year would still be only 1-1/4 percent, notice- ably below the 2 percent lower bound of the Committee's current annual range. Ã¢Ë†Å¾ Ã¢Ë†Å¾ ' Chart5 M1 - Actual Level * Short-Run Alternatives Billions of Dollars 15% 10%10% -I 1100 0 0 0 5% i --11050 ON D J F MA M J J A S O N D J 1992 1993 1994 1000 1200 1150 Chart 6 DEBT Billions of Dollars - Actual Level - - Estimated Level * Projected Level ON D J 1992 I I I I I I I I I- I I 11400 F M A M J J A S N D J 1993 1994 13000 12800 12600 12400 12200 12000 11800 11600 -22- alternative C to 6-3/4 percent under alternative A.</t>
-  </si>
-  <si>
-    <t>Consequently, market interest rates would not respond initially to the implementation of alternative B</t>
-  </si>
-  <si>
-    <t>Under alternative B, federal funds would remain in a trading range around 3 percent, in association with an initial allowance for adjustment plus seasonal borrowing of $250 million, an increase of $50 million from the current allowance to accommodate the normal pattern in seasonal borrowing at this time of the year. Consequently, market interest rates would not respond initially to the implementation of alternative B. Rates would tend to remain near current levels or edge lower over subsequent weeks should data on economic activity and prices prove to be about in line with the staff projection and should the Congress continue to make progress on passage of a deficit reduction package. Total reserves and the monetary base are projected to grow from June to September at 5-3/4 and 8-1/4 percent rates, respectively, under alternative B. -23- Directive Language (32) Presented below are draft paragraphs relating to the ranges for 1993 and 1994.</t>
-  </si>
-  <si>
-    <t>The immediate tightening of reserve market conditions under alternative C is not built into financial market quotes and would induce a rise in short-term market interest rates that about matched the 1/2 percentage</t>
-  </si>
-  <si>
-    <t>Under alternative C, which could be imple- mented through a $275 million borrowing allowance, the funds rate would vary around 3-1/2 percent. (26) The immediate tightening of reserve market conditions under alternative C is not built into financial market quotes and would induce a rise in short-term market interest rates that about matched the 1/2 percentage point increase in the federal funds rate. C Growth from June to September M2 1-1/2 1 1/2 M3 1/2 1/4 0 M1 6-3/4 5-3/4 4-3/4 Implied growth from Q4:1992 to September M2 1-1/4 1 3/4 M3 0 0 -1/4 M1 8-3/4 8-1/2 8-1/4 (29) Projected M2 growth over the third quarter diverges rela- tively little across the three alternatives, ranging from 1/2 percentage point under alternative C to 1-1/2 percentage point under alternative A. Ã‚Â° Ã‚Â° ' Chart5 M1 - Actual Level * Short-Run Alternatives Billions of Dollars 15% 10%10% -I 1100 0 0 0 5% i --11050 ON D J F MA M J J A S O N D J 1992 1993 1994 1000 1200 1150 Chart 6 DEBT Billions of Dollars - Actual Level - - Estimated Level * Projected Level ON D J 1992 I I I I I I I I I- I I 11400 F M A M J J A S N D J 1993 1994 13000 12800 12600 12400 12200 12000 11800 11600 -22- alternative C to 6-3/4 percent under alternative A.</t>
-  </si>
-  <si>
-    <t>5 Under alternative A, the federal funds rate would decline to 2-1/2 percent, either through a drop in the borrowing allowance to $225 million or a cut in the discount rate of 50 basis points in combination with an unchanged level of borrowing. (11) The easing under alternative A would come as a surprise to market participants, and short-term rates would decline by the full 50 basis point drop in the funds rate. (12) In light of the likelihood of some decline in an array of real interest rates, as well as the real foreign exchange value of the dollar, alternative A might be favored if economic growth in the staff forecast were seen to be unsatisfactory and the Committee were willing to accept little or no further disinflation. Faster growth in M2 under alternative A owes both to more growth in nominal income later in the year than under alternative B and to the improvement in the attrac- tiveness of assets in M2 relative to money market instruments. M3 under alternative A would expand slowly over the final four months of the year as bank credit growth remained damped in the context of continued heavy financing in the securities markets.</t>
-  </si>
-  <si>
-    <t>Under alternative B, federal funds would continue to trade around 3 percent in association with an allowance for adjustment plus seasonal borrowing of $250 million. Thus, under alternative B, short-term interest rates should remain around current levels in the weeks ahead. (8) The interest rates under alternative B are consistent with those of the staff Greenbook forecast, which has the federal funds rate around current levels through 1994 and long-term rates edging lower. (9) Over the balance of 1993, M2 is projected to grow at about a 1-1/2 percent pace under alternative B, and, as shown in the table below, to finish the year around the lower bound of its new annual range. 7 M3 under alternative B is projected to bottom out in August and to edge higher over the remainder of the year. The lower interest rates of this alternative would tend to boost money growth relative to alternative B and, under the spending propensities incorporated in the staff forecast, would give a little more assurance that the broad aggregates would finish the year at or above the lower bounds of their ranges for 1993. Faster growth in M2 under alternative A owes both to more growth in nominal income later in the year than under alternative B and to the improvement in the attrac- tiveness of assets in M2 relative to money market instruments.</t>
-  </si>
-  <si>
-    <t>The tightening of policy under alternative C would come much sooner than is now envisioned by market participants.</t>
-  </si>
-  <si>
-    <t>Under alternative C, the federal funds rate would rise to 3-1/2 percent accompanying a boost in adjustment plus seasonal borrowing to $275 mil- lion. (13) The tightening of policy under alternative C would come much sooner than is now envisioned by market participants. (14) Alternative C might be favored if the Committee saw a need to move sooner, rather than later, to contain or reduce future inflationary pressures. With the staff's outlook for spending propensities, M2 would expand at only a 1 percent pace over the final five months of this year under alternative C, ending the year about 3/4 percent above its fourth- quarter 1992 level.</t>
-  </si>
-  <si>
-    <t>(10) Under alternative A, money market interest rates would drop by the full 50 basis point decline in the federal funds rate. Alternative A might also be chosen if the Committee saw economic activity and inflation as possibly coming in below the staff forecast; market perceptions that the Committee was signalling an expectation that the outlook for real activity had deteriorated and for disinflation had improved could result in sub- stantial declines in bond yields.</t>
-  </si>
-  <si>
-    <t>Market participants apparently believe that the federal funds rate will remain at 3 percent</t>
-  </si>
-  <si>
-    <t>Under alternative B, federal funds would continue to trade around 3 percent in combination with an initial allowance for adjustment plus seasonal borrowing of $250 million. (7) Alternative B is consistent with the staff's economic forecast. Market participants apparently believe that the federal funds rate will remain at 3 percent, at least for the next several months, and under alternative B, money market interest rates would remain around current levels. (9) As shown in the table below, M2 under alternative B is projected to grow at a 2 percent average rate over the final four months of this year. Under alternative B, M3 would grow at a 3/4 percent rate over the remainder of this year, leaving this aggregate just above both its fourth-quarter 1992 level and the bottom of its 8. These growth rates would place both aggregates near the bottom of their annual ranges for this year, and on a lower trajectory going into 1994 than under alternative B, partly reflecting damped income growth.</t>
-  </si>
-  <si>
-    <t>Under alternative C, the federal funds rate would rise to 3-1/2 percent in association with a boost in the initial borrowing allowance. (12) Under alternative C, interest rates would rise and the dollar would strengthen on foreign exchange markets. (13) Alternative C might be favored if the modest degree of price deceleration in the staff forecast were viewed to be unsatis- factory.</t>
-  </si>
-  <si>
-    <t>This alternative may surprise market participants.</t>
-  </si>
-  <si>
-    <t>(12) Alternative A contemplates an easing in reserve market pressures and a decline in the federal funds rate to 2-1/2 percent. 13 Implementation of alternative A would be especially surprising to market participants, given their view that underlying economic growth is strengthening. (13) Alternative A might be viewed as appropriate if the Com- mittee wished to make appreciable progress in reducing remaining slack in the economy, in contrast to the plateau for the unemployment rate seen in the staff forecast.</t>
-  </si>
-  <si>
-    <t>Under alternative B, the federal funds rate would continue to trade around 3 percent. C Growth from October to December M2 2-1/2 2 1-1/2 M3 1-1/4 1 1 M1 11-1/2 10-1/2 9-1/2 Growth from October to March 1994 M2 3 2-1/2 2 M3 1-3/4 1-1/2 1-1/4 M1 11-1/4 10-1/2 9-1/2 (9) As shown in the lower panel of the above table, M2 under alternative B is projected to grow at a 2-1/2 percent rate over October to March.</t>
-  </si>
-  <si>
-    <t>(10) Under Alternative C, the federal funds rate would rise 1/2 percentage point to 3-1/2 percent. (11) The Committee might favor alternative C if strength in recent economic data were seen as implying that any delay in firming ran an unacceptably high risk that economic activity could develop excessive momentum that would rapidly erode the remaining degree of slack and produce an acceleration of prices.</t>
-  </si>
-  <si>
-    <t>In the case of alternative A, the federal funds rate would decline to 2-1/2 percent and borrowing would fall, perhaps to $25 million. (13) The easing of policy under alternative A would come as a surprise to market participants, and short-term interest rates would fall by about the 50 basis point drop in the federal funds rate. Under alternative A, M2 would expand at a 2-1/4 percent pace, close to that evident since midyear, buoyed partly by less of a slowdown in M1 than under alternatives B and C, M3 would grow at a 1-1/4 percent pace from November to March. (14) Alternative A might be favored if the current strength in the economy were seen as likely to give way to a significant weak- ening in the pace of expansion next year, considering the greater fiscal restraint in train and the backup in long-term interest rates and the dollar since mid-October.</t>
-  </si>
-  <si>
-    <t>Under alternative B, federal funds would continue to trade around 3 percent in association with adjustment plus seasonal borrowing at the discount window of $50 million. (7) Alternative B is consistent with the policy assumptions underlying the staff economic forecast. Nonetheless, market interest rates are unlikely to move down much on balance under the steady funds rate of alternative B in coming months, since the market would continue to expect a tightening before long. The foreign exchange value of the dollar under alternative B should stay around current levels. M2 by March would have expanded at a 2 per- cent annual rate from its fourth-quarter 1993 base under alternative B, placing this aggregate well above the lower end of its provisional 1 to 5 percent growth range for next year. (10) Under alternative B, M3 would advance at a 1 percent annual rate over the November-to-March period; by March this aggregate would be 1-1/4 percent above its fourth-quarter 1993 base, well within its 0 to 4 percent provisional range for 1994.</t>
-  </si>
-  <si>
-    <t>The rise in the federal funds rate under alternative C, to 3-1/2 percent, would come sooner than now anticipated by market participants and built into markets interest rates.</t>
-  </si>
-  <si>
-    <t>Under alternative C, the federal funds rate would move up to 3-1/2 percent and the borrow- ing allowance to $75 million. (11) The rise in the federal funds rate under alternative C, to 3-1/2 percent, would come sooner than now anticipated by market participants and built into markets interest rates. M3 would expand under alternative C at only a 3/4 percent pace over the November-to- March period. (12) Alternative C might be preferred if there were concerns about the inflation outlook.</t>
-  </si>
-  <si>
-    <t>Alternative A embodies a downward adjustment of the federal funds rate to 2-1/2 percent and of the borrowing allowance to $25 million. (27) The easing of policy under alternative A would come as more of a surprise to market participants.</t>
-  </si>
-  <si>
-    <t>Market participants now anticipate continuation of the money market conditions implied by alternative B over the near term, and FOMC choice of this alternative would not engender any immediate reaction in security markets.</t>
-  </si>
-  <si>
-    <t>Alternative B involves a continuation of feder- al funds trading around 3 percent and of adjustment plus seasonal borrowing averaging initially about $50 million. (25) Market participants now anticipate continuation of the money market conditions implied by alternative B over the near term, and FOMC choice of this alternative would not engender any immediate reaction in security markets. C Growth from January to June M2 2-1/4 2 1-3/4 M3 1-1/2 1-1/4 1 M1 7-1/2 6-3/4 6 Growth from 1993:Q4 to June M2 2-1/4 2 1-3/4 M3 1-3/4 1-1/2 1-1/4 M1 7-1/4 6-3/4 6-1/4 (29) M2 growth likely will be held down under alternative B by a reversal of the previous bulge attributable to mortgage refinanc- ing activity, which had boosted average M2 growth by an estimated 1 percentage point during the October through December months, before becoming a minor drag in January. With demand deposits most affected by mortgage refinancing activity, M1 growth from January to June will be depressed by around 4 percentage points by this special factor under alternative B. Growth of M1 is projected at 6-3/4 percent over this period, implying growth of total reserves and the monetary base of 4-3/4 and 9-1/2 percent, respectively. (30) M3 is projected to expand at a 1-1/4 percent rate from January to June under alternative B.</t>
-  </si>
-  <si>
-    <t>The firming in the stance of policy under alternative C would come sooner than now built into market quotes</t>
-  </si>
-  <si>
-    <t>(26) The firming in the stance of policy under alternative C would come sooner than now built into market quotes and would be re- flected in increases in short-term rates nearly equal to the 50 basis 12.</t>
-  </si>
-  <si>
-    <t>With market participants expecting appreciable increases in the federal funds rate in coming months, including 25 basis points at the March FOMC meeting, interest rates could tend to drift lower under the unchanged reserve conditions of alternative B</t>
-  </si>
-  <si>
-    <t>Under alternative B, federal funds would continue to trade around 3-1/4 percent in association with ad- justment plus seasonal borrowing of $75 million. (9) With market participants expecting appreciable increases in the federal funds rate in coming months, including 25 basis points at the March FOMC meeting, interest rates could tend to drift lower under the unchanged reserve conditions of alternative B. Rate de- clines would be quite small initially if market participants still believed that the next tightening step was imminent but had merely been delayed, perhaps by the unsettled market conditions of late. (10) Alternative B might be favored if most of the increase in intermediate- and long-term real rates over recent months were thought likely to persist and be sufficient to restrain demand and 8. Even if long-term rates were expected to decline appreci- ably, alternative B might be selected were the economy nevertheless seen as remaining below its long-term potential and inflation pres- sures contained. C Growth from February to June M2 2-1/2 2-1/4 M3 1-1/2 1-1/4 Ml 6 5-1/4 Implied growth from 1993:Q4 to June M2 2 1-3/4 M3 1/2 1/4 M1 6 5-3/4 (16) Growth in M2 would average 2-1/2 percent at an annual rate over the February-to-June period under alternative B, up from only 3/4 percent over January and February, even as growth in nominal income continues to slow. Nonetheless, M2 velocity would con- tinue to rise in the second quarter under alternative B, but its 2-3/4 percent annual pace of expansion would be well below that of the two previous quarters. Under alternative B, this aggregate would expand at a 1-1/2 percent pace over the February-to-June period.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Alternative C involves a larger immediate tightening than now built into the structure of market rates.</t>
-  </si>
-  <si>
-    <t>(11) Alternative C involves a larger immediate tightening than now built into the structure of market rates. (12) In addition to possibly contributing to more settled market conditions, alternative C might be preferred if the Committee saw significant risks of greater inflation going forward. Under alternative C, M2 would grow at a 2-1/4 percent rate over the February-to-June period, restrained by weaker inflows to liquid components as opportunity costs widen more. Still, by June, M2 would have grown at a 1-3/4 percent rate from its fourth-quarter 1993 base under alternative C, above the lower end of its 1994 annual range. Under alternative C, M3 would pick up by less, expanding at a 1-1/4 percent rate over February to June, restrained by some further outflows from M3-type money market funds. By June, M3 would stand 1/4 percent at an annual rate above its fourth-quarter base under alternative C, only a little above the lower end of its annual growth cone.</t>
-  </si>
-  <si>
-    <t>Under alternative B. federal funds would continue to trade around 3-3/4 percent, in association with the al- lowance for adjustment plus seasonal borrowing remaining initially at $175 million. (14) The case for standing pat, alternative B, is a more extreme version of the rationale for alternative C: In this case, the market assessment, and even that of the staff, of the strength of aggregate demand would be judged to be seriously off the mark, perhaps because the rise in long-term rates, along with the decline in house- hold wealth, will have a more significant restraining influence on aggregate demand. Choice of alternative B would come as a consider- able surprise--and disappointment--to financial markets; very short- term interest rates would be likely to fall appreciably, but this alternative risks a significant sell-off in the bond market before weakness in aggregate demand becomes apparent.</t>
-  </si>
-  <si>
-    <t>5 Under alternative C, the federal funds rate would move up 1/4 percentage point (one-half the usual adjustment shown in previous bluebooks for "alternative C") to 4 percent, effectuated by increasing the initial borrowing allowance to $200 million. (13) The case for increasing the intended federal funds rate only 25 basis points as under alternative C would seem to hinge on the judgment that financial market participants have exaggerated the like- ly strength of future spending relative to the economy's potential and hence of prospective inflation pressures. (14) The case for standing pat, alternative B, is a more extreme version of the rationale for alternative C: In this case, the market assessment, and even that of the staff, of the strength of aggregate demand would be judged to be seriously off the mark, perhaps because the rise in long-term rates, along with the decline in house- hold wealth, will have a more significant restraining influence on aggregate demand.</t>
-  </si>
-  <si>
-    <t>Under alternative D, the federal funds rate would be raised to 4-1/4 per- cent, either by increasing the initial borrowing allowance to $225 million or by raising the discount rate to 3-1/2 percent, while keep- ing the initial allowance for discount window borrowing at $175 mil- lion. Very short-term rates might thus increase slightly under alternative D. The behavior of rates on instruments of a few months' maturity or longer would depend importantly on whether the market interpreted the larger increase of alternative D as indicating a steeper trajectory of future policy actions, and perhaps the need for greater cumulative tightening. Bond yields could still back up somewhat in the aftermath of an announce- ment of the Federal Reserve's choice of alternative D, but these other influences should limit any increase and work to reduce yields over time. The recent increases in opportunity costs on liquid retail deposits aris- ing from the previous tightenings in the stance of monetary policy, and under alternative D from an additional firming move as well, will serve to hold back growth of M1 and some of the other components of M2 and M3.</t>
-  </si>
-  <si>
-    <t>Alternative B might be chosen by the Committee if it wished to await confirmation of the strength of aggregate demand, perhaps because there were questions about whether that strength would in fact be forthcoming. Accordingly, short-term interest rates are likely to move down a little after the meeting under alternative B. Long-term rates are not likely to decline, however, under this alternative; the dollar 15. M1 is expected to increase at only a 3-1/2 percent rate from June to September under alternative B.17 (32) Expansion of M3 is projected to pick up only slightly in the next few months.</t>
-  </si>
-  <si>
-    <t>15 The federal funds rate would be boosted 1/4 percentage point to 4-1/2 percent under alternative C, and the borrow- ing allowance would be raised to $350 million. (28) The Committee could see alternative C as appropriate if it believed that sufficient evidence had accumulated to warrant a continued gradual tightening of policy to prevent the economy from overheating.</t>
-  </si>
-  <si>
-    <t>Alternative D would increase the federal funds rate 1/2 percentage point to 4-3/4 percent. (29) Concerns that the recent behavior of the dollar and commodity prices might imply rising prices more broadly and might be associated with a ratcheting up of inflation expectations could moti- vate the Committee to select alternative D.</t>
-  </si>
-  <si>
-    <t>Under alternative B, federal funds would continue to trade around 4-1/4 percent in association with re- taining the $450 million allowance for adjustment plus seasonal bor- rowing. (8) Alternative B might be preferred if it were thought that there would be less strength in the economy than in the staff fore- cast. In these circumstances, the choice of no change in the stance of policy under alternative B would result in some decline in short-term interest rates, and the dollar might tend to weaken on foreign exchange markets. The path for alternative B -10- is based on the assumption of no change in the federal funds rate for the rest of this year. D Growth from July to December M2 1-1/2 1 M3 3/4 1/2 M1 3 2-1/4 Implied growth 93Q4 to 94Q4 M2 1-1/2 1-1/4 M3 1/2 1/2 M1 4 3-1/2 (15) M2 would grow at a 1-1/2 percent rate over the July-to- December period under alternative B, down from the July pace but quicker than that over the first six months of the year. Moreover, with short-term rates unchanged under alternative B, insti- tution-only money funds should be stable after large runoffs through the spring. M1 would expand at about a 3 percent rate over the July-to- December period under alternative B. Continued rapid currency growth would account for this expansion, as higher opportunity costs reached earlier this year and slow mortgage refinancing activity hold transaction deposits about flat.</t>
-  </si>
-  <si>
-    <t>As noted above, alternative C is about what is built into the structure of market interest rates, and neither interest nor exchange rates are likely to react very strongly to such an actio</t>
-  </si>
-  <si>
-    <t>8 Under alternative C, the federal funds rate would be raised to 4-1/2 percent and the initial borrowing allowance to $475 million. (11) Alternative C embodies a move of 25 basis points. As noted above, alternative C is about what is built into the structure of market interest rates, and neither interest nor exchange rates are likely to react very strongly to such an action. In this regard, the 50 basis points of alternative D would imply more assurance of this outcome than alternative C and, therefore, would be more likely to be followed by a period of stability of short-term rates. 9 (Money growth under the reserve conditions of alternative C would lie half way between alternatives B and D.) Alt.</t>
-  </si>
-  <si>
-    <t>Under alternative D, the funds rate would be moved to 4-3/4 percent, either through an increase in the initial borrowing allowance to $500 million or a hike in the discount rate to 4 percent and un- changed adjustment plus seasonal borrowing. (12) The more forceful move of alternative D might be chosen if the Committee viewed the economic situation as highly likely to require substantial additional monetary tightening, for example, of the scope embodied in the steep tilt to the yield curve over the next few years. In this regard, the 50 basis points of alternative D would imply more assurance of this outcome than alternative C and, therefore, would be more likely to be followed by a period of stability of short-term rates. Alternative D assumes a 50 basis point increase in the funds rate at this meeting and no change thereafter. Although these money growth rates are roughly the same as those projected for alternative D, the higher year-end level of rates assumed in the Greenbook implies slower growth of money and income in the first half of 1995 than would alternative D. Alternative Levels and Growth Rates for Key Monetary Aggregates M2 Alt. (16) Under alternative D, M2 would grow at a 1 percent rate over the July-to-December period.</t>
-  </si>
-  <si>
-    <t>Nonetheless, maintenance of existing reserve conditions under alternative B might elicit little reaction in rates beyond the very shortest maturities because market participants would assume that tightening had simply been postponed.</t>
-  </si>
-  <si>
-    <t>Under alternative B, the federal funds rate would continue to trade around 4-3/4 percent, consistent with retaining an allowance of $475 million for adjustment plus sea- sonal borrowing. (8) Alternative B, which would retain current reserve condi- tions, is not inconsistent with the staff assumption of policy firm- ing, provided that firming resumes some time soon. Nonetheless, maintenance of existing reserve conditions under alternative B might elicit little reaction in rates beyond the very shortest maturities because market participants would assume that tightening had simply been postponed. For illustrative purposes, the path under alternative B was derived assuming that the funds rate would hold at its current level for the remainder of the year. D Growth from September to December M2 1-1/2 1/2 M3 1-1/4 3/4 M1 2-1/2 1-1/2 Implied growth from 93:Q4 to 94:Q4 M2 1-1/4 1 M3 3/4 3/4 M1 3-1/4 3 (14) Over the September-to-December period, M2 would expand at a 1-1/2 percent rate under alternative B. As a result, under alternative B, the monetary base should expand at about a 8-1/4 percent rate, while total reserves should grow at a 1-3/4 percent rate over the September-to-December period.</t>
-  </si>
-  <si>
-    <t>Alternative C is consistent with the current structure of market rates, and this policy action might well trigger only muted interest rate reactions.</t>
-  </si>
-  <si>
-    <t>5 Alternative C envisages raising the federal funds rate 1/4 percentage point, to 5 percent, in conjunction with an increase in the borrowing allowance to $500 million. If the Committee were uncertain about how much tightening would be required but wanted to respond to recent data, the more modest 25 basis point move of alternative C might be considered appropriate. (11) The 25 basis point tightening of alternative C is con- sistent with the current structure of market rates, and this policy action might well trigger only muted interest rate reactions. How- ever, since most market participants expect either no action or a 50 basis point tightening, alternative C could raise questions about System intentions, potentially unsettling markets. (The response of the aggregates under alternative C would lie midway between the two alternatives.)</t>
-  </si>
-  <si>
-    <t>The 50 basis point firming of alternative D is the most likely of the three policy options to keep the Federal Reserve "ahead of the curve" of inflation pressures and consequently to limit the extent to which policy might later need to tighten. A considerable portion of the 50 basis point increase in the federal funds rate under alternative D would pass through to other short-term rates. The path for the aggregates under alternative D assumes that the funds rate moves up to 5-1/4 percent at this meeting and stays there for the balance of the year. (15) Under alternative D, M2 would grow at a 1/2 percent rate over the September-to-December period. M3 would grow at a 3/4 percent rate over the remaining months of the year, pulled down by a runoff of institu- tion-only money funds as their yields lag behind the increase in money market rates that would be in train under alternative D. 6.</t>
-  </si>
-  <si>
-    <t>Alternative B would keep the intended federal funds rate unchanged at 4-3/4 percent, in association with retaining an allowance of $225 million for adjustment plus sea- sonal borrowing at the discount window. (9) Choice of the unchanged policy of alternative B might be based on the judgments that most of the effects of previous increases in interest rates are still in the pipeline, that convincing signs of higher inflation have not yet appeared, and that under these circum- stances the Committee can await evidence indicating whether the effects of previous monetary tightening will be sufficient to restrain spending adequately. 5 (More detailed data appear on the table and charts on the following pages.) Under alternative B, offering rates through the first quarter would continue to adjust upward in the face of steady money market rates. M1 is projected to decline at a 1 percent rate from October to March under alternative B, as currency flows abroad remain robust but demand and other checkable deposits continue to decline. Rapid issuance of large time deposits will continue to fill some of the gap left by still-sluggish retail deposits, and thus M3 is projected to outpace M2 from October to March, likely expanding at a 2-1/2 percent rate under alternative B. Alt. C Growth from October to March M2 1 0 M3 2-1/2 2 M1 -1 -2 Implied growth from 1994:Q4 to March M2 1-1/2 1/2 M3 2-1/2 2-1/4 M1 0 -1-1/4 (16) Under the 50 basis point increase in the funds rate of alternative C, both M2 and M3 would record slower growth over the next five months than under alternative B.</t>
-  </si>
-  <si>
-    <t>With market participants generally appearing to have built in a move of at least this size, interest rates could exhibit little initial reaction to the implementation of alternative C</t>
-  </si>
-  <si>
-    <t>4 Alternative C embodies a 50 basis point increase in the federal funds rate to 5-1/4 percent, accomplished either by an equal rise in the discount rate to 4-1/2 percent with the borrowing allowance kept at $225 million or by an increase in the borrowing allowance to $275 million at the current discount rate of 4 percent. A still larger increase in the federal funds rate than envisioned under alternative C is also discussed. (12) With market participants generally appearing to have built in a move of at least this size, interest rates could exhibit little initial reaction to the implementation of alternative C. C Growth from October to March M2 1 0 M3 2-1/2 2 M1 -1 -2 Implied growth from 1994:Q4 to March M2 1-1/2 1/2 M3 2-1/2 2-1/4 M1 0 -1-1/4 (16) Under the 50 basis point increase in the funds rate of alternative C, both M2 and M3 would record slower growth over the next five months than under alternative B.</t>
-  </si>
-  <si>
-    <t>Alternative B would keep the intended federal funds rate at 5-1/2 percent. In these circumstances, and given the seemingly greater confidence of late in financial markets that the System will act as appropriate to counter a buildup in inflationary pressures, interest rates and the foreign exchange value of the dollar are unlikely to change very much in the immediate aftermath of a deci- sion to leave policy unchanged, as under Alternative B. Movements in financial markets subsequently will depend, of course, on the nature of incoming data. C M2 1-1/4 1/2 M3 2-1/4 2 M1 -1 -2 (15) Under alternative B, M2 would strengthen to a 1-1/4 percent rate over the November-to-March period. M2 would expand at only a 1/2 percent rate over the Novem- ber-to-March period, restrained by faster runoffs of M1 and savings deposits (including MMDAs) than under alternative B.</t>
-  </si>
-  <si>
-    <t>Alternative C entails a 50 basis point rise in the federal funds rate, to 6 percent, achieved either through an equivalent increase in the discount rate with the same path for the borrowing allowance or an increase in the initial borrowing allowance to $175 million, with the same seasonal reductions thereafter. (11) The 1/2 percentage point rise in the federal funds rate under alternative C might be favored if the Committee viewed the recent string of surprisingly strong economic data as clearly indicat- ing that the risks are still tilted in the direction of sustained faster inflation. The inclination to adopt alternative C would be bolstered by a belief that financial markets have largely absorbed the Orange County shock and the risks of further disruptions are de minimus. (12) Under alternative C, money market interest rates would firm somewhat, especially those at the shortest end, as the tightening would come somewhat sooner than now expected. The staff expects the growth of the monetary aggregates to remain damped over coming months, restrained by prior (and under alternative C, current) increases in opportunity costs. (16) Under alternative C, opportunity costs would tend to increase as the rise in money market rates outpaced those on M2 com- ponents.</t>
-  </si>
-  <si>
-    <t>While market participants currently anticipate a 50 basis point increase in the federal funds rate at this meeting, their response to the Committee's selection of alternative B would depend on how the decision were interpreted.</t>
-  </si>
-  <si>
-    <t>Under alternative B, federal funds would continue to trade around 5-1/2 percent, in association with keeping the allowance for adjustment plus seasonal borrowing at $75 million. (26) Choice of alternative B might be viewed as appropriate if the Committee desired additional readings on the extent of the economy's forward momentum and of underlying inflationary pressures to provide a firmer basis for judging whether incremental restraint will be required to damp aggregate demand sufficiently. (27) While market participants currently anticipate a 50 basis point increase in the federal funds rate at this meeting, their response to the Committee's selection of alternative B would depend on how the decision were interpreted. C Growth from January to June M2 2-1/4 1-1/2 M3 2-1/2 2 M1 1 -1/4 Growth from 1994:Q4 to June M2 2-1/2 2 M3 3 2-3/4 M1 1 1/4 (31) Under the unchanged federal funds rate of alternative B, M2 growth would be supported by some narrowing of its opportunity cost, as offering rates on retail deposits rise further in partial catch-up to earlier increases in short-term interest rates. (32) Under alternative C, the 1/2 percentage point higher funds rate would induce less rapid expansion of M2 and M3 than under alternative B as opportunity costs resumed their upward movement.</t>
-  </si>
-  <si>
-    <t>Alternative C is in line with current financial market expectations.</t>
-  </si>
-  <si>
-    <t>Under the tighter alternative C, the federal funds rate would be raised 1/2 percentage point, to 6 percent, either by an equivalent rise in the discount rate to 5-1/4 percent with the same borrowing allowance or by an increase in the borrowing allowance to $125 million with the same discount rate. (28) Concern about the possibility of an adverse market reaction, combined with a view that the economic situation still pointed to significant risk of accelerating inflation, would argue for the 50 basis point firming in the federal funds rate associated with alternative C. (29) The 1/2 percentage point rise in the federal funds rate embodied in alternative C, by matching current financial market expec- tations, would have few initial repercussions on market interest rates or exchange rates against our other G-10 trading partners. (32) Under alternative C, the 1/2 percentage point higher funds rate would induce less rapid expansion of M2 and M3 than under alternative B as opportunity costs resumed their upward movement. Growth rates of 1-1/2 percent and 2 percent, respectively, from January to June are anticipated by the staff under alternative C. 11.</t>
-  </si>
-  <si>
-    <t>Alternative A, involving a reduction of the intended funds rate to 5-1/2 percent, could be effected by lowering either the borrowing allowance to $50 million or the discount rate by 50 basis points. In effect, choice of alternative A would imply a view that not only have longer-term interest and exchange rates not overshot on the downside, but that policy may still be too tight to allow markets to compensate fully for oncoming economic weakness. (13) The 50 basis point easing of the federal funds rate under alternative A also would surprise market participants. Somewhat slower growth in the monetary aggre- gates would result from the higher opportunity costs of alternative C, while somewhat faster growth would occur under alternative A. -... *. . * A - - ,- '- " .... .... ..................................... B................. 0% Dec 1200 1150 -- 1100 Feb 1050 1994 Aug I I I I I I II I I I I I '' '''''' '' '' '' 1995 Chart 5 DEBT Billions of Dollars 1 14200 Actual Level S Projected Level - 14000 -- 13800 --1 13600 13400 - 13200 -- 13000 -- 12800 - 12600 Aug Dec 1994 Dec SI I I I l-I I II L 1995 the growth of the broader aggregates be expected to breach the upper or lower bands of their annual ranges, although M3 is virtually at the upper end of its range under alternative A. (15) Consistent with the forecasted moderation in nominal spending, the debt of domestic nonfinancial sectors is expected to slow to around a 4-3/4 percent pace from February to September, bring- ing its rate of growth from the fourth quarter of last year to 5 per- cent--the mid-point of its monitoring range.</t>
-  </si>
-  <si>
-    <t>Under alternative B, federal funds trading would continue around 6 percent, in association with adjustment plus seasonal borrowing of $75 mil- lion. If the Committee believes such an outcome were both likely and acceptable, then it may be inclined to leave the current level of the federal funds rate in place, as under alternative B, unless and 6. Consequently, there would likely be little change in interest rates in response to the choice of alternative B. (14) The table below shows staff projections of money and debt aggregates through September under the unchanged reserve market conditions of alternative B. (More detailed data, including money growth rates under alternatives A and C, are shown in the table and charts on the following pages.) From a March base, average M2 growth would pick up to a 2-1/2 percent rate, while average M3 growth would slow to a 3 percent pace. The Alternative B Growth from March to September M2 2-1/2 M3 3 M1 1/4 Domestic Nonfinancial Debt1 4-3/4 Growth from 1994:Q4 to September M2 2-1/4 M3 3-3/4 M1 1/4 Domestic Nonfinancial Debt 5 1.</t>
-  </si>
-  <si>
-    <t>With financial markets having built in no near-term monetary policy tightening, choice of alternative C would come as a surprise.</t>
-  </si>
-  <si>
-    <t>6 Under alternative C, the federal funds rate would be in- creased to 6-1/2 percent by raising either the borrowing allowance to $125 million or the discount rate by 50 basis points. (10) A case for the 1/2 percentage point increase in the federal funds rate of alternative C could be made on the grounds that, with economic activity having already overshot its potential and the persistence of the slowdown in economic growth not yet firmly estab- lished, more insurance should be taken out against a serious deterior- ation in inflation trends. (11) With financial markets having built in no near-term monetary policy tightening, choice of alternative C would come as a surprise. Somewhat slower growth in the monetary aggre- gates would result from the higher opportunity costs of alternative C, while somewhat faster growth would occur under alternative A.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> This alternative would represent a considerably more aggressive policy action than currently is priced into financial markets.</t>
-  </si>
-  <si>
-    <t>Alternative A would reduce the intended trading level of the funds rate to 5-1/2 percent. Alternative C could be accomplished through an increase in the borrowing allowance to $275 million, while alternative A could be implemented by leaving the allowance for borrowing unchanged at $175 million in the face of seasonally elevated demand. (12) The Committee might consider the easing of monetary policy under alternative A appropriate if it saw substantial risks that the recent sluggish growth of final demand and the associated inventory correction could develop into a prolonged period of growth below potential. (13) Short-term market rates under alternative A would like- ly drop close to one-half percentage point.</t>
-  </si>
-  <si>
-    <t>Under alternative B, federal funds would continue to trade around 6 percent. If the Committee sees the staff forecast as the likely and desired outcome and the risks around it to be reasonably well-balanced, then selection of unchanged reserve market conditions, as under alternative B, would be favored. To accommodate rising demands for seasonal credit, the allowance for adjustment and seasonal borrowings would be raised initially to $225 million under alternative B. Further increases would likely be necessary during the intermeeting period under all of the alterna- tives. Thus, market rates would not be expected to react to selection of alternative B by the Committee. (14) Growth of the monetary and credit aggregates under the unchanged reserve market conditions of alternative B is presented in the table below. Nonetheless, M3 is projected to remain above the upper end of its current 0-to-4 percent annual range through September under alternative B, and even the tighter reserve market conditions of alternative C would not likely be adequate to bring M3 within its range by September. (17) M2 growth, by contrast, is projected to edge up slight- ly from that of the previous four months, to a 2-1/2 percent pace over April through September; this aggregate would remain in the lower half of its l-to-5 percent annual range under alternative B. Although slower growth of nominal income over the second and third quarters will damp the demand for money, opportunity costs of holding M2 assets have leveled off and begun to fall; as the depressing effects of earlier increases in opportunity costs diminish, M2 should grow more closely in line with income.</t>
-  </si>
-  <si>
-    <t>With markets apparently having concluded that rates are unlikely to rise significantly further, the response in the financial markets to the 50 basis point increase of alternative C could be sub- stantial.</t>
-  </si>
-  <si>
-    <t>Under alternative C, the federal funds rate would be boosted 1/2 percentage point, to 6-1/2 percent. Alternative C could be accomplished through an increase in the borrowing allowance to $275 million, while alternative A could be implemented by leaving the allowance for borrowing unchanged at $175 million in the face of seasonally elevated demand. (10) The fifty-basis-point firming of alternative C might be favored by the Committee if it wished to provide more assurance that pressures on resources would soon diminish, so as not to perpetuate the recently elevated rate of inflation and, over time, to return the economy toward a disinflationary path. (11) With markets apparently having concluded that rates are unlikely to rise significantly further, the response in the financial markets to the 50 basis point increase of alternative C could be sub- stantial. Nonetheless, M3 is projected to remain above the upper end of its current 0-to-4 percent annual range through September under alternative B, and even the tighter reserve market conditions of alternative C would not likely be adequate to bring M3 within its range by September.</t>
-  </si>
-  <si>
-    <t>Under the easier policy stance of alternative A, the intended federal funds rate would be reduced by 1/2 percentage point to 5-1/2 percent. (28) A reduction in the federal funds rate, perhaps of the 1/2 percentage point size embodied in alternative A, could be favored as a form of insurance against the downside risks in the economic outlook. (29) Immediate implementation of the 1/2 percentage point cut in the federal funds rate of alternative A would represent a considerably more aggressive policy action than currently is priced into financial markets.</t>
-  </si>
-  <si>
-    <t>Under alternative B, the intended federal funds rate would be maintained at 6 percent. (26) The decision to leave reserve market conditions un- changed, as under alternative B, might be favored if the staff economic forecast, which assumes a constant federal funds rate through early 1996, were viewed as both a reasonable and desirable outcome. (27) Over the past few days, markets have come to view policy action at this meeting as much less likely, and interest and exchange rates probably would change little with the choice of alternative B, -20- though a further small backup in yields cannot be ruled out with the disappointment of some residual expectations of prompt easing. That is, the financial market conditions associated with the unchanged policy of alternative B, including the backup in long-term rates in -21- the staff forecast, might be seen as unnecessarily risking weak spend- ing.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> This alternative would be much larger and sooner than market participants currently expect. </t>
-  </si>
-  <si>
-    <t>(10) A further easing of policy, as under alternative A, could be supported if recent price and wage news were read as suggest- ing that the underlying determinants of inflation were more favorable than in the staff forecast. (11) The drop in the federal funds rate of 1/2 percentage point contemplated under alternative A would be much larger and sooner than market participants currently expect. For the year, M2 is expected to remain below the 5 percent upper bound of its annual range, even under alternative A.4 The projected softening in M3 owes primarily to lower growth in institutional money funds as their yields become better aligned with market rates.</t>
-  </si>
-  <si>
-    <t>Thus, the choice of the unchanged federal funds rate of alternative B should have little immediate impact on market interest rates. (9) Alternative B might be favored to the extent that the staff forecast were seen to be credible and the outcome to balance acceptably Committee concerns about expansion in output with those of the containment of inflation. Growth rates based on alternative B. (15) Growth rates of the broad monetary aggregates are ex- pected to continue to slow from their recent very rapid pace, but to remain relatively strong.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Alternative C would come as a surprise to market par- ticipants, and money market interest rates would rise at least 50 basis points</t>
-  </si>
-  <si>
-    <t>(12) The choice of the higher rates of alternative C would seem to rest on concerns about the longer-term inflation outlook. (13) Alternative C would come as a surprise to market par- ticipants, and money market interest rates would rise at least 50 basis points and the dollar would strengthen further on foreign ex- change markets.</t>
-  </si>
-  <si>
-    <t>(12) If the Committee saw reasonably high odds of more restrictive effects on the economy than the staff forecast, it might -10- favor an easing of the funds rate, as under alternative A.</t>
-  </si>
-  <si>
-    <t>(10) The case for keeping the funds rate at 5-3/4 percent as under alternative B could rest on an assessment that the current funds rate may well provide the appropriate monetary impulse, at least for the time being. Thus, choice by the Commit- tee of alternative B's unchanged funds rate likely would engender just a minor increase of short-term rates. Implied Sept. to1 1994-Q4 1995 December to 1995-Q4 Ranges M2 5.7 4.9 1 - 5 M3 6.0 6.7 2 - 6 M1 -1.6 -1.0 Total debt 4.0 5.2 3 - 7 Nonfederal 4.3 5.4 Note: Growth rates based on alternative B. 1. 4 Under alternative B, M2 is projected to grow at a 5-3/4 percent rate over the final three months of the year. M1 is expected to continue to decline over the remainder of the year, at about a 1-1/2 percent rate under alternative B, as still more banks introduce sweep accounts that transfer funds automatically from NOW accounts to MMDAs to reduce reserve requirements. Actual M1 over the four quarters of this year is now projected to edge down by 1 percent under alternative B. Alternative Levels and Growth Rates for Key Monetary Aggregates M2 Alt.</t>
-  </si>
-  <si>
-    <t>The 1/2 percentage point hike in the funds rate of alternative C would catch market participants off guard.</t>
-  </si>
-  <si>
-    <t>On the basis of relationships embodied in the Greenbook alternative simulation, a policy tightening of the dimensions of alternative C would nudge economic growth to below 2 percent over the next two years, opening up enough slack in labor and product markets to make more noticeable progress toward price stability in 1997 and beyond. (15) The 1/2 percentage point hike in the funds rate of alternative C would catch market participants off guard.</t>
-  </si>
-  <si>
-    <t>The cut in the federal funds rate of 50 basis points under alternative A would come sooner and be larger than now expected in the market.</t>
-  </si>
-  <si>
-    <t>(11) The choice of easing under alternative A might be favored if it were thought that some information about spending--for example, soft industrial commodity prices and a sluggish manufacturing sector or slowing growth of broad money and credit--was suggesting a weakening in aggregate demand not yet evident in more general statis- tics. -10- (12) The cut in the federal funds rate of 50 basis points under alternative A would come sooner and be larger than now expected in the market.</t>
-  </si>
-  <si>
-    <t>Despite the lack of a downward tilt to the inflation projection, the Committee still might favor the unchanged stance of policy in alternative B if it viewed the benefits of further disinflation as insufficient to justify a more restrictive policy stance that pushed the economy below its potential. The case for alternative B would be even stronger if the Committee viewed the staff inflation forecast as too pessimistic-- either because spending would be weaker or because the price-output relationship would be more favorable than the staff assessment. (10) Earlier expectations of the possibility of easing at the November FOMC meeting have largely been erased and, thus, the choice of alternative B should have little impact on market interest rates. -11- (15) The table below presents expected growth of money and debt under the unchanged reserve conditions of alternative B. The rebound in M2 growth, combined with still-brisk issuance of large time deposits to fund bank credit, would result in about 5-1/2 percent M3 growth under alternative B.</t>
-  </si>
-  <si>
-    <t>Alternative C would surprise market participants, who continue to hold the view, supported by statements from some Committee members, that the next policy move will be to ease.</t>
-  </si>
-  <si>
-    <t>(13) The choice of alternative C might be favored to the extent that the Committee wished to have greater assurance that infla- tion would continue to edge down. (14) A move to tighten policy by 50 basis points as under alternative C would especially surprise market participants, who con- tinue to hold the view, supported by statements from some Committee members, that the next policy move will be to ease.</t>
-  </si>
-  <si>
-    <t>Although market participants expect monetary policy to be eased over the next few months, a reduction of 50 basis points in the federal funds rate implemented at this meeting, as called for under alternative A, would be larger than generally expected.</t>
-  </si>
-  <si>
-    <t>(11) Although market participants expect monetary policy to be eased over the next few months, a reduction of 50 basis points in the federal funds rate implemented at this meeting, as called for under alternative A, would be larger than generally expected. (12) Under the staff forecast, alternative A would risk fostering greater inflation pressures, and the move would eventually need to be reversed.</t>
-  </si>
-  <si>
-    <t>(9) In these circumstances, adoption of the unchanged money market conditions of alternative B could prompt a small backup in market interest rates. Accordingly, in the staff forecast, alternative B keeps policy on a path that produces results for economic growth and inflation over 1996 closely in line with the Committee's expectations for next year that were reported in July. (15) The table below presents staff forecasts for money and credit growth for the November-to-March period under the unchanged money market conditions of alternative B.7 Broad measures of money 7. Expansion of M3 picks up to a 5-3/4 percent annual rate over the November-to-March period under alternative B. M2 growth also firms from its unexpectedly weak pace so far in the fourth quarter.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">With market participants expecting an easing rather than a tightening of policy, the 50-basis-point increase in the federal funds rate under alternative C would lead to a sharp jump in other money market interest rates. </t>
-  </si>
-  <si>
-    <t>-10- (13) With market participants expecting an easing rather than a tightening of policy, the 50-basis-point increase in the federal funds rate under alternative C would lead to a sharp jump in other money market interest rates. (14) The FOMC might select alternative C if it saw the risks to inflation at current interest rates as reasonably well balanced and wished to gain more assurance of making longer-term progress toward price stability. Given the demand and inflation relationships incorporated in the staff forecast, the rise in the federal funds rate under alternative C would tilt the inflation rate down slightly in 1997.</t>
-  </si>
-  <si>
-    <t>(25) Justification for a quarter-point reduction in the federal funds rate under alternative A would seem to rest on a belief that the economy is weaker than in the staff outlook, as might be inferred from the tone of some anecdotal reports and recent data, or that the prospects for disinflation are brighter. (26) Money market interest rates would fall by less than a quarter point under alternative A, given current expectations.</t>
-  </si>
-  <si>
-    <t>-18- Short-run Policy Alternatives (23) The unchanged funds rate of alternative B is consistent with the staff Greenbook forecast. Not only might alternative B be seen as attractive if the Committee concurred with this outlook and found the results acceptable, but it also might have appeal as a "wait and see" strategy because delays in data have curtailed the new infor- mation available to the Committee since it eased policy in December. Thus, rates could edge higher under alternative B.16 However, the extent of any rise in such rates likely would be tempered in the near term by the perception that the Committee had merely postponed easing pending the availabi- lity of more information. (28) The table below shows money and credit growth under alternative B for the January-to-June period.</t>
-  </si>
-  <si>
-    <t>(27) If the Committee agreed with the staff outlook for spending and inflation and wanted to make deliberate progress toward price stability, the choice of a quarter-point increase in the federal funds rate under alternative C might be favored.</t>
-  </si>
-  <si>
-    <t>it is difficult to gauge how market participants would react to the 1/2 percentage point of policy ease envisioned under alternative A.</t>
-  </si>
-  <si>
-    <t>(10) Given the staff's assessment of the economy, the 1/2 percentage point easing in reserve market conditions offered under alternative A would boost the economy marginally further beyond its potential and tilt the inflation rate up a bit more noticeably. With the latter outcome apparently inconsistent with the Committee's strategy for achieving its long-run goals, adopting alternative A would seem to require that, relative to the staff, Committee members expect somewhat weaker spending or better inflation. (11) In light of the uncertainty about the current economic situation and the widespread expectation that System policy is on hold, it is difficult to gauge how market participants would react to the 1/2 percentage point of policy ease envisioned under alternative A.</t>
-  </si>
-  <si>
-    <t>With market participants apparently expecting no policy action over the next few months, maintenance of current reserve condi- tions, as under alternative B, would elicit little reaction in credit markets.</t>
-  </si>
-  <si>
-    <t>(8) An unchanged policy stance, as in alternative B, would probably be preferred if the Committee concurred with the staff's as- sessment of the economy, viewed potential risks as about evenly balanced, and was willing to accept the possibility of a slight inten- sification of price pressures. (9) With market participants apparently expecting no policy action over the next few months, maintenance of current reserve condi- tions, as under alternative B, would elicit little reaction in credit markets.</t>
-  </si>
-  <si>
-    <t>The 50 basis point tightening of alternative C would catch market participants unawares and show through to instruments at the shortest maturities.</t>
-  </si>
-  <si>
-    <t>(12) A 1/2 percentage point tightening in reserve conditions, as under alternative C, might be favored if the Committee agreed with the staff forecast but viewed its outcome for inflation as undesir- able, particularly if the Committee wanted to make some progress to- ward price stability. (13) The 50 basis point tightening of alternative C would catch market participants unawares and show through to instruments at the shortest maturities.</t>
-  </si>
-  <si>
-    <t>Financial market partici- pants are anticipating that the FOMC will leave its policy stance unchanged at this meeting, implying that selection of alternative B would have little market impact.</t>
-  </si>
-  <si>
-    <t>In these circumstances, the Committee may prefer to adopt alternative B, 3. Financial market partici- pants are anticipating that the FOMC will leave its policy stance unchanged at this meeting, implying that selection of alternative B would have little market impact. (12) The interest rates of alternative B and associated staff forecast for the economy are thought to be consistent with a slight moderation in the growth of money and credit over coming months relative to their pace of expansion so far in 1996.</t>
-  </si>
-  <si>
-    <t>The Federal Reserve is not expected by market participants to tighten for several months, and hence, investors would be caught off guard</t>
-  </si>
-  <si>
-    <t>Alternative C embodies a 50 basis point increase in the federal funds rate to 5-3/4 percent in order to counter the incipient increase in price pressures. The Federal Reserve is not expected by market participants to tighten for several months, and hence, investors would be caught off guard by the FOMC's choice of alternative C at this meeting.</t>
-  </si>
-  <si>
-    <t>Under alternative B, federal funds would continue to trade around 5-1/4 percent. (23) The money and credit flows associated with a flat federal funds rate under alternative B were discussed in the previous sections of this document under the baseline case.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> A 25 basis point rise in the federal funds rate at this meeting as under alternative C would exceed the small amount currently built into money market yields.</t>
-  </si>
-  <si>
-    <t>-18- (21) A 1/4 percentage point increase in the federal funds rate, as under alternative C, might be favored if the Committee wished to impose greater restraint on spending to reduce the odds of a gradual increase of inflation pressures. (22) A 25 basis point rise in the federal funds rate at this meeting as under alternative C would exceed the small amount currently built into money market yields. Money growth would be expected to slow somewhat more under alternative C, putting the broad aggregates on paths more likely to leave them below the upper ends of their longer-term ranges.</t>
-  </si>
-  <si>
-    <t>(8) Nonetheless, the Committee may well feel that it can afford to wait, as in alternative B, for additional data to accumulate to allow a more confident judgment concerning whether an underlying process of rising inflation seems to be taking hold.</t>
-  </si>
-  <si>
-    <t>Market participants would be somewhat surprised by a Committee decision to raise its intended federal funds rate by 25 basis points</t>
-  </si>
-  <si>
-    <t>(11) Given the recent adjustment to their expectations for monetary policy, market participants would be somewhat surprised by a Committee decision to raise its intended federal funds rate by 25 basis points, as under alternative C.</t>
-  </si>
-  <si>
-    <t>With market participants apparently placing greater than even odds on policy tightening at this meeting, interest rates would likely decline and the dollar weaken on foreign exchange markets if the unchanged policy of alternative B were adopted. Even before the discount rate story earlier this week, markets had built in close to 50/50 odds of a slight policy tightening, and alternative B probably would trigger rate declines that not only reversed the increases associated with the story, but some of those registered earlier in the intermeeting period as well</t>
-  </si>
-  <si>
-    <t>Nonetheless, there are reasons why the Committee might choose the unchanged federal funds rate of alternative B for the upcoming intermeeting period. (9) With market participants apparently placing greater than even odds on policy tightening at this meeting, interest rates would likely decline and the dollar weaken on foreign exchange markets if the unchanged policy of alternative B were adopted. Even before the discount rate story earlier this week, markets had built in close to 50/50 odds of a slight policy tightening, and alternative B probably would trigger rate declines that not only reversed the increases associated with the story, but some of those registered earlier in the intermeeting period as well. M2 is now expected to increase at a 4-1/2 percent rate this year and M3 at a 5-3/4 percent rate under alternative B, somewhat below the upper ends of their growth ranges for the year. Over the August-to-December period, the expansion of M2 is projected to pick up to about a 4-3/4 percent pace, broadly in line with GDP growth under alternative B.</t>
-  </si>
-  <si>
-    <t>(10) A tightening of policy at this Committee meeting, whether by 50 basis points, as assumed in alternative C, or by only 25 basis points, would improve the chances that price pressures would be contained and inflation outcomes would be consistent with the Commit- tee members' expectations in July.</t>
-  </si>
-  <si>
-    <t>This alternative would most likely be read as evidence that the Committee has serious reservations about the prospects for spending.</t>
-  </si>
-  <si>
-    <t>(10) A 50 basis point reduction in the federal funds rate, as under alternative A, might be favored if the Committee viewed the recent softness of final sales as likely to persist. A 50 basis point reduction in the funds rate, as under alternative A, would most likely be read as evidence that the Committee has serious reservations about the prospects for spending.</t>
-  </si>
-  <si>
-    <t>With market participants widely expecting policy to remain on hold for some time, the Committee's selection of alternative B should elicit little response in financial markets.</t>
-  </si>
-  <si>
-    <t>(6) If the Committee views the staff forecast as both likely and acceptable, it presumably would favor standing pat--alternative B. Even if the Committee found unacceptable the forecasted upcreep in core inflation (abstracting from technical CPI adjustments), it might want to wait for more evidence that such an outcome is in train before taking action. (7) With market participants widely expecting policy to remain on hold for some time, the Committee's selection of alternative B should elicit little response in financial markets. (13) In coming months, offering rates on M2 accounts are not expected to change much under alternative B, maintaining opportunity costs at around their recent levels. As a result, M1 is anticipated to decline at a 9 percent rate over the October-to-March period under alternative B; adjusted for sweeps, M1 would increase at a 3-3/4 percent rate over that span.</t>
-  </si>
-  <si>
-    <t>The choice of alternative C would come as a surprise to market participants.</t>
-  </si>
-  <si>
-    <t>(8) A policy tightening, such as the 50 basis point firming of the federal funds rate under alternative C, might be favored should the Committee wish to move promptly to counter the updrift in underlying inflation embedded in the staff outlook. (9) The choice of alternative C would come as a surprise to market participants.</t>
-  </si>
-  <si>
-    <t>the market is not expecting a change in policy, a 50 basis point funds rate reduction would show through completely to other short-term rates.</t>
-  </si>
-  <si>
-    <t>(12) A 50 basis point reduction in the federal funds rate (alternative A) would seem to require a judgment that the upward pressure on prices is less than in the staff forecast at current interest rate levels. (13) Because the market is not expecting a change in policy, a 50 basis point funds rate reduction, as in alternative A, would show through completely to other short-term rates.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">With market participants almost universally expecting policy to be on hold for a time, the Committee's selection of alternative B would prompt little response in financial markets. </t>
-  </si>
-  <si>
-    <t>In these circumstances, the Committee may wish to keep policy unchanged (alternative B), awaiting more information to assess how markets may evolve and how the other uncertainties may be resolved. (9) With market participants almost universally expecting policy to be on hold for a time, the Committee's selection of alternative B would prompt little response in -8- financial markets. (14) Under alternative B and the staff forecast, both debt and money should expand at moderate rates in coming months, in line with projected nominal GDP.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The choice of alternative C would surprise market participants and perhaps lead them to reconsider their view on the Federal Reserve's longer-term objectives.</t>
-  </si>
-  <si>
-    <t>(10) A 50 basis point firming of the funds rate (alternative C) might be favored if the Committee wished to move promptly to stem the rise in underlying inflation in the staff forecast and increase the odds on making some headway on its longer-run objective of price stability. (11) The choice of alternative C would surprise market participants and perhaps lead them to reconsider their view on the Federal Reserve's longer-term objectives.</t>
-  </si>
-  <si>
-    <t>Under alternative B, the federal funds rate would kept at 5-1/4 percent. (22) Financial markets currently are not anticipating a change in policy at the February meeting, and thus the choice of alternative B should initially have little impact on interest rates or the foreign exchange value of the dollar. (25) Growth of the broad monetary aggregates is expected to slow under alternative B from the very rapid pace of late 1996.</t>
-  </si>
-  <si>
-    <t>The tightening of policy under alternative C would surprise market participants, and short-term interest rates, including the prime rate, would rise by the half-point hike in the federal funds rate.</t>
-  </si>
-  <si>
-    <t>Under alternative C, the federal funds rate would be raised by 1/2 percentage point to 5-3/4 percent, either through a less generous provision of nonborrowed reserves or a hike in the discount rate. While inflation does not deteriorate appreciably in the near term, given the lags in the effect of policy, the sooner the Committee begins to tighten--as under alternative C--the lower the odds that higher inflation will become embedded in price and wage setting. (24) The tightening of policy under alternative C would surprise market participants, and short-term interest rates, including the prime rate, would rise by the half-point hike in the federal funds rate.</t>
-  </si>
-  <si>
-    <t>With market participants apparently placing high odds on a 25 basis point tightening in the federal funds rate at the March meeting, interest rates probably would fall somewhat if the unchanged policy of alternative B were adopted.</t>
-  </si>
-  <si>
-    <t>(7) Nonetheless, a number of considerations regarding the outlook might induce the Committee to forgo tightening at the March meeting, as under alternative B. (8) With market participants apparently placing high odds on a 25 basis point tightening in the federal funds rate at the March meeting, interest rates probably would fall somewhat if the unchanged policy of alternative B were adopted. (12) Under alternative B and the staff forecast, debt is expected to continue to grow around its recent pace in the months ahead, while money growth tends to moderate as the expansion of nominal GDP slows. (13) M2 growth from February to June under alternative B is projected to slow to a 4-1/2 percent rate, reflecting the deceleration in nominal GDP.</t>
-  </si>
-  <si>
-    <t>(9) The Committee might choose to increase the federal funds rate, perhaps by the 50 basis points of alternative C, in order to lean against the likely buildup of inflation pressures.</t>
-  </si>
-  <si>
-    <t>(8) Despite the staffs perception that underlying inflation pressures will be building, the Committee may find reasons to leave its policy stance unchanged, at least for the time being, as incorporated in alternative B, which keeps the intended federal funds rate at 5-1/2 percent. However, in recent weeks, markets appear to have removed all but modest odds of any action, and the choice of alternative B should trigger a relatively minor decline in rates. - 11 - (14) The runoff of the tax-related deposit surge of April should be completed in May, after which the monthly growth of M2 and M3 under alternative B is expected to stabilize at annual rates of 4-1/2 and 6 percent, respectively, through September--somewhat below the pace of the first five months of the year.</t>
-  </si>
-  <si>
-    <t>Rise in the federal funds rate under alternative C would come as a major surprise to financial market participants</t>
-  </si>
-  <si>
-    <t>(11) The 1/2 percentage point rise in the federal funds rate under alternative C would come as a major surprise to financial market participants and likely would spark a considerable rise in interest rates and the exchange value of the dollar.</t>
-  </si>
-  <si>
-    <t>No change in the stance of monetary policy at this FOMC meeting is built into the structure of market interest rates, so financial market prices would react little to the Committee's choice of alternative B.</t>
-  </si>
-  <si>
-    <t>Under alternative B, the intended federal funds rate would be maintained at its current 5-1/2 percent level. (34) The Committee may favor the unchanged federal funds rate of alternative B if it thinks that chances are that the staff has not gone far enough to incorporate a more favorable tradeoff between resource use and inflation into the outlook. No change in the stance of monetary policy at this FOMC meeting is built into the structure of market interest rates, so financial market prices would react little to the Committee's choice of alternative B. (37) The staffs projections of money and debt growth this year, assuming main- tenance of the unchanged federal funds rate of alternative B, were described in the previous section.</t>
-  </si>
-  <si>
-    <t>Under alternative C, it would be raised 1/4 percentage point to 5-3/4 percent. (35) The 1/4 percentage-point increase in the federal funds rate embodied in alternative C might seem appropriate if the Committee sees the likelihood of intensifying inflation pressures, as in the Greenbook, and wishes to impart some resistance to the anticipated acceleration of prices. (36) The 25 basis point firming in alternative C would catch market participants off guard, inducing an immediate selloff in securities markets and an appreciation of the dollar in exchange markets, with short-term interest rates jumping by virtually the same amount as the intended funds rate. Maintenance of the slightly higher short-term interest rates of alternative C would lower these growth rates only slightly over this year.</t>
-  </si>
-  <si>
-    <t>Market participants uniformly do not expect a near-term policy move by the Federal Reserve, and selection of alternative B by the Committee should elicit little imme- diate market reaction.</t>
-  </si>
-  <si>
-    <t>Under alternative B, the intended federal funds rate would be kept at its current level of 5-1/2 percent. (8) Market participants uniformly do not expect a near-term policy move by the Federal Reserve, and selection of alternative B by the Committee should elicit little imme- diate market reaction. (11) Under the unchanged federal funds rate of alternative B, M2 is projected to grow at a moderate 4-1/2 percent rate on average over the remaining months of the year, around the expected rate of expansion of nominal GDP, leaving this aggregate a little below the upper limit of its 1 to 5 percent growth range for the year.</t>
-  </si>
-  <si>
-    <t>Under alternative C, it would be boosted to 5-3/4 percent, either through reduced provision of nonborrowed reserves or a hike in the discount rate. If the Committee wants more insurance against the possibility that inflation will begin to pick up, and especially if it wishes to tilt the odds a little in the direction of further progress toward price stability over coming years, it may wish to raise the intended federal funds rate at this meeting, perhaps by the 25 basis points of alternative C. (10) With no near-term tightening expected, the market response to implementation of alternative C could be sharp.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Virtually no one in the market anticipates action at this meeting, so that yields across the term structure are not likely to budge much and the dollar should continue to trade around its current level on foreign exchange markets immediately following the adoption of the unchanged policy stance of alternative B. </t>
-  </si>
-  <si>
-    <t>(6) The staff assessment of the pressures on resources implies that policy restraint is in order at some point to check an upcreep in inflation, but the Committee may, nonetheless, prefer to hold the federal funds rate at its current level of 5-1/2 percent at this meeting, as in alternative B. (8) Virtually no one in the market anticipates action at this meeting, so that yields across the term structure are not likely to budge much and the dollar should continue to trade around its current level on foreign exchange markets immediately following the adoption of the unchanged policy stance of alternative B. Treasury bill rates have been depressed of late by low issuance, and the turnaround in bill sales in the fourth quarter prompted by the seasonal bulge in the federal deficit may roll back some of the decline in rates on those securities. - 10- (10) Under the unchanged policy stance of alternative B, the growth of the monetary aggregates should slow significantly.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Committee's choice of alternative C at this meeting would catch market participants completely unawares. </t>
-  </si>
-  <si>
-    <t>(7) If the Committee were confident that the staff had correctly identified the threat that inflation would pick up, or wanted some greater assurance of further progress toward price stability, it would likely favor raising the federal funds rate promptly, perhaps at this meeting by the 25 basis points of alternative C. (9) The Committee's choice of alternative C at this meeting would catch market participants completely unawares. Under alternative C, even though opportunity costs would likely rise with the imposition of monetary restraint, M2 might be bolstered to some extent in the near term should a correction in the stock and bond markets induce investors to favor money market over bond and stock mutual funds.</t>
-  </si>
-  <si>
-    <t>(10) Alternative B, which would leave the intended federal funds rate at 5-1/2 percent, could be chosen at this meeting either merely as a deferral of a tighter stance until financial markets have become more resilient, or, more positively, as a justifiable policy posture, absent some change in the tenor of incoming information about inflation prospects. (12) The staff anticipates that, under alternative B, M2 and M3 will grow at annual rates of 4-1/2 and 6-1/4 percent, respectively, over the five months from October to March of next year.</t>
-  </si>
-  <si>
-    <t>(9) If the Committee shares the staffs assessment that the U.S. economy has overshot its sustainable productive potential, it may be disposed to tighten its policy stance, as in the 25 basis point rise in the funds rate in alternative C.</t>
-  </si>
-  <si>
-    <t>(13) The 25 basis point easing of Alternative A might be favored if the Committee were concerned that turmoil abroad might have an even greater impact on the U.S. economy than the staff has built into the forecast.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The markets expect no policy action over the next few months and would react little, if at all, to the choice of alternative B</t>
-  </si>
-  <si>
-    <t>Even if the Committee is concerned about the pressures on labor resources and finds the eventual uptrend in underlying -9- inflation unacceptable, it may be willing to keep the funds rate constant at this meeting, as under Alternative B. Under alternative B, the Committee would be buying time to assess the extent to which developments abroad restrain aggregate demand, depress oil prices, and support the dollar, as well as the degree to which recent momentum in the economy might be sustained. (10) The markets expect no policy action over the next few months and would react little, if at all, to the choice of alternative B. Apart from year-end effects, interest rates-- especially Treasury yields--should fluctuate close to recent lows over the intermeeting period. M2 growth is projected at around a 4 percent annual pace over the November-to-March period under alternative B, leaving this aggregate near the upper end of its provisional 1998 range.</t>
-  </si>
-  <si>
-    <t>(11) The 25 basis point tightening of Alternative C might be favored if the Committee wanted to lean against the inflationary bias that may well be inherent in the current and prospective tautness of labor markets.</t>
-  </si>
-  <si>
-    <t>sufficient chances of a shortfall in activity from the staff forecast to suggest a small easing at this time-</t>
-  </si>
-  <si>
-    <t>The dollar would be expected to trade around its levels of late, off some from its recent peak (23) The Committee may see sufficient chances of a shortfall in activity from the staff forecast to suggest a small easing at this time--as in the 25 basis point decline in the federal funds rate under alternative A.</t>
-  </si>
-  <si>
-    <t>The staff forecast is built on an unchanged federal funds rate, and if the Committee agrees that this is both a reasonable and desirable outcome under those conditions, retaining the current stance of policy under alternative B would be appropriate.</t>
   </si>
   <si>
     <t>(24) Alternative C might be favored if the Committee saw the economy as continuing to operate beyond its potential, with the risk that sustained pressures on labor markets might show through more forcefully than in the staff forecast to higher labor costs and prices, perhaps hinted at in the recent employment cost report.</t>
@@ -4023,8 +4023,8 @@
   <dimension ref="A1:AA376"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A334" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E351" sqref="E351"/>
+      <pane ySplit="1" topLeftCell="A311" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P322" sqref="P322"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4036,10 +4036,12 @@
     <col min="6" max="6" width="19.6640625" customWidth="1"/>
     <col min="9" max="9" width="15.1640625" customWidth="1"/>
     <col min="10" max="10" width="44" customWidth="1"/>
+    <col min="11" max="11" width="18" customWidth="1"/>
     <col min="12" max="12" width="32.33203125" customWidth="1"/>
     <col min="13" max="13" width="30.83203125" customWidth="1"/>
     <col min="14" max="14" width="55.33203125" customWidth="1"/>
-    <col min="16" max="16" width="14.6640625" customWidth="1"/>
+    <col min="15" max="15" width="19.5" customWidth="1"/>
+    <col min="16" max="16" width="23.33203125" customWidth="1"/>
     <col min="17" max="18" width="31.5" customWidth="1"/>
     <col min="19" max="19" width="26.33203125" customWidth="1"/>
     <col min="20" max="20" width="22.33203125" customWidth="1"/>
@@ -12810,16 +12812,16 @@
         <v>652</v>
       </c>
       <c r="O234" t="s">
-        <v>653</v>
+        <v>571</v>
       </c>
       <c r="P234">
         <v>0.5</v>
       </c>
       <c r="Q234" t="s">
+        <v>653</v>
+      </c>
+      <c r="R234" t="s">
         <v>654</v>
-      </c>
-      <c r="R234" t="s">
-        <v>655</v>
       </c>
       <c r="V234" t="s">
         <v>30</v>
@@ -12854,7 +12856,7 @@
         <v>-0.5</v>
       </c>
       <c r="J235" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="K235" t="s">
         <v>569</v>
@@ -12864,7 +12866,7 @@
         <v>0</v>
       </c>
       <c r="N235" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="O235" t="s">
         <v>582</v>
@@ -12908,7 +12910,7 @@
         <v>-0.5</v>
       </c>
       <c r="J236" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="K236" t="s">
         <v>569</v>
@@ -12918,7 +12920,7 @@
         <v>0</v>
       </c>
       <c r="N236" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="O236" t="s">
         <v>582</v>
@@ -12962,7 +12964,7 @@
         <v>-0.5</v>
       </c>
       <c r="J237" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="K237" t="s">
         <v>569</v>
@@ -12972,7 +12974,7 @@
         <v>0</v>
       </c>
       <c r="N237" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="O237" t="s">
         <v>582</v>
@@ -13016,7 +13018,7 @@
         <v>-0.5</v>
       </c>
       <c r="J238" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="K238" t="s">
         <v>569</v>
@@ -13026,7 +13028,7 @@
         <v>0</v>
       </c>
       <c r="N238" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="O238" t="s">
         <v>582</v>
@@ -13070,7 +13072,7 @@
         <v>-0.5</v>
       </c>
       <c r="J239" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="K239" t="s">
         <v>569</v>
@@ -13080,7 +13082,7 @@
         <v>0</v>
       </c>
       <c r="N239" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="O239" t="s">
         <v>582</v>
@@ -13124,10 +13126,10 @@
         <v>-0.5</v>
       </c>
       <c r="I240" t="s">
+        <v>665</v>
+      </c>
+      <c r="J240" t="s">
         <v>666</v>
-      </c>
-      <c r="J240" t="s">
-        <v>667</v>
       </c>
       <c r="K240" t="s">
         <v>569</v>
@@ -13137,7 +13139,7 @@
         <v>0</v>
       </c>
       <c r="N240" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="O240" t="s">
         <v>571</v>
@@ -13146,7 +13148,7 @@
         <v>0.5</v>
       </c>
       <c r="R240" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="V240" t="s">
         <v>30</v>
@@ -13181,7 +13183,7 @@
         <v>-0.5</v>
       </c>
       <c r="J241" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="K241" t="s">
         <v>569</v>
@@ -13191,7 +13193,7 @@
         <v>0</v>
       </c>
       <c r="N241" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="O241" t="s">
         <v>571</v>
@@ -13200,7 +13202,7 @@
         <v>0.5</v>
       </c>
       <c r="R241" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="V241" t="s">
         <v>30</v>
@@ -13235,7 +13237,7 @@
         <v>-0.5</v>
       </c>
       <c r="J242" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="K242" t="s">
         <v>569</v>
@@ -13245,7 +13247,7 @@
         <v>0</v>
       </c>
       <c r="N242" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="O242" t="s">
         <v>571</v>
@@ -13254,7 +13256,7 @@
         <v>0.5</v>
       </c>
       <c r="R242" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="V242" t="s">
         <v>30</v>
@@ -13289,7 +13291,7 @@
         <v>-0.5</v>
       </c>
       <c r="J243" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="K243" t="s">
         <v>569</v>
@@ -13299,7 +13301,7 @@
         <v>0</v>
       </c>
       <c r="N243" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="O243" t="s">
         <v>571</v>
@@ -13308,7 +13310,7 @@
         <v>0.5</v>
       </c>
       <c r="R243" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="V243" t="s">
         <v>30</v>
@@ -13343,7 +13345,7 @@
         <v>-0.5</v>
       </c>
       <c r="J244" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="K244" t="s">
         <v>569</v>
@@ -13353,7 +13355,7 @@
         <v>0</v>
       </c>
       <c r="N244" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="O244" t="s">
         <v>571</v>
@@ -13397,7 +13399,7 @@
         <v>-0.5</v>
       </c>
       <c r="J245" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="K245" t="s">
         <v>569</v>
@@ -13407,7 +13409,7 @@
         <v>0</v>
       </c>
       <c r="N245" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="O245" t="s">
         <v>571</v>
@@ -13451,7 +13453,7 @@
         <v>-0.5</v>
       </c>
       <c r="J246" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="K246" t="s">
         <v>569</v>
@@ -13461,7 +13463,7 @@
         <v>0</v>
       </c>
       <c r="N246" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="O246" t="s">
         <v>571</v>
@@ -13470,7 +13472,7 @@
         <v>0.5</v>
       </c>
       <c r="R246" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="V246" t="s">
         <v>30</v>
@@ -13505,7 +13507,7 @@
         <v>-0.5</v>
       </c>
       <c r="J247" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="K247" t="s">
         <v>569</v>
@@ -13514,10 +13516,10 @@
         <v>0</v>
       </c>
       <c r="M247" t="s">
+        <v>686</v>
+      </c>
+      <c r="N247" t="s">
         <v>687</v>
-      </c>
-      <c r="N247" t="s">
-        <v>688</v>
       </c>
       <c r="O247" t="s">
         <v>571</v>
@@ -13526,10 +13528,10 @@
         <v>0.5</v>
       </c>
       <c r="Q247" t="s">
+        <v>688</v>
+      </c>
+      <c r="R247" t="s">
         <v>689</v>
-      </c>
-      <c r="R247" t="s">
-        <v>690</v>
       </c>
       <c r="V247" t="s">
         <v>30</v>
@@ -13564,7 +13566,7 @@
         <v>-0.5</v>
       </c>
       <c r="J248" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="K248" t="s">
         <v>569</v>
@@ -13573,7 +13575,7 @@
         <v>0</v>
       </c>
       <c r="N248" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="O248" t="s">
         <v>571</v>
@@ -13582,10 +13584,10 @@
         <v>0.5</v>
       </c>
       <c r="Q248" t="s">
+        <v>692</v>
+      </c>
+      <c r="R248" t="s">
         <v>693</v>
-      </c>
-      <c r="R248" t="s">
-        <v>694</v>
       </c>
       <c r="V248" t="s">
         <v>30</v>
@@ -13620,7 +13622,7 @@
         <v>-0.5</v>
       </c>
       <c r="J249" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="K249" t="s">
         <v>569</v>
@@ -13629,10 +13631,10 @@
         <v>0</v>
       </c>
       <c r="M249" t="s">
+        <v>695</v>
+      </c>
+      <c r="N249" t="s">
         <v>696</v>
-      </c>
-      <c r="N249" t="s">
-        <v>697</v>
       </c>
       <c r="O249" t="s">
         <v>571</v>
@@ -13641,10 +13643,10 @@
         <v>0.5</v>
       </c>
       <c r="Q249" t="s">
+        <v>697</v>
+      </c>
+      <c r="R249" t="s">
         <v>698</v>
-      </c>
-      <c r="R249" t="s">
-        <v>699</v>
       </c>
       <c r="V249" t="s">
         <v>30</v>
@@ -13679,7 +13681,7 @@
         <v>-0.5</v>
       </c>
       <c r="J250" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="K250" t="s">
         <v>569</v>
@@ -13688,10 +13690,10 @@
         <v>0</v>
       </c>
       <c r="M250" t="s">
+        <v>700</v>
+      </c>
+      <c r="N250" t="s">
         <v>701</v>
-      </c>
-      <c r="N250" t="s">
-        <v>702</v>
       </c>
       <c r="O250" t="s">
         <v>571</v>
@@ -13700,10 +13702,10 @@
         <v>0.5</v>
       </c>
       <c r="Q250" t="s">
+        <v>702</v>
+      </c>
+      <c r="R250" t="s">
         <v>703</v>
-      </c>
-      <c r="R250" t="s">
-        <v>704</v>
       </c>
       <c r="V250" t="s">
         <v>30</v>
@@ -13738,7 +13740,7 @@
         <v>-0.5</v>
       </c>
       <c r="J251" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="K251" t="s">
         <v>569</v>
@@ -13747,7 +13749,7 @@
         <v>0</v>
       </c>
       <c r="N251" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="O251" t="s">
         <v>571</v>
@@ -13756,10 +13758,10 @@
         <v>0.5</v>
       </c>
       <c r="Q251" t="s">
+        <v>706</v>
+      </c>
+      <c r="R251" t="s">
         <v>707</v>
-      </c>
-      <c r="R251" t="s">
-        <v>708</v>
       </c>
       <c r="V251" t="s">
         <v>30</v>
@@ -13794,7 +13796,7 @@
         <v>-0.5</v>
       </c>
       <c r="J252" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="K252" t="s">
         <v>569</v>
@@ -13803,10 +13805,10 @@
         <v>0</v>
       </c>
       <c r="M252" t="s">
+        <v>709</v>
+      </c>
+      <c r="N252" t="s">
         <v>710</v>
-      </c>
-      <c r="N252" t="s">
-        <v>711</v>
       </c>
       <c r="O252" t="s">
         <v>571</v>
@@ -13815,7 +13817,7 @@
         <v>0.5</v>
       </c>
       <c r="R252" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="V252" t="s">
         <v>30</v>
@@ -13850,10 +13852,10 @@
         <v>-0.5</v>
       </c>
       <c r="I253" t="s">
+        <v>712</v>
+      </c>
+      <c r="J253" t="s">
         <v>713</v>
-      </c>
-      <c r="J253" t="s">
-        <v>714</v>
       </c>
       <c r="K253" t="s">
         <v>569</v>
@@ -13862,7 +13864,7 @@
         <v>0</v>
       </c>
       <c r="N253" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="O253" t="s">
         <v>571</v>
@@ -13871,7 +13873,7 @@
         <v>0.5</v>
       </c>
       <c r="R253" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="V253" t="s">
         <v>30</v>
@@ -13906,10 +13908,10 @@
         <v>-0.5</v>
       </c>
       <c r="I254" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="J254" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="K254" t="s">
         <v>569</v>
@@ -13918,7 +13920,7 @@
         <v>0</v>
       </c>
       <c r="N254" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="O254" t="s">
         <v>571</v>
@@ -13927,10 +13929,10 @@
         <v>0.5</v>
       </c>
       <c r="Q254" t="s">
+        <v>718</v>
+      </c>
+      <c r="R254" t="s">
         <v>719</v>
-      </c>
-      <c r="R254" t="s">
-        <v>720</v>
       </c>
       <c r="V254" t="s">
         <v>30</v>
@@ -13965,10 +13967,10 @@
         <v>-0.5</v>
       </c>
       <c r="I255" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="J255" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="K255" t="s">
         <v>569</v>
@@ -13977,10 +13979,10 @@
         <v>0</v>
       </c>
       <c r="M255" t="s">
+        <v>721</v>
+      </c>
+      <c r="N255" t="s">
         <v>722</v>
-      </c>
-      <c r="N255" t="s">
-        <v>723</v>
       </c>
       <c r="O255" t="s">
         <v>571</v>
@@ -13989,10 +13991,10 @@
         <v>0.5</v>
       </c>
       <c r="Q255" t="s">
+        <v>723</v>
+      </c>
+      <c r="R255" t="s">
         <v>724</v>
-      </c>
-      <c r="R255" t="s">
-        <v>725</v>
       </c>
       <c r="V255" t="s">
         <v>30</v>
@@ -14036,10 +14038,10 @@
         <v>0</v>
       </c>
       <c r="M256" t="s">
+        <v>725</v>
+      </c>
+      <c r="N256" t="s">
         <v>726</v>
-      </c>
-      <c r="N256" t="s">
-        <v>727</v>
       </c>
       <c r="O256" t="s">
         <v>571</v>
@@ -14048,10 +14050,10 @@
         <v>0.5</v>
       </c>
       <c r="Q256" t="s">
+        <v>727</v>
+      </c>
+      <c r="R256" t="s">
         <v>728</v>
-      </c>
-      <c r="R256" t="s">
-        <v>729</v>
       </c>
       <c r="V256" t="s">
         <v>30</v>
@@ -14095,7 +14097,7 @@
         <v>0</v>
       </c>
       <c r="N257" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="O257" t="s">
         <v>571</v>
@@ -14104,7 +14106,7 @@
         <v>0.25</v>
       </c>
       <c r="R257" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="S257" t="s">
         <v>571</v>
@@ -14113,7 +14115,7 @@
         <v>0.5</v>
       </c>
       <c r="V257" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="Z257" t="s">
         <v>31</v>
@@ -14148,13 +14150,13 @@
         <v>27</v>
       </c>
       <c r="K258" t="s">
-        <v>653</v>
+        <v>569</v>
       </c>
       <c r="L258">
         <v>0</v>
       </c>
       <c r="N258" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="O258" t="s">
         <v>571</v>
@@ -14163,7 +14165,7 @@
         <v>0.25</v>
       </c>
       <c r="R258" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="S258" t="s">
         <v>571</v>
@@ -14172,7 +14174,7 @@
         <v>0.5</v>
       </c>
       <c r="V258" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="Z258" t="s">
         <v>31</v>
@@ -14213,7 +14215,7 @@
         <v>0</v>
       </c>
       <c r="N259" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="O259" t="s">
         <v>571</v>
@@ -14222,10 +14224,10 @@
         <v>0.25</v>
       </c>
       <c r="Q259" t="s">
+        <v>736</v>
+      </c>
+      <c r="R259" t="s">
         <v>737</v>
-      </c>
-      <c r="R259" t="s">
-        <v>738</v>
       </c>
       <c r="S259" t="s">
         <v>571</v>
@@ -14234,7 +14236,7 @@
         <v>0.5</v>
       </c>
       <c r="V259" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="Z259" t="s">
         <v>31</v>
@@ -14275,10 +14277,10 @@
         <v>0</v>
       </c>
       <c r="M260" t="s">
+        <v>739</v>
+      </c>
+      <c r="N260" t="s">
         <v>740</v>
-      </c>
-      <c r="N260" t="s">
-        <v>741</v>
       </c>
       <c r="O260" t="s">
         <v>571</v>
@@ -14287,10 +14289,10 @@
         <v>0.25</v>
       </c>
       <c r="Q260" t="s">
+        <v>741</v>
+      </c>
+      <c r="R260" t="s">
         <v>742</v>
-      </c>
-      <c r="R260" t="s">
-        <v>743</v>
       </c>
       <c r="S260" t="s">
         <v>571</v>
@@ -14299,7 +14301,7 @@
         <v>0.5</v>
       </c>
       <c r="V260" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="Z260" t="s">
         <v>31</v>
@@ -14340,7 +14342,7 @@
         <v>0</v>
       </c>
       <c r="N261" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="O261" t="s">
         <v>571</v>
@@ -14349,10 +14351,10 @@
         <v>0.5</v>
       </c>
       <c r="Q261" t="s">
+        <v>745</v>
+      </c>
+      <c r="R261" t="s">
         <v>746</v>
-      </c>
-      <c r="R261" t="s">
-        <v>747</v>
       </c>
       <c r="V261" t="s">
         <v>30</v>
@@ -14396,7 +14398,7 @@
         <v>0</v>
       </c>
       <c r="N262" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="O262" t="s">
         <v>571</v>
@@ -14405,7 +14407,7 @@
         <v>0.5</v>
       </c>
       <c r="R262" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="V262" t="s">
         <v>30</v>
@@ -14449,10 +14451,10 @@
         <v>0</v>
       </c>
       <c r="M263" t="s">
+        <v>749</v>
+      </c>
+      <c r="N263" t="s">
         <v>750</v>
-      </c>
-      <c r="N263" t="s">
-        <v>751</v>
       </c>
       <c r="O263" t="s">
         <v>571</v>
@@ -14461,10 +14463,10 @@
         <v>0.5</v>
       </c>
       <c r="Q263" t="s">
+        <v>751</v>
+      </c>
+      <c r="R263" t="s">
         <v>752</v>
-      </c>
-      <c r="R263" t="s">
-        <v>753</v>
       </c>
       <c r="V263" t="s">
         <v>30</v>
@@ -14499,10 +14501,10 @@
         <v>-0.5</v>
       </c>
       <c r="I264" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="J264" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="K264" t="s">
         <v>569</v>
@@ -14511,7 +14513,7 @@
         <v>0</v>
       </c>
       <c r="N264" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="O264" t="s">
         <v>571</v>
@@ -14520,10 +14522,10 @@
         <v>0.5</v>
       </c>
       <c r="Q264" t="s">
+        <v>755</v>
+      </c>
+      <c r="R264" t="s">
         <v>756</v>
-      </c>
-      <c r="R264" t="s">
-        <v>757</v>
       </c>
       <c r="V264" t="s">
         <v>30</v>
@@ -14558,10 +14560,10 @@
         <v>-0.5</v>
       </c>
       <c r="I265" t="s">
+        <v>757</v>
+      </c>
+      <c r="J265" t="s">
         <v>758</v>
-      </c>
-      <c r="J265" t="s">
-        <v>759</v>
       </c>
       <c r="K265" t="s">
         <v>569</v>
@@ -14570,7 +14572,7 @@
         <v>0</v>
       </c>
       <c r="N265" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="O265" t="s">
         <v>571</v>
@@ -14579,10 +14581,10 @@
         <v>0.5</v>
       </c>
       <c r="Q265" t="s">
+        <v>760</v>
+      </c>
+      <c r="R265" t="s">
         <v>761</v>
-      </c>
-      <c r="R265" t="s">
-        <v>762</v>
       </c>
       <c r="V265" t="s">
         <v>30</v>
@@ -14617,10 +14619,10 @@
         <v>-0.5</v>
       </c>
       <c r="I266" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="J266" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="K266" t="s">
         <v>569</v>
@@ -14629,7 +14631,7 @@
         <v>0</v>
       </c>
       <c r="N266" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="O266" t="s">
         <v>582</v>
@@ -14670,19 +14672,19 @@
         <v>-0.5</v>
       </c>
       <c r="I267" t="s">
+        <v>764</v>
+      </c>
+      <c r="J267" t="s">
         <v>765</v>
       </c>
-      <c r="J267" t="s">
-        <v>766</v>
-      </c>
       <c r="K267" t="s">
-        <v>653</v>
+        <v>569</v>
       </c>
       <c r="L267">
         <v>0</v>
       </c>
       <c r="N267" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="O267" t="s">
         <v>571</v>
@@ -14691,10 +14693,10 @@
         <v>0.5</v>
       </c>
       <c r="Q267" t="s">
+        <v>767</v>
+      </c>
+      <c r="R267" t="s">
         <v>768</v>
-      </c>
-      <c r="R267" t="s">
-        <v>769</v>
       </c>
       <c r="V267" t="s">
         <v>30</v>
@@ -14729,7 +14731,7 @@
         <v>-0.5</v>
       </c>
       <c r="J268" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="K268" t="s">
         <v>569</v>
@@ -14738,7 +14740,7 @@
         <v>0</v>
       </c>
       <c r="N268" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="O268" t="s">
         <v>571</v>
@@ -14747,10 +14749,10 @@
         <v>0.5</v>
       </c>
       <c r="Q268" t="s">
+        <v>771</v>
+      </c>
+      <c r="R268" t="s">
         <v>772</v>
-      </c>
-      <c r="R268" t="s">
-        <v>773</v>
       </c>
       <c r="V268" t="s">
         <v>30</v>
@@ -14785,10 +14787,10 @@
         <v>-0.5</v>
       </c>
       <c r="I269" t="s">
+        <v>773</v>
+      </c>
+      <c r="J269" t="s">
         <v>774</v>
-      </c>
-      <c r="J269" t="s">
-        <v>775</v>
       </c>
       <c r="K269" t="s">
         <v>569</v>
@@ -14797,7 +14799,7 @@
         <v>0</v>
       </c>
       <c r="N269" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="O269" t="s">
         <v>571</v>
@@ -14806,10 +14808,10 @@
         <v>0.5</v>
       </c>
       <c r="Q269" t="s">
+        <v>776</v>
+      </c>
+      <c r="R269" t="s">
         <v>777</v>
-      </c>
-      <c r="R269" t="s">
-        <v>778</v>
       </c>
       <c r="V269" t="s">
         <v>30</v>
@@ -14844,10 +14846,10 @@
         <v>-0.5</v>
       </c>
       <c r="I270" t="s">
+        <v>778</v>
+      </c>
+      <c r="J270" t="s">
         <v>779</v>
-      </c>
-      <c r="J270" t="s">
-        <v>780</v>
       </c>
       <c r="K270" t="s">
         <v>569</v>
@@ -14856,7 +14858,7 @@
         <v>0</v>
       </c>
       <c r="N270" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="O270" t="s">
         <v>571</v>
@@ -14865,10 +14867,10 @@
         <v>0.5</v>
       </c>
       <c r="Q270" t="s">
+        <v>781</v>
+      </c>
+      <c r="R270" t="s">
         <v>782</v>
-      </c>
-      <c r="R270" t="s">
-        <v>783</v>
       </c>
       <c r="V270" t="s">
         <v>30</v>
@@ -14903,7 +14905,7 @@
         <v>-0.25</v>
       </c>
       <c r="J271" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="K271" t="s">
         <v>569</v>
@@ -14912,7 +14914,7 @@
         <v>0</v>
       </c>
       <c r="N271" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="O271" t="s">
         <v>571</v>
@@ -14921,7 +14923,7 @@
         <v>0.25</v>
       </c>
       <c r="R271" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="V271" t="s">
         <v>30</v>
@@ -14956,10 +14958,10 @@
         <v>-0.5</v>
       </c>
       <c r="I272" t="s">
+        <v>786</v>
+      </c>
+      <c r="J272" t="s">
         <v>787</v>
-      </c>
-      <c r="J272" t="s">
-        <v>788</v>
       </c>
       <c r="K272" t="s">
         <v>569</v>
@@ -14968,10 +14970,10 @@
         <v>0</v>
       </c>
       <c r="M272" t="s">
+        <v>788</v>
+      </c>
+      <c r="N272" t="s">
         <v>789</v>
-      </c>
-      <c r="N272" t="s">
-        <v>790</v>
       </c>
       <c r="O272" t="s">
         <v>571</v>
@@ -14980,10 +14982,10 @@
         <v>0.5</v>
       </c>
       <c r="Q272" t="s">
+        <v>790</v>
+      </c>
+      <c r="R272" t="s">
         <v>791</v>
-      </c>
-      <c r="R272" t="s">
-        <v>792</v>
       </c>
       <c r="V272" t="s">
         <v>30</v>
@@ -15027,10 +15029,10 @@
         <v>0</v>
       </c>
       <c r="M273" t="s">
+        <v>792</v>
+      </c>
+      <c r="N273" t="s">
         <v>793</v>
-      </c>
-      <c r="N273" t="s">
-        <v>794</v>
       </c>
       <c r="O273" t="s">
         <v>571</v>
@@ -15039,10 +15041,10 @@
         <v>0.5</v>
       </c>
       <c r="Q273" t="s">
+        <v>794</v>
+      </c>
+      <c r="R273" t="s">
         <v>795</v>
-      </c>
-      <c r="R273" t="s">
-        <v>796</v>
       </c>
       <c r="V273" t="s">
         <v>30</v>
@@ -15086,7 +15088,7 @@
         <v>0</v>
       </c>
       <c r="N274" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="O274" t="s">
         <v>571</v>
@@ -15095,10 +15097,10 @@
         <v>0.25</v>
       </c>
       <c r="Q274" t="s">
+        <v>797</v>
+      </c>
+      <c r="R274" t="s">
         <v>798</v>
-      </c>
-      <c r="R274" t="s">
-        <v>799</v>
       </c>
       <c r="V274" t="s">
         <v>30</v>
@@ -15142,7 +15144,7 @@
         <v>0</v>
       </c>
       <c r="N275" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="O275" t="s">
         <v>571</v>
@@ -15151,10 +15153,10 @@
         <v>0.25</v>
       </c>
       <c r="Q275" t="s">
+        <v>800</v>
+      </c>
+      <c r="R275" t="s">
         <v>801</v>
-      </c>
-      <c r="R275" t="s">
-        <v>802</v>
       </c>
       <c r="V275" t="s">
         <v>30</v>
@@ -15198,10 +15200,10 @@
         <v>0</v>
       </c>
       <c r="M276" t="s">
+        <v>802</v>
+      </c>
+      <c r="N276" t="s">
         <v>803</v>
-      </c>
-      <c r="N276" t="s">
-        <v>804</v>
       </c>
       <c r="O276" t="s">
         <v>571</v>
@@ -15210,7 +15212,7 @@
         <v>0.5</v>
       </c>
       <c r="R276" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="V276" t="s">
         <v>30</v>
@@ -15245,10 +15247,10 @@
         <v>-0.5</v>
       </c>
       <c r="I277" t="s">
+        <v>805</v>
+      </c>
+      <c r="J277" t="s">
         <v>806</v>
-      </c>
-      <c r="J277" t="s">
-        <v>807</v>
       </c>
       <c r="K277" t="s">
         <v>569</v>
@@ -15257,10 +15259,10 @@
         <v>0</v>
       </c>
       <c r="M277" t="s">
+        <v>807</v>
+      </c>
+      <c r="N277" t="s">
         <v>808</v>
-      </c>
-      <c r="N277" t="s">
-        <v>809</v>
       </c>
       <c r="O277" t="s">
         <v>571</v>
@@ -15269,10 +15271,10 @@
         <v>0.5</v>
       </c>
       <c r="Q277" t="s">
+        <v>809</v>
+      </c>
+      <c r="R277" t="s">
         <v>810</v>
-      </c>
-      <c r="R277" t="s">
-        <v>811</v>
       </c>
       <c r="V277" t="s">
         <v>30</v>
@@ -15307,10 +15309,10 @@
         <v>-0.5</v>
       </c>
       <c r="I278" t="s">
+        <v>811</v>
+      </c>
+      <c r="J278" t="s">
         <v>812</v>
-      </c>
-      <c r="J278" t="s">
-        <v>813</v>
       </c>
       <c r="K278" t="s">
         <v>569</v>
@@ -15319,10 +15321,10 @@
         <v>0</v>
       </c>
       <c r="M278" t="s">
+        <v>813</v>
+      </c>
+      <c r="N278" t="s">
         <v>814</v>
-      </c>
-      <c r="N278" t="s">
-        <v>815</v>
       </c>
       <c r="O278" t="s">
         <v>571</v>
@@ -15331,10 +15333,10 @@
         <v>0.5</v>
       </c>
       <c r="Q278" t="s">
+        <v>815</v>
+      </c>
+      <c r="R278" t="s">
         <v>816</v>
-      </c>
-      <c r="R278" t="s">
-        <v>817</v>
       </c>
       <c r="V278" t="s">
         <v>30</v>
@@ -15378,7 +15380,7 @@
         <v>0</v>
       </c>
       <c r="N279" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="O279" t="s">
         <v>571</v>
@@ -15387,10 +15389,10 @@
         <v>0.5</v>
       </c>
       <c r="Q279" t="s">
+        <v>818</v>
+      </c>
+      <c r="R279" t="s">
         <v>819</v>
-      </c>
-      <c r="R279" t="s">
-        <v>820</v>
       </c>
       <c r="V279" t="s">
         <v>30</v>
@@ -15434,10 +15436,10 @@
         <v>0</v>
       </c>
       <c r="M280" t="s">
+        <v>820</v>
+      </c>
+      <c r="N280" t="s">
         <v>821</v>
-      </c>
-      <c r="N280" t="s">
-        <v>822</v>
       </c>
       <c r="O280" t="s">
         <v>571</v>
@@ -15446,7 +15448,7 @@
         <v>0.5</v>
       </c>
       <c r="R280" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="V280" t="s">
         <v>30</v>
@@ -15490,7 +15492,7 @@
         <v>0</v>
       </c>
       <c r="N281" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="O281" t="s">
         <v>571</v>
@@ -15499,10 +15501,10 @@
         <v>0.5</v>
       </c>
       <c r="Q281" t="s">
+        <v>824</v>
+      </c>
+      <c r="R281" t="s">
         <v>825</v>
-      </c>
-      <c r="R281" t="s">
-        <v>826</v>
       </c>
       <c r="V281" t="s">
         <v>30</v>
@@ -15546,10 +15548,10 @@
         <v>0</v>
       </c>
       <c r="M282" t="s">
+        <v>826</v>
+      </c>
+      <c r="N282" t="s">
         <v>827</v>
-      </c>
-      <c r="N282" t="s">
-        <v>828</v>
       </c>
       <c r="O282" t="s">
         <v>571</v>
@@ -15558,7 +15560,7 @@
         <v>0.25</v>
       </c>
       <c r="R282" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="V282" t="s">
         <v>30</v>
@@ -15602,10 +15604,10 @@
         <v>0</v>
       </c>
       <c r="M283" t="s">
+        <v>829</v>
+      </c>
+      <c r="N283" t="s">
         <v>830</v>
-      </c>
-      <c r="N283" t="s">
-        <v>831</v>
       </c>
       <c r="O283" t="s">
         <v>571</v>
@@ -15614,7 +15616,7 @@
         <v>0.25</v>
       </c>
       <c r="R283" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="V283" t="s">
         <v>30</v>
@@ -15658,10 +15660,10 @@
         <v>0</v>
       </c>
       <c r="M284" t="s">
+        <v>832</v>
+      </c>
+      <c r="N284" t="s">
         <v>833</v>
-      </c>
-      <c r="N284" t="s">
-        <v>834</v>
       </c>
       <c r="O284" t="s">
         <v>571</v>
@@ -15670,10 +15672,10 @@
         <v>0.25</v>
       </c>
       <c r="Q284" t="s">
+        <v>834</v>
+      </c>
+      <c r="R284" t="s">
         <v>835</v>
-      </c>
-      <c r="R284" t="s">
-        <v>836</v>
       </c>
       <c r="V284" t="s">
         <v>30</v>
@@ -15717,7 +15719,7 @@
         <v>0</v>
       </c>
       <c r="N285" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="O285" t="s">
         <v>571</v>
@@ -15726,7 +15728,7 @@
         <v>0.25</v>
       </c>
       <c r="R285" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="V285" t="s">
         <v>30</v>
@@ -15761,7 +15763,7 @@
         <v>-0.25</v>
       </c>
       <c r="J286" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="K286" t="s">
         <v>569</v>
@@ -15770,10 +15772,10 @@
         <v>0</v>
       </c>
       <c r="M286" t="s">
+        <v>839</v>
+      </c>
+      <c r="N286" t="s">
         <v>840</v>
-      </c>
-      <c r="N286" t="s">
-        <v>841</v>
       </c>
       <c r="O286" t="s">
         <v>571</v>
@@ -15782,7 +15784,7 @@
         <v>0.25</v>
       </c>
       <c r="R286" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="V286" t="s">
         <v>30</v>
@@ -15817,10 +15819,10 @@
         <v>-0.25</v>
       </c>
       <c r="I287" t="s">
+        <v>842</v>
+      </c>
+      <c r="J287" t="s">
         <v>843</v>
-      </c>
-      <c r="J287" t="s">
-        <v>844</v>
       </c>
       <c r="K287" t="s">
         <v>569</v>
@@ -15829,13 +15831,13 @@
         <v>0</v>
       </c>
       <c r="N287" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="O287" t="s">
         <v>571</v>
       </c>
       <c r="P287" t="s">
-        <v>653</v>
+        <v>845</v>
       </c>
       <c r="R287" t="s">
         <v>846</v>
@@ -17155,7 +17157,7 @@
         <v>913</v>
       </c>
       <c r="O311" t="s">
-        <v>582</v>
+        <v>569</v>
       </c>
       <c r="P311">
         <v>0</v>
@@ -17208,7 +17210,7 @@
         <v>915</v>
       </c>
       <c r="O312" t="s">
-        <v>582</v>
+        <v>567</v>
       </c>
       <c r="P312">
         <v>-0.25</v>
@@ -17261,7 +17263,7 @@
         <v>915</v>
       </c>
       <c r="O313" t="s">
-        <v>582</v>
+        <v>567</v>
       </c>
       <c r="P313">
         <v>-0.75</v>
@@ -17314,7 +17316,7 @@
         <v>915</v>
       </c>
       <c r="O314" t="s">
-        <v>582</v>
+        <v>567</v>
       </c>
       <c r="P314">
         <v>-0.5</v>
@@ -17367,7 +17369,7 @@
         <v>915</v>
       </c>
       <c r="O315" t="s">
-        <v>582</v>
+        <v>567</v>
       </c>
       <c r="P315">
         <v>-0.5</v>
@@ -17473,7 +17475,7 @@
         <v>915</v>
       </c>
       <c r="O317" t="s">
-        <v>582</v>
+        <v>567</v>
       </c>
       <c r="P317">
         <v>-0.5</v>
@@ -17526,7 +17528,7 @@
         <v>915</v>
       </c>
       <c r="O318" t="s">
-        <v>582</v>
+        <v>567</v>
       </c>
       <c r="P318">
         <v>-0.5</v>
@@ -17632,7 +17634,7 @@
         <v>915</v>
       </c>
       <c r="O320" t="s">
-        <v>582</v>
+        <v>571</v>
       </c>
       <c r="P320">
         <v>0.25</v>
@@ -17676,10 +17678,10 @@
         <v>914</v>
       </c>
       <c r="K321" t="s">
-        <v>653</v>
-      </c>
-      <c r="L321" t="s">
-        <v>653</v>
+        <v>571</v>
+      </c>
+      <c r="L321">
+        <v>0.25</v>
       </c>
       <c r="N321" t="s">
         <v>915</v>
@@ -17687,8 +17689,8 @@
       <c r="O321" t="s">
         <v>582</v>
       </c>
-      <c r="P321">
-        <v>0.25</v>
+      <c r="P321" t="s">
+        <v>582</v>
       </c>
       <c r="R321" t="s">
         <v>29</v>
@@ -17738,7 +17740,7 @@
         <v>915</v>
       </c>
       <c r="O322" t="s">
-        <v>582</v>
+        <v>571</v>
       </c>
       <c r="P322">
         <v>0.25</v>
@@ -17844,7 +17846,7 @@
         <v>915</v>
       </c>
       <c r="O324" t="s">
-        <v>582</v>
+        <v>567</v>
       </c>
       <c r="P324">
         <v>-0.5</v>
@@ -17897,7 +17899,7 @@
         <v>915</v>
       </c>
       <c r="O325" t="s">
-        <v>582</v>
+        <v>567</v>
       </c>
       <c r="P325">
         <v>-0.5</v>
@@ -18056,7 +18058,7 @@
         <v>915</v>
       </c>
       <c r="O328" t="s">
-        <v>582</v>
+        <v>567</v>
       </c>
       <c r="P328">
         <v>-0.5</v>
@@ -18109,7 +18111,7 @@
         <v>915</v>
       </c>
       <c r="O329" t="s">
-        <v>582</v>
+        <v>567</v>
       </c>
       <c r="P329">
         <v>-0.5</v>
@@ -18162,7 +18164,7 @@
         <v>915</v>
       </c>
       <c r="O330" t="s">
-        <v>582</v>
+        <v>569</v>
       </c>
       <c r="P330">
         <v>0</v>
@@ -20592,7 +20594,7 @@
         <v>567</v>
       </c>
       <c r="L375" t="s">
-        <v>653</v>
+        <v>845</v>
       </c>
       <c r="N375" t="s">
         <v>1043</v>

</xml_diff>

<commit_message>
Choose the horizon for the summary statistics
Former-commit-id: c4229409bc1f352bd352a5ac369df330416a539d
</commit_message>
<xml_diff>
--- a/src/analysis/python/data/bluebook_manual_data_online_WORKING.xlsx
+++ b/src/analysis/python/data/bluebook_manual_data_online_WORKING.xlsx
@@ -8,22 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivergiesecke/Dropbox/MPCounterfactual/src/analysis/python/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E61F004-E507-B64B-9B0C-C3598BEC0995}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DABE776-B11D-8943-9873-0F009E6AB873}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="460" windowWidth="15600" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6140" yWindow="3740" windowWidth="19560" windowHeight="19360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -4022,9 +4014,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA376"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A311" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P322" sqref="P322"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A275" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L317" sqref="L317"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17416,7 +17408,7 @@
         <v>567</v>
       </c>
       <c r="L316">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="N316" t="s">
         <v>915</v>

</xml_diff>